<commit_message>
Resa più decente la visualizzazione delle settimane, ma non dinamiche, al massimo pianificazione annuale
</commit_message>
<xml_diff>
--- a/windows_form_app/ConditionalFormatColorScale.xlsx
+++ b/windows_form_app/ConditionalFormatColorScale.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R840017bc46374bc3"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R01d0a0c65d534108"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -345,642 +345,642 @@
   <x:sheetData>
     <x:row r="1">
       <x:c r="A1">
-        <x:v>89.5750950507704</x:v>
+        <x:v>48.0404218882511</x:v>
       </x:c>
       <x:c r="B1">
-        <x:v>94.0452800570267</x:v>
+        <x:v>97.5989306800062</x:v>
       </x:c>
       <x:c r="C1">
-        <x:v>141.791857938185</x:v>
+        <x:v>184.821959577884</x:v>
       </x:c>
       <x:c r="D1">
-        <x:v>119.069754108353</x:v>
+        <x:v>161.672081780467</x:v>
       </x:c>
       <x:c r="E1">
-        <x:v>14.6485924788977</x:v>
+        <x:v>26.0244057634959</x:v>
       </x:c>
       <x:c r="F1">
-        <x:v>164.2961582934</x:v>
+        <x:v>9.45886429839715</x:v>
       </x:c>
       <x:c r="G1">
-        <x:v>182.667794070518</x:v>
+        <x:v>198.601725324337</x:v>
       </x:c>
       <x:c r="H1">
-        <x:v>117.738301175525</x:v>
+        <x:v>143.573255996952</x:v>
       </x:c>
       <x:c r="I1">
-        <x:v>185.289386746143</x:v>
+        <x:v>38.2128565750145</x:v>
       </x:c>
       <x:c r="J1">
-        <x:v>135.153108898156</x:v>
+        <x:v>162.330589053375</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>119.724857769778</x:v>
+        <x:v>104.984851137262</x:v>
       </x:c>
       <x:c r="B2">
-        <x:v>75.5074097195209</x:v>
+        <x:v>23.8904076739635</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>199.48462145379</x:v>
+        <x:v>60.0762073230353</x:v>
       </x:c>
       <x:c r="D2">
-        <x:v>6.74498258472652</x:v>
+        <x:v>77.2711618231941</x:v>
       </x:c>
       <x:c r="E2">
-        <x:v>64.9426101078012</x:v>
+        <x:v>149.651743355045</x:v>
       </x:c>
       <x:c r="F2">
-        <x:v>162.51977335779</x:v>
+        <x:v>92.0145681556382</x:v>
       </x:c>
       <x:c r="G2">
-        <x:v>48.1061750315624</x:v>
+        <x:v>15.5266159286381</x:v>
       </x:c>
       <x:c r="H2">
-        <x:v>64.8571703885017</x:v>
+        <x:v>19.3194829948803</x:v>
       </x:c>
       <x:c r="I2">
-        <x:v>126.972872916131</x:v>
+        <x:v>6.53834278068428</x:v>
       </x:c>
       <x:c r="J2">
-        <x:v>116.614572851274</x:v>
+        <x:v>89.9085517460054</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>193.787493553845</x:v>
+        <x:v>37.1586835184873</x:v>
       </x:c>
       <x:c r="B3">
-        <x:v>167.685202400985</x:v>
+        <x:v>27.5334047281805</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>169.083986696361</x:v>
+        <x:v>151.242737356221</x:v>
       </x:c>
       <x:c r="D3">
-        <x:v>187.549088051333</x:v>
+        <x:v>134.950748987007</x:v>
       </x:c>
       <x:c r="E3">
-        <x:v>87.096197012391</x:v>
+        <x:v>159.091253559613</x:v>
       </x:c>
       <x:c r="F3">
-        <x:v>104.906654406761</x:v>
+        <x:v>45.4644146587068</x:v>
       </x:c>
       <x:c r="G3">
-        <x:v>173.882843262461</x:v>
+        <x:v>72.0924906768335</x:v>
       </x:c>
       <x:c r="H3">
-        <x:v>83.7461701052944</x:v>
+        <x:v>194.582911205749</x:v>
       </x:c>
       <x:c r="I3">
-        <x:v>39.5988826824347</x:v>
+        <x:v>122.188384329057</x:v>
       </x:c>
       <x:c r="J3">
-        <x:v>161.395175737047</x:v>
+        <x:v>199.384425487083</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>143.539823099757</x:v>
+        <x:v>33.3120031437427</x:v>
       </x:c>
       <x:c r="B4">
-        <x:v>42.1243332522569</x:v>
+        <x:v>105.305086497825</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>16.2448043079324</x:v>
+        <x:v>76.8719453722574</x:v>
       </x:c>
       <x:c r="D4">
-        <x:v>127.210642084112</x:v>
+        <x:v>1.45210940458444</x:v>
       </x:c>
       <x:c r="E4">
-        <x:v>161.353505291675</x:v>
+        <x:v>176.642692450733</x:v>
       </x:c>
       <x:c r="F4">
-        <x:v>181.734327590901</x:v>
+        <x:v>121.071253400795</x:v>
       </x:c>
       <x:c r="G4">
-        <x:v>32.679386545289</x:v>
+        <x:v>175.423231150686</x:v>
       </x:c>
       <x:c r="H4">
-        <x:v>134.255028764836</x:v>
+        <x:v>31.9730667546266</x:v>
       </x:c>
       <x:c r="I4">
-        <x:v>133.061267497512</x:v>
+        <x:v>111.062208242278</x:v>
       </x:c>
       <x:c r="J4">
-        <x:v>78.9299265849078</x:v>
+        <x:v>14.4631481796797</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5">
-        <x:v>34.5473026086331</x:v>
+        <x:v>120.360910203476</x:v>
       </x:c>
       <x:c r="B5">
-        <x:v>14.3251224487671</x:v>
+        <x:v>76.5528200550716</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>30.9780983398566</x:v>
+        <x:v>50.061680213577</x:v>
       </x:c>
       <x:c r="D5">
-        <x:v>84.2593057473466</x:v>
+        <x:v>15.6393317578544</x:v>
       </x:c>
       <x:c r="E5">
-        <x:v>139.427703683929</x:v>
+        <x:v>28.2757044901493</x:v>
       </x:c>
       <x:c r="F5">
-        <x:v>8.58511710939236</x:v>
+        <x:v>134.180644310164</x:v>
       </x:c>
       <x:c r="G5">
-        <x:v>40.4905161077578</x:v>
+        <x:v>73.6901930876496</x:v>
       </x:c>
       <x:c r="H5">
-        <x:v>140.302587831534</x:v>
+        <x:v>9.35079846966583</x:v>
       </x:c>
       <x:c r="I5">
-        <x:v>72.8774358857784</x:v>
+        <x:v>172.538007037965</x:v>
       </x:c>
       <x:c r="J5">
-        <x:v>57.2849838329875</x:v>
+        <x:v>147.579582942454</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>57.6243303984517</x:v>
+        <x:v>104.525548361487</x:v>
       </x:c>
       <x:c r="B6">
-        <x:v>22.7017681220089</x:v>
+        <x:v>88.2553300299939</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>178.910091509535</x:v>
+        <x:v>25.9046786585379</x:v>
       </x:c>
       <x:c r="D6">
-        <x:v>72.4766007962062</x:v>
+        <x:v>178.122212355082</x:v>
       </x:c>
       <x:c r="E6">
-        <x:v>183.670085195298</x:v>
+        <x:v>45.008178448774</x:v>
       </x:c>
       <x:c r="F6">
-        <x:v>121.889892649786</x:v>
+        <x:v>20.5070171600706</x:v>
       </x:c>
       <x:c r="G6">
-        <x:v>124.961293360666</x:v>
+        <x:v>146.356193323786</x:v>
       </x:c>
       <x:c r="H6">
-        <x:v>154.242769886853</x:v>
+        <x:v>49.8712105908763</x:v>
       </x:c>
       <x:c r="I6">
-        <x:v>31.9735570959624</x:v>
+        <x:v>2.58082822085397</x:v>
       </x:c>
       <x:c r="J6">
-        <x:v>109.741938072137</x:v>
+        <x:v>180.559991104789</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>190.413315030939</x:v>
+        <x:v>137.366373621564</x:v>
       </x:c>
       <x:c r="B7">
-        <x:v>98.9216239652231</x:v>
+        <x:v>4.01881411858779</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>78.1394184930899</x:v>
+        <x:v>21.3848716678959</x:v>
       </x:c>
       <x:c r="D7">
-        <x:v>23.8942110090955</x:v>
+        <x:v>38.8284310879318</x:v>
       </x:c>
       <x:c r="E7">
-        <x:v>191.613285798399</x:v>
+        <x:v>129.018585909632</x:v>
       </x:c>
       <x:c r="F7">
-        <x:v>77.6005245175215</x:v>
+        <x:v>199.679764639437</x:v>
       </x:c>
       <x:c r="G7">
-        <x:v>59.2626054115885</x:v>
+        <x:v>147.018462301706</x:v>
       </x:c>
       <x:c r="H7">
-        <x:v>72.2739793696785</x:v>
+        <x:v>58.6240979184509</x:v>
       </x:c>
       <x:c r="I7">
-        <x:v>45.3914772930515</x:v>
+        <x:v>100.628469372461</x:v>
       </x:c>
       <x:c r="J7">
-        <x:v>83.2082825169006</x:v>
+        <x:v>28.5804899542502</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>129.840386812501</x:v>
+        <x:v>116.591337004952</x:v>
       </x:c>
       <x:c r="B8">
-        <x:v>113.851146266726</x:v>
+        <x:v>183.553549174011</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>131.79590289099</x:v>
+        <x:v>108.257274752603</x:v>
       </x:c>
       <x:c r="D8">
-        <x:v>48.042946331223</x:v>
+        <x:v>192.075194601005</x:v>
       </x:c>
       <x:c r="E8">
-        <x:v>82.0672702426404</x:v>
+        <x:v>169.54764154253</x:v>
       </x:c>
       <x:c r="F8">
-        <x:v>179.462371105078</x:v>
+        <x:v>160.605863463416</x:v>
       </x:c>
       <x:c r="G8">
-        <x:v>136.707104061128</x:v>
+        <x:v>177.471724514603</x:v>
       </x:c>
       <x:c r="H8">
-        <x:v>84.824680949014</x:v>
+        <x:v>135.603405598366</x:v>
       </x:c>
       <x:c r="I8">
-        <x:v>48.1213843674033</x:v>
+        <x:v>106.675044496858</x:v>
       </x:c>
       <x:c r="J8">
-        <x:v>78.5110799029987</x:v>
+        <x:v>24.9106092494496</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>64.4161382990033</x:v>
+        <x:v>171.774221571057</x:v>
       </x:c>
       <x:c r="B9">
-        <x:v>33.5802554309276</x:v>
+        <x:v>62.7416922071677</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>10.868734219516</x:v>
+        <x:v>22.0449041677848</x:v>
       </x:c>
       <x:c r="D9">
-        <x:v>182.313898849447</x:v>
+        <x:v>174.608801386603</x:v>
       </x:c>
       <x:c r="E9">
-        <x:v>103.770845338595</x:v>
+        <x:v>94.8588771255961</x:v>
       </x:c>
       <x:c r="F9">
-        <x:v>120.838054977748</x:v>
+        <x:v>145.056673113749</x:v>
       </x:c>
       <x:c r="G9">
-        <x:v>63.2142417427219</x:v>
+        <x:v>79.4004078392873</x:v>
       </x:c>
       <x:c r="H9">
-        <x:v>143.768203511726</x:v>
+        <x:v>98.7497330171753</x:v>
       </x:c>
       <x:c r="I9">
-        <x:v>143.540556888813</x:v>
+        <x:v>156.44393095581</x:v>
       </x:c>
       <x:c r="J9">
-        <x:v>39.4636126418894</x:v>
+        <x:v>156.135675290663</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>56.7730342302346</x:v>
+        <x:v>174.715060077009</x:v>
       </x:c>
       <x:c r="B10">
-        <x:v>78.4366166584364</x:v>
+        <x:v>125.55202055981</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>102.281471668874</x:v>
+        <x:v>29.3922385337726</x:v>
       </x:c>
       <x:c r="D10">
-        <x:v>23.3193294253756</x:v>
+        <x:v>130.502217137489</x:v>
       </x:c>
       <x:c r="E10">
-        <x:v>88.5166115539691</x:v>
+        <x:v>77.0967745581161</x:v>
       </x:c>
       <x:c r="F10">
-        <x:v>135.62567864341</x:v>
+        <x:v>116.342096084888</x:v>
       </x:c>
       <x:c r="G10">
-        <x:v>136.185703955677</x:v>
+        <x:v>55.1679483871758</x:v>
       </x:c>
       <x:c r="H10">
-        <x:v>7.08388733076113</x:v>
+        <x:v>11.2332491256451</x:v>
       </x:c>
       <x:c r="I10">
-        <x:v>92.6460199489473</x:v>
+        <x:v>86.620745848222</x:v>
       </x:c>
       <x:c r="J10">
-        <x:v>61.8271791664079</x:v>
+        <x:v>28.5959398507122</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>149.322511697804</x:v>
+        <x:v>187.162182008457</x:v>
       </x:c>
       <x:c r="B11">
-        <x:v>168.216536738079</x:v>
+        <x:v>15.0660951691987</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>94.9111105384823</x:v>
+        <x:v>108.722329097205</x:v>
       </x:c>
       <x:c r="D11">
-        <x:v>189.669153368878</x:v>
+        <x:v>143.957517083714</x:v>
       </x:c>
       <x:c r="E11">
-        <x:v>127.444597020487</x:v>
+        <x:v>30.9882459375021</x:v>
       </x:c>
       <x:c r="F11">
-        <x:v>143.773184131725</x:v>
+        <x:v>120.971999187475</x:v>
       </x:c>
       <x:c r="G11">
-        <x:v>90.9058652310194</x:v>
+        <x:v>179.998055277391</x:v>
       </x:c>
       <x:c r="H11">
-        <x:v>130.867145178312</x:v>
+        <x:v>33.8294840575333</x:v>
       </x:c>
       <x:c r="I11">
-        <x:v>190.409330553566</x:v>
+        <x:v>8.5745708125525</x:v>
       </x:c>
       <x:c r="J11">
-        <x:v>4.2077140902205</x:v>
+        <x:v>84.4023149853583</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
       <x:c r="A12">
-        <x:v>185.182788588657</x:v>
+        <x:v>43.0352926454671</x:v>
       </x:c>
       <x:c r="B12">
-        <x:v>40.136612411652</x:v>
+        <x:v>10.7527877254192</x:v>
       </x:c>
       <x:c r="C12">
-        <x:v>106.121385519449</x:v>
+        <x:v>143.196166094018</x:v>
       </x:c>
       <x:c r="D12">
-        <x:v>153.462477192964</x:v>
+        <x:v>177.670218971404</x:v>
       </x:c>
       <x:c r="E12">
-        <x:v>45.3257997731333</x:v>
+        <x:v>8.78576953373187</x:v>
       </x:c>
       <x:c r="F12">
-        <x:v>156.833059600011</x:v>
+        <x:v>74.6246814143959</x:v>
       </x:c>
       <x:c r="G12">
-        <x:v>88.0528897457071</x:v>
+        <x:v>181.973909950803</x:v>
       </x:c>
       <x:c r="H12">
-        <x:v>95.8255196436427</x:v>
+        <x:v>46.7760702812933</x:v>
       </x:c>
       <x:c r="I12">
-        <x:v>120.1233656705</x:v>
+        <x:v>143.969553962336</x:v>
       </x:c>
       <x:c r="J12">
-        <x:v>70.7752308206517</x:v>
+        <x:v>183.961912795884</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="A13">
-        <x:v>14.3862827747996</x:v>
+        <x:v>120.27935680015</x:v>
       </x:c>
       <x:c r="B13">
-        <x:v>115.494401899862</x:v>
+        <x:v>48.2687292845308</x:v>
       </x:c>
       <x:c r="C13">
-        <x:v>128.733422480865</x:v>
+        <x:v>102.18016696264</x:v>
       </x:c>
       <x:c r="D13">
-        <x:v>5.92786465116211</x:v>
+        <x:v>144.492794081798</x:v>
       </x:c>
       <x:c r="E13">
-        <x:v>26.435248286666</x:v>
+        <x:v>53.8654298772409</x:v>
       </x:c>
       <x:c r="F13">
-        <x:v>51.4037701540644</x:v>
+        <x:v>191.039316445142</x:v>
       </x:c>
       <x:c r="G13">
-        <x:v>11.5696745978527</x:v>
+        <x:v>154.161310640239</x:v>
       </x:c>
       <x:c r="H13">
-        <x:v>108.476573465614</x:v>
+        <x:v>177.755057615114</x:v>
       </x:c>
       <x:c r="I13">
-        <x:v>159.526334777254</x:v>
+        <x:v>114.978420042888</x:v>
       </x:c>
       <x:c r="J13">
-        <x:v>146.44159159923</x:v>
+        <x:v>53.2055454576414</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="A14">
-        <x:v>43.2766671494007</x:v>
+        <x:v>105.43791507624</x:v>
       </x:c>
       <x:c r="B14">
-        <x:v>129.623216730367</x:v>
+        <x:v>166.238475388958</x:v>
       </x:c>
       <x:c r="C14">
-        <x:v>192.178661000067</x:v>
+        <x:v>48.9826597501443</x:v>
       </x:c>
       <x:c r="D14">
-        <x:v>186.294205200995</x:v>
+        <x:v>78.0791046461459</x:v>
       </x:c>
       <x:c r="E14">
-        <x:v>129.188568205195</x:v>
+        <x:v>37.7484272409922</x:v>
       </x:c>
       <x:c r="F14">
-        <x:v>96.199601560924</x:v>
+        <x:v>156.708126401858</x:v>
       </x:c>
       <x:c r="G14">
-        <x:v>138.669144892445</x:v>
+        <x:v>154.019363109963</x:v>
       </x:c>
       <x:c r="H14">
-        <x:v>21.1995808506383</x:v>
+        <x:v>78.0873870840703</x:v>
       </x:c>
       <x:c r="I14">
-        <x:v>54.8693018289606</x:v>
+        <x:v>143.6205554491</x:v>
       </x:c>
       <x:c r="J14">
-        <x:v>159.99766120687</x:v>
+        <x:v>173.886877938121</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="A15">
-        <x:v>29.9321897467283</x:v>
+        <x:v>165.058617836357</x:v>
       </x:c>
       <x:c r="B15">
-        <x:v>132.34709656441</x:v>
+        <x:v>45.5709237817539</x:v>
       </x:c>
       <x:c r="C15">
-        <x:v>153.35887295816</x:v>
+        <x:v>90.1751622046228</x:v>
       </x:c>
       <x:c r="D15">
-        <x:v>139.332842798593</x:v>
+        <x:v>72.0416159704521</x:v>
       </x:c>
       <x:c r="E15">
-        <x:v>54.280824053232</x:v>
+        <x:v>113.100382645196</x:v>
       </x:c>
       <x:c r="F15">
-        <x:v>16.6364218185825</x:v>
+        <x:v>163.96227235159</x:v>
       </x:c>
       <x:c r="G15">
-        <x:v>172.315231138987</x:v>
+        <x:v>182.355854465792</x:v>
       </x:c>
       <x:c r="H15">
-        <x:v>148.81899447591</x:v>
+        <x:v>51.7220195623683</x:v>
       </x:c>
       <x:c r="I15">
-        <x:v>177.993529652242</x:v>
+        <x:v>121.716447603757</x:v>
       </x:c>
       <x:c r="J15">
-        <x:v>131.683551953958</x:v>
+        <x:v>2.47209314372022</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="A16">
-        <x:v>47.5727888977028</x:v>
+        <x:v>134.368186134085</x:v>
       </x:c>
       <x:c r="B16">
-        <x:v>40.3601843120345</x:v>
+        <x:v>8.3918781058825</x:v>
       </x:c>
       <x:c r="C16">
-        <x:v>86.9605216602611</x:v>
+        <x:v>67.2636951633094</x:v>
       </x:c>
       <x:c r="D16">
-        <x:v>21.8707891282955</x:v>
+        <x:v>102.658833052338</x:v>
       </x:c>
       <x:c r="E16">
-        <x:v>47.4408963916082</x:v>
+        <x:v>108.316583050562</x:v>
       </x:c>
       <x:c r="F16">
-        <x:v>33.8281097979416</x:v>
+        <x:v>138.893452723927</x:v>
       </x:c>
       <x:c r="G16">
-        <x:v>39.4831142572142</x:v>
+        <x:v>112.885928206558</x:v>
       </x:c>
       <x:c r="H16">
-        <x:v>88.9832458873201</x:v>
+        <x:v>164.229535015407</x:v>
       </x:c>
       <x:c r="I16">
-        <x:v>163.233905082212</x:v>
+        <x:v>90.0920872064736</x:v>
       </x:c>
       <x:c r="J16">
-        <x:v>76.0408268664222</x:v>
+        <x:v>39.9489294923604</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="A17">
-        <x:v>132.203509533873</x:v>
+        <x:v>166.810688547236</x:v>
       </x:c>
       <x:c r="B17">
-        <x:v>182.429291765405</x:v>
+        <x:v>2.24299766227743</x:v>
       </x:c>
       <x:c r="C17">
-        <x:v>171.340810401058</x:v>
+        <x:v>118.851064014645</x:v>
       </x:c>
       <x:c r="D17">
-        <x:v>43.9677389543353</x:v>
+        <x:v>155.369025354911</x:v>
       </x:c>
       <x:c r="E17">
-        <x:v>160.93104694082</x:v>
+        <x:v>178.964399909118</x:v>
       </x:c>
       <x:c r="F17">
-        <x:v>55.5595718582904</x:v>
+        <x:v>76.7968172565088</x:v>
       </x:c>
       <x:c r="G17">
-        <x:v>47.9579514115853</x:v>
+        <x:v>161.770127975275</x:v>
       </x:c>
       <x:c r="H17">
-        <x:v>119.827180318454</x:v>
+        <x:v>65.1170614478723</x:v>
       </x:c>
       <x:c r="I17">
-        <x:v>24.2739089877689</x:v>
+        <x:v>139.921791730412</x:v>
       </x:c>
       <x:c r="J17">
-        <x:v>149.126198212209</x:v>
+        <x:v>52.0776431318734</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="A18">
-        <x:v>18.1639147075656</x:v>
+        <x:v>120.605318304433</x:v>
       </x:c>
       <x:c r="B18">
-        <x:v>66.8533088950688</x:v>
+        <x:v>103.886522866733</x:v>
       </x:c>
       <x:c r="C18">
-        <x:v>40.9562178146822</x:v>
+        <x:v>103.155514832193</x:v>
       </x:c>
       <x:c r="D18">
-        <x:v>160.12570446363</x:v>
+        <x:v>170.082676024215</x:v>
       </x:c>
       <x:c r="E18">
-        <x:v>40.8430410739235</x:v>
+        <x:v>18.9032949595262</x:v>
       </x:c>
       <x:c r="F18">
-        <x:v>82.0391862103898</x:v>
+        <x:v>74.7084330183959</x:v>
       </x:c>
       <x:c r="G18">
-        <x:v>162.135528941702</x:v>
+        <x:v>158.093567079908</x:v>
       </x:c>
       <x:c r="H18">
-        <x:v>189.400579682272</x:v>
+        <x:v>30.1385509921883</x:v>
       </x:c>
       <x:c r="I18">
-        <x:v>151.64704059793</x:v>
+        <x:v>31.3924114366027</x:v>
       </x:c>
       <x:c r="J18">
-        <x:v>9.79882646808346</x:v>
+        <x:v>89.9031575256508</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="A19">
-        <x:v>79.0885390150773</x:v>
+        <x:v>8.68346197934982</x:v>
       </x:c>
       <x:c r="B19">
-        <x:v>62.7506801219427</x:v>
+        <x:v>102.439291077871</x:v>
       </x:c>
       <x:c r="C19">
-        <x:v>130.483043813372</x:v>
+        <x:v>56.0386100113572</x:v>
       </x:c>
       <x:c r="D19">
-        <x:v>27.8427828232957</x:v>
+        <x:v>112.506326899168</x:v>
       </x:c>
       <x:c r="E19">
-        <x:v>98.8688027015276</x:v>
+        <x:v>118.837359323556</x:v>
       </x:c>
       <x:c r="F19">
-        <x:v>2.91648283736617</x:v>
+        <x:v>97.0460369703574</x:v>
       </x:c>
       <x:c r="G19">
-        <x:v>42.6626950701059</x:v>
+        <x:v>98.9747802256489</x:v>
       </x:c>
       <x:c r="H19">
-        <x:v>170.307871871771</x:v>
+        <x:v>146.323826697806</x:v>
       </x:c>
       <x:c r="I19">
-        <x:v>138.853308809387</x:v>
+        <x:v>169.762521595584</x:v>
       </x:c>
       <x:c r="J19">
-        <x:v>95.3604584072532</x:v>
+        <x:v>98.8549745170656</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
       <x:c r="A20">
-        <x:v>56.7164873037098</x:v>
+        <x:v>43.8221981953002</x:v>
       </x:c>
       <x:c r="B20">
-        <x:v>49.6858990051252</x:v>
+        <x:v>189.789828094556</x:v>
       </x:c>
       <x:c r="C20">
-        <x:v>57.9656757684265</x:v>
+        <x:v>187.995299877597</x:v>
       </x:c>
       <x:c r="D20">
-        <x:v>178.828474962538</x:v>
+        <x:v>103.67162595674</x:v>
       </x:c>
       <x:c r="E20">
-        <x:v>27.7941516729976</x:v>
+        <x:v>7.0761893908848</x:v>
       </x:c>
       <x:c r="F20">
-        <x:v>47.5028979813228</x:v>
+        <x:v>162.81562017408</x:v>
       </x:c>
       <x:c r="G20">
-        <x:v>161.006286163352</x:v>
+        <x:v>126.719859767109</x:v>
       </x:c>
       <x:c r="H20">
-        <x:v>109.391134003825</x:v>
+        <x:v>134.806136849712</x:v>
       </x:c>
       <x:c r="I20">
-        <x:v>178.401795857773</x:v>
+        <x:v>93.0772160613338</x:v>
       </x:c>
       <x:c r="J20">
-        <x:v>198.721252194942</x:v>
+        <x:v>36.3035653886868</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Creato il calendario con la separazione delle settimane da gennaio a fine aprile, da sistemare la visualizzazione della data e dell'ora
</commit_message>
<xml_diff>
--- a/windows_form_app/ConditionalFormatColorScale.xlsx
+++ b/windows_form_app/ConditionalFormatColorScale.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R01d0a0c65d534108"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R221ec6a6e31847ea"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -345,642 +345,642 @@
   <x:sheetData>
     <x:row r="1">
       <x:c r="A1">
-        <x:v>48.0404218882511</x:v>
+        <x:v>174.614824342828</x:v>
       </x:c>
       <x:c r="B1">
-        <x:v>97.5989306800062</x:v>
+        <x:v>79.9171846732112</x:v>
       </x:c>
       <x:c r="C1">
-        <x:v>184.821959577884</x:v>
+        <x:v>163.248516695224</x:v>
       </x:c>
       <x:c r="D1">
-        <x:v>161.672081780467</x:v>
+        <x:v>152.714640345757</x:v>
       </x:c>
       <x:c r="E1">
-        <x:v>26.0244057634959</x:v>
+        <x:v>43.6933046410295</x:v>
       </x:c>
       <x:c r="F1">
-        <x:v>9.45886429839715</x:v>
+        <x:v>91.3657947868881</x:v>
       </x:c>
       <x:c r="G1">
-        <x:v>198.601725324337</x:v>
+        <x:v>18.9352595335502</x:v>
       </x:c>
       <x:c r="H1">
-        <x:v>143.573255996952</x:v>
+        <x:v>132.25148512621</x:v>
       </x:c>
       <x:c r="I1">
-        <x:v>38.2128565750145</x:v>
+        <x:v>187.063584284421</x:v>
       </x:c>
       <x:c r="J1">
-        <x:v>162.330589053375</x:v>
+        <x:v>6.48669312078817</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>104.984851137262</x:v>
+        <x:v>150.866383663782</x:v>
       </x:c>
       <x:c r="B2">
-        <x:v>23.8904076739635</x:v>
+        <x:v>26.0114197740384</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>60.0762073230353</x:v>
+        <x:v>16.6590415950208</x:v>
       </x:c>
       <x:c r="D2">
-        <x:v>77.2711618231941</x:v>
+        <x:v>72.7183658968277</x:v>
       </x:c>
       <x:c r="E2">
-        <x:v>149.651743355045</x:v>
+        <x:v>163.46372438756</x:v>
       </x:c>
       <x:c r="F2">
-        <x:v>92.0145681556382</x:v>
+        <x:v>68.4148016704315</x:v>
       </x:c>
       <x:c r="G2">
-        <x:v>15.5266159286381</x:v>
+        <x:v>128.843220290189</x:v>
       </x:c>
       <x:c r="H2">
-        <x:v>19.3194829948803</x:v>
+        <x:v>78.2641375801825</x:v>
       </x:c>
       <x:c r="I2">
-        <x:v>6.53834278068428</x:v>
+        <x:v>174.00358895492</x:v>
       </x:c>
       <x:c r="J2">
-        <x:v>89.9085517460054</x:v>
+        <x:v>30.5255962677885</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>37.1586835184873</x:v>
+        <x:v>37.0394148105008</x:v>
       </x:c>
       <x:c r="B3">
-        <x:v>27.5334047281805</x:v>
+        <x:v>92.808758417521</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>151.242737356221</x:v>
+        <x:v>82.9473020895139</x:v>
       </x:c>
       <x:c r="D3">
-        <x:v>134.950748987007</x:v>
+        <x:v>13.4338728214772</x:v>
       </x:c>
       <x:c r="E3">
-        <x:v>159.091253559613</x:v>
+        <x:v>90.14611313592</x:v>
       </x:c>
       <x:c r="F3">
-        <x:v>45.4644146587068</x:v>
+        <x:v>197.089343702928</x:v>
       </x:c>
       <x:c r="G3">
-        <x:v>72.0924906768335</x:v>
+        <x:v>39.1669149692948</x:v>
       </x:c>
       <x:c r="H3">
-        <x:v>194.582911205749</x:v>
+        <x:v>168.83658048177</x:v>
       </x:c>
       <x:c r="I3">
-        <x:v>122.188384329057</x:v>
+        <x:v>60.9308183476938</x:v>
       </x:c>
       <x:c r="J3">
-        <x:v>199.384425487083</x:v>
+        <x:v>65.4367342895999</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>33.3120031437427</x:v>
+        <x:v>18.0905228564937</x:v>
       </x:c>
       <x:c r="B4">
-        <x:v>105.305086497825</x:v>
+        <x:v>114.608184860371</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>76.8719453722574</x:v>
+        <x:v>191.565176281876</x:v>
       </x:c>
       <x:c r="D4">
-        <x:v>1.45210940458444</x:v>
+        <x:v>36.8937738411565</x:v>
       </x:c>
       <x:c r="E4">
-        <x:v>176.642692450733</x:v>
+        <x:v>146.780665845974</x:v>
       </x:c>
       <x:c r="F4">
-        <x:v>121.071253400795</x:v>
+        <x:v>38.7618960061864</x:v>
       </x:c>
       <x:c r="G4">
-        <x:v>175.423231150686</x:v>
+        <x:v>114.890729316925</x:v>
       </x:c>
       <x:c r="H4">
-        <x:v>31.9730667546266</x:v>
+        <x:v>108.486213585588</x:v>
       </x:c>
       <x:c r="I4">
-        <x:v>111.062208242278</x:v>
+        <x:v>150.807154807638</x:v>
       </x:c>
       <x:c r="J4">
-        <x:v>14.4631481796797</x:v>
+        <x:v>30.9052166672913</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5">
-        <x:v>120.360910203476</x:v>
+        <x:v>45.7007184837482</x:v>
       </x:c>
       <x:c r="B5">
-        <x:v>76.5528200550716</x:v>
+        <x:v>163.005481363742</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>50.061680213577</x:v>
+        <x:v>169.108958248565</x:v>
       </x:c>
       <x:c r="D5">
-        <x:v>15.6393317578544</x:v>
+        <x:v>34.397506823017</x:v>
       </x:c>
       <x:c r="E5">
-        <x:v>28.2757044901493</x:v>
+        <x:v>174.217484786276</x:v>
       </x:c>
       <x:c r="F5">
-        <x:v>134.180644310164</x:v>
+        <x:v>151.109676971617</x:v>
       </x:c>
       <x:c r="G5">
-        <x:v>73.6901930876496</x:v>
+        <x:v>31.8791303932104</x:v>
       </x:c>
       <x:c r="H5">
-        <x:v>9.35079846966583</x:v>
+        <x:v>46.2921630806719</x:v>
       </x:c>
       <x:c r="I5">
-        <x:v>172.538007037965</x:v>
+        <x:v>164.163637517096</x:v>
       </x:c>
       <x:c r="J5">
-        <x:v>147.579582942454</x:v>
+        <x:v>127.563915647363</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>104.525548361487</x:v>
+        <x:v>145.105422542014</x:v>
       </x:c>
       <x:c r="B6">
-        <x:v>88.2553300299939</x:v>
+        <x:v>54.5950544320955</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>25.9046786585379</x:v>
+        <x:v>193.323494211456</x:v>
       </x:c>
       <x:c r="D6">
-        <x:v>178.122212355082</x:v>
+        <x:v>142.025130773906</x:v>
       </x:c>
       <x:c r="E6">
-        <x:v>45.008178448774</x:v>
+        <x:v>7.84210851781168</x:v>
       </x:c>
       <x:c r="F6">
-        <x:v>20.5070171600706</x:v>
+        <x:v>81.8060659253067</x:v>
       </x:c>
       <x:c r="G6">
-        <x:v>146.356193323786</x:v>
+        <x:v>196.969882583697</x:v>
       </x:c>
       <x:c r="H6">
-        <x:v>49.8712105908763</x:v>
+        <x:v>149.814643873747</x:v>
       </x:c>
       <x:c r="I6">
-        <x:v>2.58082822085397</x:v>
+        <x:v>62.5685272098372</x:v>
       </x:c>
       <x:c r="J6">
-        <x:v>180.559991104789</x:v>
+        <x:v>46.6039609381016</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>137.366373621564</x:v>
+        <x:v>52.1988798175933</x:v>
       </x:c>
       <x:c r="B7">
-        <x:v>4.01881411858779</x:v>
+        <x:v>50.0986790517805</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>21.3848716678959</x:v>
+        <x:v>71.3206667785163</x:v>
       </x:c>
       <x:c r="D7">
-        <x:v>38.8284310879318</x:v>
+        <x:v>121.626849994821</x:v>
       </x:c>
       <x:c r="E7">
-        <x:v>129.018585909632</x:v>
+        <x:v>188.396170264294</x:v>
       </x:c>
       <x:c r="F7">
-        <x:v>199.679764639437</x:v>
+        <x:v>36.258198803411</x:v>
       </x:c>
       <x:c r="G7">
-        <x:v>147.018462301706</x:v>
+        <x:v>34.4462434921629</x:v>
       </x:c>
       <x:c r="H7">
-        <x:v>58.6240979184509</x:v>
+        <x:v>179.765267753864</x:v>
       </x:c>
       <x:c r="I7">
-        <x:v>100.628469372461</x:v>
+        <x:v>125.937700050854</x:v>
       </x:c>
       <x:c r="J7">
-        <x:v>28.5804899542502</x:v>
+        <x:v>124.701828381373</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>116.591337004952</x:v>
+        <x:v>153.524072353506</x:v>
       </x:c>
       <x:c r="B8">
-        <x:v>183.553549174011</x:v>
+        <x:v>20.357006704601</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>108.257274752603</x:v>
+        <x:v>127.456982772544</x:v>
       </x:c>
       <x:c r="D8">
-        <x:v>192.075194601005</x:v>
+        <x:v>143.098372287628</x:v>
       </x:c>
       <x:c r="E8">
-        <x:v>169.54764154253</x:v>
+        <x:v>184.82487778404</x:v>
       </x:c>
       <x:c r="F8">
-        <x:v>160.605863463416</x:v>
+        <x:v>74.0339334467584</x:v>
       </x:c>
       <x:c r="G8">
-        <x:v>177.471724514603</x:v>
+        <x:v>123.699800168956</x:v>
       </x:c>
       <x:c r="H8">
-        <x:v>135.603405598366</x:v>
+        <x:v>48.5497952664969</x:v>
       </x:c>
       <x:c r="I8">
-        <x:v>106.675044496858</x:v>
+        <x:v>39.2163880352007</x:v>
       </x:c>
       <x:c r="J8">
-        <x:v>24.9106092494496</x:v>
+        <x:v>139.036436164303</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>171.774221571057</x:v>
+        <x:v>165.210213309717</x:v>
       </x:c>
       <x:c r="B9">
-        <x:v>62.7416922071677</x:v>
+        <x:v>192.874751888623</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>22.0449041677848</x:v>
+        <x:v>4.67294296467348</x:v>
       </x:c>
       <x:c r="D9">
-        <x:v>174.608801386603</x:v>
+        <x:v>133.366902700331</x:v>
       </x:c>
       <x:c r="E9">
-        <x:v>94.8588771255961</x:v>
+        <x:v>120.331311747586</x:v>
       </x:c>
       <x:c r="F9">
-        <x:v>145.056673113749</x:v>
+        <x:v>163.495468424398</x:v>
       </x:c>
       <x:c r="G9">
-        <x:v>79.4004078392873</x:v>
+        <x:v>121.284690648916</x:v>
       </x:c>
       <x:c r="H9">
-        <x:v>98.7497330171753</x:v>
+        <x:v>49.5400455079694</x:v>
       </x:c>
       <x:c r="I9">
-        <x:v>156.44393095581</x:v>
+        <x:v>29.0516653233448</x:v>
       </x:c>
       <x:c r="J9">
-        <x:v>156.135675290663</x:v>
+        <x:v>64.9745999206671</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>174.715060077009</x:v>
+        <x:v>41.7920134224892</x:v>
       </x:c>
       <x:c r="B10">
-        <x:v>125.55202055981</x:v>
+        <x:v>165.076085443178</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>29.3922385337726</x:v>
+        <x:v>45.917686375751</x:v>
       </x:c>
       <x:c r="D10">
-        <x:v>130.502217137489</x:v>
+        <x:v>104.203193869536</x:v>
       </x:c>
       <x:c r="E10">
-        <x:v>77.0967745581161</x:v>
+        <x:v>178.706336849698</x:v>
       </x:c>
       <x:c r="F10">
-        <x:v>116.342096084888</x:v>
+        <x:v>195.602039431968</x:v>
       </x:c>
       <x:c r="G10">
-        <x:v>55.1679483871758</x:v>
+        <x:v>91.684814585226</x:v>
       </x:c>
       <x:c r="H10">
-        <x:v>11.2332491256451</x:v>
+        <x:v>47.4821082537445</x:v>
       </x:c>
       <x:c r="I10">
-        <x:v>86.620745848222</x:v>
+        <x:v>46.0013365587226</x:v>
       </x:c>
       <x:c r="J10">
-        <x:v>28.5959398507122</x:v>
+        <x:v>137.959285982866</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>187.162182008457</x:v>
+        <x:v>116.663433479454</x:v>
       </x:c>
       <x:c r="B11">
-        <x:v>15.0660951691987</x:v>
+        <x:v>52.1138626393461</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>108.722329097205</x:v>
+        <x:v>120.354463029818</x:v>
       </x:c>
       <x:c r="D11">
-        <x:v>143.957517083714</x:v>
+        <x:v>39.4618091357228</x:v>
       </x:c>
       <x:c r="E11">
-        <x:v>30.9882459375021</x:v>
+        <x:v>174.039843293857</x:v>
       </x:c>
       <x:c r="F11">
-        <x:v>120.971999187475</x:v>
+        <x:v>124.748415837413</x:v>
       </x:c>
       <x:c r="G11">
-        <x:v>179.998055277391</x:v>
+        <x:v>127.138071659551</x:v>
       </x:c>
       <x:c r="H11">
-        <x:v>33.8294840575333</x:v>
+        <x:v>50.2251219238272</x:v>
       </x:c>
       <x:c r="I11">
-        <x:v>8.5745708125525</x:v>
+        <x:v>157.200252989866</x:v>
       </x:c>
       <x:c r="J11">
-        <x:v>84.4023149853583</x:v>
+        <x:v>133.808175071053</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
       <x:c r="A12">
-        <x:v>43.0352926454671</x:v>
+        <x:v>158.106265756351</x:v>
       </x:c>
       <x:c r="B12">
-        <x:v>10.7527877254192</x:v>
+        <x:v>148.4200873172</x:v>
       </x:c>
       <x:c r="C12">
-        <x:v>143.196166094018</x:v>
+        <x:v>110.598255838546</x:v>
       </x:c>
       <x:c r="D12">
-        <x:v>177.670218971404</x:v>
+        <x:v>123.532091045534</x:v>
       </x:c>
       <x:c r="E12">
-        <x:v>8.78576953373187</x:v>
+        <x:v>81.3937476283841</x:v>
       </x:c>
       <x:c r="F12">
-        <x:v>74.6246814143959</x:v>
+        <x:v>59.3241279289704</x:v>
       </x:c>
       <x:c r="G12">
-        <x:v>181.973909950803</x:v>
+        <x:v>45.425736087107</x:v>
       </x:c>
       <x:c r="H12">
-        <x:v>46.7760702812933</x:v>
+        <x:v>137.953764078186</x:v>
       </x:c>
       <x:c r="I12">
-        <x:v>143.969553962336</x:v>
+        <x:v>1.2955382472349</x:v>
       </x:c>
       <x:c r="J12">
-        <x:v>183.961912795884</x:v>
+        <x:v>24.9007018398962</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="A13">
-        <x:v>120.27935680015</x:v>
+        <x:v>114.973508154495</x:v>
       </x:c>
       <x:c r="B13">
-        <x:v>48.2687292845308</x:v>
+        <x:v>184.906197984194</x:v>
       </x:c>
       <x:c r="C13">
-        <x:v>102.18016696264</x:v>
+        <x:v>150.713602430519</x:v>
       </x:c>
       <x:c r="D13">
-        <x:v>144.492794081798</x:v>
+        <x:v>60.9631001301869</x:v>
       </x:c>
       <x:c r="E13">
-        <x:v>53.8654298772409</x:v>
+        <x:v>82.9098149588843</x:v>
       </x:c>
       <x:c r="F13">
-        <x:v>191.039316445142</x:v>
+        <x:v>188.447986910328</x:v>
       </x:c>
       <x:c r="G13">
-        <x:v>154.161310640239</x:v>
+        <x:v>174.43932032885</x:v>
       </x:c>
       <x:c r="H13">
-        <x:v>177.755057615114</x:v>
+        <x:v>23.2537889030081</x:v>
       </x:c>
       <x:c r="I13">
-        <x:v>114.978420042888</x:v>
+        <x:v>164.39203543793</x:v>
       </x:c>
       <x:c r="J13">
-        <x:v>53.2055454576414</x:v>
+        <x:v>189.222838352072</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="A14">
-        <x:v>105.43791507624</x:v>
+        <x:v>182.349118861532</x:v>
       </x:c>
       <x:c r="B14">
-        <x:v>166.238475388958</x:v>
+        <x:v>76.2176919152111</x:v>
       </x:c>
       <x:c r="C14">
-        <x:v>48.9826597501443</x:v>
+        <x:v>2.54845870777427</x:v>
       </x:c>
       <x:c r="D14">
-        <x:v>78.0791046461459</x:v>
+        <x:v>101.257102052335</x:v>
       </x:c>
       <x:c r="E14">
-        <x:v>37.7484272409922</x:v>
+        <x:v>22.3730026848488</x:v>
       </x:c>
       <x:c r="F14">
-        <x:v>156.708126401858</x:v>
+        <x:v>113.096350670371</x:v>
       </x:c>
       <x:c r="G14">
-        <x:v>154.019363109963</x:v>
+        <x:v>72.520288858805</x:v>
       </x:c>
       <x:c r="H14">
-        <x:v>78.0873870840703</x:v>
+        <x:v>165.211133828951</x:v>
       </x:c>
       <x:c r="I14">
-        <x:v>143.6205554491</x:v>
+        <x:v>159.327059406474</x:v>
       </x:c>
       <x:c r="J14">
-        <x:v>173.886877938121</x:v>
+        <x:v>195.582895910173</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="A15">
-        <x:v>165.058617836357</x:v>
+        <x:v>36.3573967648472</x:v>
       </x:c>
       <x:c r="B15">
-        <x:v>45.5709237817539</x:v>
+        <x:v>71.0595687250884</x:v>
       </x:c>
       <x:c r="C15">
-        <x:v>90.1751622046228</x:v>
+        <x:v>92.3397925181034</x:v>
       </x:c>
       <x:c r="D15">
-        <x:v>72.0416159704521</x:v>
+        <x:v>95.2434902522916</x:v>
       </x:c>
       <x:c r="E15">
-        <x:v>113.100382645196</x:v>
+        <x:v>106.868334164316</x:v>
       </x:c>
       <x:c r="F15">
-        <x:v>163.96227235159</x:v>
+        <x:v>93.3719261052888</x:v>
       </x:c>
       <x:c r="G15">
-        <x:v>182.355854465792</x:v>
+        <x:v>54.4778296046321</x:v>
       </x:c>
       <x:c r="H15">
-        <x:v>51.7220195623683</x:v>
+        <x:v>122.385595330217</x:v>
       </x:c>
       <x:c r="I15">
-        <x:v>121.716447603757</x:v>
+        <x:v>22.8094462411522</x:v>
       </x:c>
       <x:c r="J15">
-        <x:v>2.47209314372022</x:v>
+        <x:v>119.382208920728</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="A16">
-        <x:v>134.368186134085</x:v>
+        <x:v>150.176303344861</x:v>
       </x:c>
       <x:c r="B16">
-        <x:v>8.3918781058825</x:v>
+        <x:v>153.73105050704</x:v>
       </x:c>
       <x:c r="C16">
-        <x:v>67.2636951633094</x:v>
+        <x:v>46.1865700065096</x:v>
       </x:c>
       <x:c r="D16">
-        <x:v>102.658833052338</x:v>
+        <x:v>21.1006347188263</x:v>
       </x:c>
       <x:c r="E16">
-        <x:v>108.316583050562</x:v>
+        <x:v>22.9857778283701</x:v>
       </x:c>
       <x:c r="F16">
-        <x:v>138.893452723927</x:v>
+        <x:v>131.757235495261</x:v>
       </x:c>
       <x:c r="G16">
-        <x:v>112.885928206558</x:v>
+        <x:v>101.400260208827</x:v>
       </x:c>
       <x:c r="H16">
-        <x:v>164.229535015407</x:v>
+        <x:v>59.391362899631</x:v>
       </x:c>
       <x:c r="I16">
-        <x:v>90.0920872064736</x:v>
+        <x:v>156.551994176839</x:v>
       </x:c>
       <x:c r="J16">
-        <x:v>39.9489294923604</x:v>
+        <x:v>185.591856383528</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="A17">
-        <x:v>166.810688547236</x:v>
+        <x:v>150.309095508563</x:v>
       </x:c>
       <x:c r="B17">
-        <x:v>2.24299766227743</x:v>
+        <x:v>103.884282756543</x:v>
       </x:c>
       <x:c r="C17">
-        <x:v>118.851064014645</x:v>
+        <x:v>85.8330864858968</x:v>
       </x:c>
       <x:c r="D17">
-        <x:v>155.369025354911</x:v>
+        <x:v>167.977414637794</x:v>
       </x:c>
       <x:c r="E17">
-        <x:v>178.964399909118</x:v>
+        <x:v>151.459056209521</x:v>
       </x:c>
       <x:c r="F17">
-        <x:v>76.7968172565088</x:v>
+        <x:v>81.8885738411399</x:v>
       </x:c>
       <x:c r="G17">
-        <x:v>161.770127975275</x:v>
+        <x:v>145.871628609426</x:v>
       </x:c>
       <x:c r="H17">
-        <x:v>65.1170614478723</x:v>
+        <x:v>9.34115378621088</x:v>
       </x:c>
       <x:c r="I17">
-        <x:v>139.921791730412</x:v>
+        <x:v>101.159088360685</x:v>
       </x:c>
       <x:c r="J17">
-        <x:v>52.0776431318734</x:v>
+        <x:v>168.297396958013</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="A18">
-        <x:v>120.605318304433</x:v>
+        <x:v>186.803839070165</x:v>
       </x:c>
       <x:c r="B18">
-        <x:v>103.886522866733</x:v>
+        <x:v>80.2146022581563</x:v>
       </x:c>
       <x:c r="C18">
-        <x:v>103.155514832193</x:v>
+        <x:v>178.626704671712</x:v>
       </x:c>
       <x:c r="D18">
-        <x:v>170.082676024215</x:v>
+        <x:v>5.71264233706176</x:v>
       </x:c>
       <x:c r="E18">
-        <x:v>18.9032949595262</x:v>
+        <x:v>188.543305075049</x:v>
       </x:c>
       <x:c r="F18">
-        <x:v>74.7084330183959</x:v>
+        <x:v>43.913939429407</x:v>
       </x:c>
       <x:c r="G18">
-        <x:v>158.093567079908</x:v>
+        <x:v>92.5664054660901</x:v>
       </x:c>
       <x:c r="H18">
-        <x:v>30.1385509921883</x:v>
+        <x:v>55.4701121782279</x:v>
       </x:c>
       <x:c r="I18">
-        <x:v>31.3924114366027</x:v>
+        <x:v>154.094765965871</x:v>
       </x:c>
       <x:c r="J18">
-        <x:v>89.9031575256508</x:v>
+        <x:v>189.537888853596</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="A19">
-        <x:v>8.68346197934982</x:v>
+        <x:v>133.970157305696</x:v>
       </x:c>
       <x:c r="B19">
-        <x:v>102.439291077871</x:v>
+        <x:v>52.0537249986332</x:v>
       </x:c>
       <x:c r="C19">
-        <x:v>56.0386100113572</x:v>
+        <x:v>0.444342661855902</x:v>
       </x:c>
       <x:c r="D19">
-        <x:v>112.506326899168</x:v>
+        <x:v>45.0098265172028</x:v>
       </x:c>
       <x:c r="E19">
-        <x:v>118.837359323556</x:v>
+        <x:v>39.0465350072116</x:v>
       </x:c>
       <x:c r="F19">
-        <x:v>97.0460369703574</x:v>
+        <x:v>28.6180683544921</x:v>
       </x:c>
       <x:c r="G19">
-        <x:v>98.9747802256489</x:v>
+        <x:v>30.0311219087015</x:v>
       </x:c>
       <x:c r="H19">
-        <x:v>146.323826697806</x:v>
+        <x:v>181.447823988948</x:v>
       </x:c>
       <x:c r="I19">
-        <x:v>169.762521595584</x:v>
+        <x:v>78.2713242239651</x:v>
       </x:c>
       <x:c r="J19">
-        <x:v>98.8549745170656</x:v>
+        <x:v>90.6157671895883</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
       <x:c r="A20">
-        <x:v>43.8221981953002</x:v>
+        <x:v>11.6960904615447</x:v>
       </x:c>
       <x:c r="B20">
-        <x:v>189.789828094556</x:v>
+        <x:v>13.128925959174</x:v>
       </x:c>
       <x:c r="C20">
-        <x:v>187.995299877597</x:v>
+        <x:v>8.6591396521121</x:v>
       </x:c>
       <x:c r="D20">
-        <x:v>103.67162595674</x:v>
+        <x:v>173.735203022945</x:v>
       </x:c>
       <x:c r="E20">
-        <x:v>7.0761893908848</x:v>
+        <x:v>45.2738004016102</x:v>
       </x:c>
       <x:c r="F20">
-        <x:v>162.81562017408</x:v>
+        <x:v>132.473114008304</x:v>
       </x:c>
       <x:c r="G20">
-        <x:v>126.719859767109</x:v>
+        <x:v>185.226482239192</x:v>
       </x:c>
       <x:c r="H20">
-        <x:v>134.806136849712</x:v>
+        <x:v>124.36237788031</x:v>
       </x:c>
       <x:c r="I20">
-        <x:v>93.0772160613338</x:v>
+        <x:v>143.784434042771</x:v>
       </x:c>
       <x:c r="J20">
-        <x:v>36.3035653886868</x:v>
+        <x:v>24.979760323176</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
da sistemare la visualizzazione del template e della data in una funzione dedicata da richiamare nel genra excel, poi una breve nota nel codice sulle cose da fare
</commit_message>
<xml_diff>
--- a/windows_form_app/ConditionalFormatColorScale.xlsx
+++ b/windows_form_app/ConditionalFormatColorScale.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R221ec6a6e31847ea"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R9a01dab572b94683"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -345,642 +345,642 @@
   <x:sheetData>
     <x:row r="1">
       <x:c r="A1">
-        <x:v>174.614824342828</x:v>
+        <x:v>55.8603827170378</x:v>
       </x:c>
       <x:c r="B1">
-        <x:v>79.9171846732112</x:v>
+        <x:v>46.3780275761979</x:v>
       </x:c>
       <x:c r="C1">
-        <x:v>163.248516695224</x:v>
+        <x:v>152.243937995398</x:v>
       </x:c>
       <x:c r="D1">
-        <x:v>152.714640345757</x:v>
+        <x:v>78.9956533717903</x:v>
       </x:c>
       <x:c r="E1">
-        <x:v>43.6933046410295</x:v>
+        <x:v>135.261113538994</x:v>
       </x:c>
       <x:c r="F1">
-        <x:v>91.3657947868881</x:v>
+        <x:v>46.9787431168271</x:v>
       </x:c>
       <x:c r="G1">
-        <x:v>18.9352595335502</x:v>
+        <x:v>91.0547565161505</x:v>
       </x:c>
       <x:c r="H1">
-        <x:v>132.25148512621</x:v>
+        <x:v>108.087243655737</x:v>
       </x:c>
       <x:c r="I1">
-        <x:v>187.063584284421</x:v>
+        <x:v>131.641277918425</x:v>
       </x:c>
       <x:c r="J1">
-        <x:v>6.48669312078817</x:v>
+        <x:v>26.7630994444541</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>150.866383663782</x:v>
+        <x:v>141.496570101705</x:v>
       </x:c>
       <x:c r="B2">
-        <x:v>26.0114197740384</x:v>
+        <x:v>178.752195638955</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>16.6590415950208</x:v>
+        <x:v>1.22404526976126</x:v>
       </x:c>
       <x:c r="D2">
-        <x:v>72.7183658968277</x:v>
+        <x:v>199.819334689444</x:v>
       </x:c>
       <x:c r="E2">
-        <x:v>163.46372438756</x:v>
+        <x:v>149.854011624052</x:v>
       </x:c>
       <x:c r="F2">
-        <x:v>68.4148016704315</x:v>
+        <x:v>105.145647239473</x:v>
       </x:c>
       <x:c r="G2">
-        <x:v>128.843220290189</x:v>
+        <x:v>199.634231254288</x:v>
       </x:c>
       <x:c r="H2">
-        <x:v>78.2641375801825</x:v>
+        <x:v>35.8542567285962</x:v>
       </x:c>
       <x:c r="I2">
-        <x:v>174.00358895492</x:v>
+        <x:v>39.9836600944324</x:v>
       </x:c>
       <x:c r="J2">
-        <x:v>30.5255962677885</x:v>
+        <x:v>172.899967885064</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>37.0394148105008</x:v>
+        <x:v>171.821368379435</x:v>
       </x:c>
       <x:c r="B3">
-        <x:v>92.808758417521</x:v>
+        <x:v>183.284240580762</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>82.9473020895139</x:v>
+        <x:v>99.8080708551258</x:v>
       </x:c>
       <x:c r="D3">
-        <x:v>13.4338728214772</x:v>
+        <x:v>179.59213768113</x:v>
       </x:c>
       <x:c r="E3">
-        <x:v>90.14611313592</x:v>
+        <x:v>96.4630233573089</x:v>
       </x:c>
       <x:c r="F3">
-        <x:v>197.089343702928</x:v>
+        <x:v>5.09410631148802</x:v>
       </x:c>
       <x:c r="G3">
-        <x:v>39.1669149692948</x:v>
+        <x:v>187.341186212069</x:v>
       </x:c>
       <x:c r="H3">
-        <x:v>168.83658048177</x:v>
+        <x:v>132.477039998619</x:v>
       </x:c>
       <x:c r="I3">
-        <x:v>60.9308183476938</x:v>
+        <x:v>107.713346233458</x:v>
       </x:c>
       <x:c r="J3">
-        <x:v>65.4367342895999</x:v>
+        <x:v>40.3243849241754</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>18.0905228564937</x:v>
+        <x:v>70.8726690480824</x:v>
       </x:c>
       <x:c r="B4">
-        <x:v>114.608184860371</x:v>
+        <x:v>28.3576615286794</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>191.565176281876</x:v>
+        <x:v>69.8911891644314</x:v>
       </x:c>
       <x:c r="D4">
-        <x:v>36.8937738411565</x:v>
+        <x:v>117.031572161723</x:v>
       </x:c>
       <x:c r="E4">
-        <x:v>146.780665845974</x:v>
+        <x:v>107.564645590058</x:v>
       </x:c>
       <x:c r="F4">
-        <x:v>38.7618960061864</x:v>
+        <x:v>66.6489888292965</x:v>
       </x:c>
       <x:c r="G4">
-        <x:v>114.890729316925</x:v>
+        <x:v>137.187778547959</x:v>
       </x:c>
       <x:c r="H4">
-        <x:v>108.486213585588</x:v>
+        <x:v>144.921344399881</x:v>
       </x:c>
       <x:c r="I4">
-        <x:v>150.807154807638</x:v>
+        <x:v>29.2703065226182</x:v>
       </x:c>
       <x:c r="J4">
-        <x:v>30.9052166672913</x:v>
+        <x:v>152.582909330997</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5">
-        <x:v>45.7007184837482</x:v>
+        <x:v>78.0191712444737</x:v>
       </x:c>
       <x:c r="B5">
-        <x:v>163.005481363742</x:v>
+        <x:v>183.04097791344</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>169.108958248565</x:v>
+        <x:v>188.052196888277</x:v>
       </x:c>
       <x:c r="D5">
-        <x:v>34.397506823017</x:v>
+        <x:v>98.3287659000274</x:v>
       </x:c>
       <x:c r="E5">
-        <x:v>174.217484786276</x:v>
+        <x:v>55.9140092022317</x:v>
       </x:c>
       <x:c r="F5">
-        <x:v>151.109676971617</x:v>
+        <x:v>11.3105726480999</x:v>
       </x:c>
       <x:c r="G5">
-        <x:v>31.8791303932104</x:v>
+        <x:v>60.8798746303096</x:v>
       </x:c>
       <x:c r="H5">
-        <x:v>46.2921630806719</x:v>
+        <x:v>13.4657994906724</x:v>
       </x:c>
       <x:c r="I5">
-        <x:v>164.163637517096</x:v>
+        <x:v>194.316295345461</x:v>
       </x:c>
       <x:c r="J5">
-        <x:v>127.563915647363</x:v>
+        <x:v>181.430495707984</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>145.105422542014</x:v>
+        <x:v>3.9219872112954</x:v>
       </x:c>
       <x:c r="B6">
-        <x:v>54.5950544320955</x:v>
+        <x:v>163.538239041128</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>193.323494211456</x:v>
+        <x:v>25.0210194964991</x:v>
       </x:c>
       <x:c r="D6">
-        <x:v>142.025130773906</x:v>
+        <x:v>33.8525410899206</x:v>
       </x:c>
       <x:c r="E6">
-        <x:v>7.84210851781168</x:v>
+        <x:v>181.53562768434</x:v>
       </x:c>
       <x:c r="F6">
-        <x:v>81.8060659253067</x:v>
+        <x:v>72.5761421362758</x:v>
       </x:c>
       <x:c r="G6">
-        <x:v>196.969882583697</x:v>
+        <x:v>146.569956721072</x:v>
       </x:c>
       <x:c r="H6">
-        <x:v>149.814643873747</x:v>
+        <x:v>172.651800314268</x:v>
       </x:c>
       <x:c r="I6">
-        <x:v>62.5685272098372</x:v>
+        <x:v>182.532630014481</x:v>
       </x:c>
       <x:c r="J6">
-        <x:v>46.6039609381016</x:v>
+        <x:v>130.167007227506</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>52.1988798175933</x:v>
+        <x:v>59.6375569047581</x:v>
       </x:c>
       <x:c r="B7">
-        <x:v>50.0986790517805</x:v>
+        <x:v>158.577716517531</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>71.3206667785163</x:v>
+        <x:v>0.373897422279183</x:v>
       </x:c>
       <x:c r="D7">
-        <x:v>121.626849994821</x:v>
+        <x:v>91.3168929942497</x:v>
       </x:c>
       <x:c r="E7">
-        <x:v>188.396170264294</x:v>
+        <x:v>155.890430396372</x:v>
       </x:c>
       <x:c r="F7">
-        <x:v>36.258198803411</x:v>
+        <x:v>113.138908573025</x:v>
       </x:c>
       <x:c r="G7">
-        <x:v>34.4462434921629</x:v>
+        <x:v>108.861006474523</x:v>
       </x:c>
       <x:c r="H7">
-        <x:v>179.765267753864</x:v>
+        <x:v>84.1924731080385</x:v>
       </x:c>
       <x:c r="I7">
-        <x:v>125.937700050854</x:v>
+        <x:v>92.2546890993857</x:v>
       </x:c>
       <x:c r="J7">
-        <x:v>124.701828381373</x:v>
+        <x:v>83.2050227947556</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>153.524072353506</x:v>
+        <x:v>167.957868691514</x:v>
       </x:c>
       <x:c r="B8">
-        <x:v>20.357006704601</x:v>
+        <x:v>54.7128868544069</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>127.456982772544</x:v>
+        <x:v>6.58395020597798</x:v>
       </x:c>
       <x:c r="D8">
-        <x:v>143.098372287628</x:v>
+        <x:v>87.4007507634353</x:v>
       </x:c>
       <x:c r="E8">
-        <x:v>184.82487778404</x:v>
+        <x:v>94.8807966405902</x:v>
       </x:c>
       <x:c r="F8">
-        <x:v>74.0339334467584</x:v>
+        <x:v>188.780390465995</x:v>
       </x:c>
       <x:c r="G8">
-        <x:v>123.699800168956</x:v>
+        <x:v>195.232043692485</x:v>
       </x:c>
       <x:c r="H8">
-        <x:v>48.5497952664969</x:v>
+        <x:v>1.47930495509845</x:v>
       </x:c>
       <x:c r="I8">
-        <x:v>39.2163880352007</x:v>
+        <x:v>123.678128478899</x:v>
       </x:c>
       <x:c r="J8">
-        <x:v>139.036436164303</x:v>
+        <x:v>85.1524507092091</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>165.210213309717</x:v>
+        <x:v>144.214231681178</x:v>
       </x:c>
       <x:c r="B9">
-        <x:v>192.874751888623</x:v>
+        <x:v>173.875386721397</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>4.67294296467348</x:v>
+        <x:v>138.160744653158</x:v>
       </x:c>
       <x:c r="D9">
-        <x:v>133.366902700331</x:v>
+        <x:v>126.282850525474</x:v>
       </x:c>
       <x:c r="E9">
-        <x:v>120.331311747586</x:v>
+        <x:v>36.40239771288</x:v>
       </x:c>
       <x:c r="F9">
-        <x:v>163.495468424398</x:v>
+        <x:v>107.334430006954</x:v>
       </x:c>
       <x:c r="G9">
-        <x:v>121.284690648916</x:v>
+        <x:v>3.33664203218028</x:v>
       </x:c>
       <x:c r="H9">
-        <x:v>49.5400455079694</x:v>
+        <x:v>36.0386480745108</x:v>
       </x:c>
       <x:c r="I9">
-        <x:v>29.0516653233448</x:v>
+        <x:v>135.495944477383</x:v>
       </x:c>
       <x:c r="J9">
-        <x:v>64.9745999206671</x:v>
+        <x:v>34.9885034537821</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>41.7920134224892</x:v>
+        <x:v>120.079032108224</x:v>
       </x:c>
       <x:c r="B10">
-        <x:v>165.076085443178</x:v>
+        <x:v>164.535978233691</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>45.917686375751</x:v>
+        <x:v>162.3887143854</x:v>
       </x:c>
       <x:c r="D10">
-        <x:v>104.203193869536</x:v>
+        <x:v>99.1032992951122</x:v>
       </x:c>
       <x:c r="E10">
-        <x:v>178.706336849698</x:v>
+        <x:v>92.945352426239</x:v>
       </x:c>
       <x:c r="F10">
-        <x:v>195.602039431968</x:v>
+        <x:v>119.441454726943</x:v>
       </x:c>
       <x:c r="G10">
-        <x:v>91.684814585226</x:v>
+        <x:v>182.667080491161</x:v>
       </x:c>
       <x:c r="H10">
-        <x:v>47.4821082537445</x:v>
+        <x:v>96.7353038940278</x:v>
       </x:c>
       <x:c r="I10">
-        <x:v>46.0013365587226</x:v>
+        <x:v>142.438335503656</x:v>
       </x:c>
       <x:c r="J10">
-        <x:v>137.959285982866</x:v>
+        <x:v>142.775100629206</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>116.663433479454</x:v>
+        <x:v>102.449566173577</x:v>
       </x:c>
       <x:c r="B11">
-        <x:v>52.1138626393461</x:v>
+        <x:v>176.687401522271</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>120.354463029818</x:v>
+        <x:v>121.211110391287</x:v>
       </x:c>
       <x:c r="D11">
-        <x:v>39.4618091357228</x:v>
+        <x:v>111.111272550705</x:v>
       </x:c>
       <x:c r="E11">
-        <x:v>174.039843293857</x:v>
+        <x:v>13.4726270164701</x:v>
       </x:c>
       <x:c r="F11">
-        <x:v>124.748415837413</x:v>
+        <x:v>149.209100356889</x:v>
       </x:c>
       <x:c r="G11">
-        <x:v>127.138071659551</x:v>
+        <x:v>156.95428883515</x:v>
       </x:c>
       <x:c r="H11">
-        <x:v>50.2251219238272</x:v>
+        <x:v>137.620268733064</x:v>
       </x:c>
       <x:c r="I11">
-        <x:v>157.200252989866</x:v>
+        <x:v>138.97174444933</x:v>
       </x:c>
       <x:c r="J11">
-        <x:v>133.808175071053</x:v>
+        <x:v>192.755237218344</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
       <x:c r="A12">
-        <x:v>158.106265756351</x:v>
+        <x:v>77.3440984437913</x:v>
       </x:c>
       <x:c r="B12">
-        <x:v>148.4200873172</x:v>
+        <x:v>145.090651765974</x:v>
       </x:c>
       <x:c r="C12">
-        <x:v>110.598255838546</x:v>
+        <x:v>48.9736718353693</x:v>
       </x:c>
       <x:c r="D12">
-        <x:v>123.532091045534</x:v>
+        <x:v>97.3801793052723</x:v>
       </x:c>
       <x:c r="E12">
-        <x:v>81.3937476283841</x:v>
+        <x:v>185.952775546328</x:v>
       </x:c>
       <x:c r="F12">
-        <x:v>59.3241279289704</x:v>
+        <x:v>85.7621701833616</x:v>
       </x:c>
       <x:c r="G12">
-        <x:v>45.425736087107</x:v>
+        <x:v>20.4169718643729</x:v>
       </x:c>
       <x:c r="H12">
-        <x:v>137.953764078186</x:v>
+        <x:v>74.0910468968056</x:v>
       </x:c>
       <x:c r="I12">
-        <x:v>1.2955382472349</x:v>
+        <x:v>54.9144952813697</x:v>
       </x:c>
       <x:c r="J12">
-        <x:v>24.9007018398962</x:v>
+        <x:v>48.5560003894176</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="A13">
-        <x:v>114.973508154495</x:v>
+        <x:v>109.802266540845</x:v>
       </x:c>
       <x:c r="B13">
-        <x:v>184.906197984194</x:v>
+        <x:v>72.8223584000125</x:v>
       </x:c>
       <x:c r="C13">
-        <x:v>150.713602430519</x:v>
+        <x:v>148.696528630656</x:v>
       </x:c>
       <x:c r="D13">
-        <x:v>60.9631001301869</x:v>
+        <x:v>57.2661856456037</x:v>
       </x:c>
       <x:c r="E13">
-        <x:v>82.9098149588843</x:v>
+        <x:v>163.125990686531</x:v>
       </x:c>
       <x:c r="F13">
-        <x:v>188.447986910328</x:v>
+        <x:v>3.42189045782289</x:v>
       </x:c>
       <x:c r="G13">
-        <x:v>174.43932032885</x:v>
+        <x:v>92.3241724690069</x:v>
       </x:c>
       <x:c r="H13">
-        <x:v>23.2537889030081</x:v>
+        <x:v>107.480650910866</x:v>
       </x:c>
       <x:c r="I13">
-        <x:v>164.39203543793</x:v>
+        <x:v>194.455398337196</x:v>
       </x:c>
       <x:c r="J13">
-        <x:v>189.222838352072</x:v>
+        <x:v>175.439341913648</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="A14">
-        <x:v>182.349118861532</x:v>
+        <x:v>6.11330997483493</x:v>
       </x:c>
       <x:c r="B14">
-        <x:v>76.2176919152111</x:v>
+        <x:v>98.4967397984568</x:v>
       </x:c>
       <x:c r="C14">
-        <x:v>2.54845870777427</x:v>
+        <x:v>59.0409694514428</x:v>
       </x:c>
       <x:c r="D14">
-        <x:v>101.257102052335</x:v>
+        <x:v>180.903027849692</x:v>
       </x:c>
       <x:c r="E14">
-        <x:v>22.3730026848488</x:v>
+        <x:v>182.702884535633</x:v>
       </x:c>
       <x:c r="F14">
-        <x:v>113.096350670371</x:v>
+        <x:v>167.526830158907</x:v>
       </x:c>
       <x:c r="G14">
-        <x:v>72.520288858805</x:v>
+        <x:v>52.6642763301098</x:v>
       </x:c>
       <x:c r="H14">
-        <x:v>165.211133828951</x:v>
+        <x:v>27.0494721024528</x:v>
       </x:c>
       <x:c r="I14">
-        <x:v>159.327059406474</x:v>
+        <x:v>112.810223509004</x:v>
       </x:c>
       <x:c r="J14">
-        <x:v>195.582895910173</x:v>
+        <x:v>87.1932973559915</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="A15">
-        <x:v>36.3573967648472</x:v>
+        <x:v>150.380141171804</x:v>
       </x:c>
       <x:c r="B15">
-        <x:v>71.0595687250884</x:v>
+        <x:v>65.7163732991164</x:v>
       </x:c>
       <x:c r="C15">
-        <x:v>92.3397925181034</x:v>
+        <x:v>97.0669036251804</x:v>
       </x:c>
       <x:c r="D15">
-        <x:v>95.2434902522916</x:v>
+        <x:v>142.740707259039</x:v>
       </x:c>
       <x:c r="E15">
-        <x:v>106.868334164316</x:v>
+        <x:v>157.644405009991</x:v>
       </x:c>
       <x:c r="F15">
-        <x:v>93.3719261052888</x:v>
+        <x:v>174.988380342251</x:v>
       </x:c>
       <x:c r="G15">
-        <x:v>54.4778296046321</x:v>
+        <x:v>115.562306398322</x:v>
       </x:c>
       <x:c r="H15">
-        <x:v>122.385595330217</x:v>
+        <x:v>65.0085350801277</x:v>
       </x:c>
       <x:c r="I15">
-        <x:v>22.8094462411522</x:v>
+        <x:v>113.150523748785</x:v>
       </x:c>
       <x:c r="J15">
-        <x:v>119.382208920728</x:v>
+        <x:v>7.1831822428774</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="A16">
-        <x:v>150.176303344861</x:v>
+        <x:v>99.0244828625696</x:v>
       </x:c>
       <x:c r="B16">
-        <x:v>153.73105050704</x:v>
+        <x:v>108.576033594355</x:v>
       </x:c>
       <x:c r="C16">
-        <x:v>46.1865700065096</x:v>
+        <x:v>41.8208086126581</x:v>
       </x:c>
       <x:c r="D16">
-        <x:v>21.1006347188263</x:v>
+        <x:v>93.882335114238</x:v>
       </x:c>
       <x:c r="E16">
-        <x:v>22.9857778283701</x:v>
+        <x:v>32.9728340883613</x:v>
       </x:c>
       <x:c r="F16">
-        <x:v>131.757235495261</x:v>
+        <x:v>29.627207773564</x:v>
       </x:c>
       <x:c r="G16">
-        <x:v>101.400260208827</x:v>
+        <x:v>27.9908728916156</x:v>
       </x:c>
       <x:c r="H16">
-        <x:v>59.391362899631</x:v>
+        <x:v>63.9449247456831</x:v>
       </x:c>
       <x:c r="I16">
-        <x:v>156.551994176839</x:v>
+        <x:v>147.985281864174</x:v>
       </x:c>
       <x:c r="J16">
-        <x:v>185.591856383528</x:v>
+        <x:v>10.0507365586472</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="A17">
-        <x:v>150.309095508563</x:v>
+        <x:v>56.8849278878816</x:v>
       </x:c>
       <x:c r="B17">
-        <x:v>103.884282756543</x:v>
+        <x:v>49.4736379242845</x:v>
       </x:c>
       <x:c r="C17">
-        <x:v>85.8330864858968</x:v>
+        <x:v>143.164870395868</x:v>
       </x:c>
       <x:c r="D17">
-        <x:v>167.977414637794</x:v>
+        <x:v>163.532402535683</x:v>
       </x:c>
       <x:c r="E17">
-        <x:v>151.459056209521</x:v>
+        <x:v>186.641927243509</x:v>
       </x:c>
       <x:c r="F17">
-        <x:v>81.8885738411399</x:v>
+        <x:v>178.847358645335</x:v>
       </x:c>
       <x:c r="G17">
-        <x:v>145.871628609426</x:v>
+        <x:v>86.0496823145308</x:v>
       </x:c>
       <x:c r="H17">
-        <x:v>9.34115378621088</x:v>
+        <x:v>68.0706439856769</x:v>
       </x:c>
       <x:c r="I17">
-        <x:v>101.159088360685</x:v>
+        <x:v>114.67729476964</x:v>
       </x:c>
       <x:c r="J17">
-        <x:v>168.297396958013</x:v>
+        <x:v>18.4259453874202</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="A18">
-        <x:v>186.803839070165</x:v>
+        <x:v>33.0978938532518</x:v>
       </x:c>
       <x:c r="B18">
-        <x:v>80.2146022581563</x:v>
+        <x:v>193.36749976192</x:v>
       </x:c>
       <x:c r="C18">
-        <x:v>178.626704671712</x:v>
+        <x:v>161.280823387802</x:v>
       </x:c>
       <x:c r="D18">
-        <x:v>5.71264233706176</x:v>
+        <x:v>167.721197925378</x:v>
       </x:c>
       <x:c r="E18">
-        <x:v>188.543305075049</x:v>
+        <x:v>98.1758592176139</x:v>
       </x:c>
       <x:c r="F18">
-        <x:v>43.913939429407</x:v>
+        <x:v>44.0858932417286</x:v>
       </x:c>
       <x:c r="G18">
-        <x:v>92.5664054660901</x:v>
+        <x:v>175.755454774832</x:v>
       </x:c>
       <x:c r="H18">
-        <x:v>55.4701121782279</x:v>
+        <x:v>5.95582137161671</x:v>
       </x:c>
       <x:c r="I18">
-        <x:v>154.094765965871</x:v>
+        <x:v>99.6217806356129</x:v>
       </x:c>
       <x:c r="J18">
-        <x:v>189.537888853596</x:v>
+        <x:v>188.13761034428</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="A19">
-        <x:v>133.970157305696</x:v>
+        <x:v>87.8595840595009</x:v>
       </x:c>
       <x:c r="B19">
-        <x:v>52.0537249986332</x:v>
+        <x:v>27.3156373888793</x:v>
       </x:c>
       <x:c r="C19">
-        <x:v>0.444342661855902</x:v>
+        <x:v>194.330127162081</x:v>
       </x:c>
       <x:c r="D19">
-        <x:v>45.0098265172028</x:v>
+        <x:v>187.272216094319</x:v>
       </x:c>
       <x:c r="E19">
-        <x:v>39.0465350072116</x:v>
+        <x:v>76.414859051078</x:v>
       </x:c>
       <x:c r="F19">
-        <x:v>28.6180683544921</x:v>
+        <x:v>97.5372763804799</x:v>
       </x:c>
       <x:c r="G19">
-        <x:v>30.0311219087015</x:v>
+        <x:v>56.6759311857987</x:v>
       </x:c>
       <x:c r="H19">
-        <x:v>181.447823988948</x:v>
+        <x:v>165.158634337205</x:v>
       </x:c>
       <x:c r="I19">
-        <x:v>78.2713242239651</x:v>
+        <x:v>147.930193761331</x:v>
       </x:c>
       <x:c r="J19">
-        <x:v>90.6157671895883</x:v>
+        <x:v>153.075676762068</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
       <x:c r="A20">
-        <x:v>11.6960904615447</x:v>
+        <x:v>139.535957267292</x:v>
       </x:c>
       <x:c r="B20">
-        <x:v>13.128925959174</x:v>
+        <x:v>188.719351584427</x:v>
       </x:c>
       <x:c r="C20">
-        <x:v>8.6591396521121</x:v>
+        <x:v>79.0641902382784</x:v>
       </x:c>
       <x:c r="D20">
-        <x:v>173.735203022945</x:v>
+        <x:v>102.759486950356</x:v>
       </x:c>
       <x:c r="E20">
-        <x:v>45.2738004016102</x:v>
+        <x:v>30.3083694681099</x:v>
       </x:c>
       <x:c r="F20">
-        <x:v>132.473114008304</x:v>
+        <x:v>100.906503247519</x:v>
       </x:c>
       <x:c r="G20">
-        <x:v>185.226482239192</x:v>
+        <x:v>122.551502903249</x:v>
       </x:c>
       <x:c r="H20">
-        <x:v>124.36237788031</x:v>
+        <x:v>133.534501089498</x:v>
       </x:c>
       <x:c r="I20">
-        <x:v>143.784434042771</x:v>
+        <x:v>156.09878001553</x:v>
       </x:c>
       <x:c r="J20">
-        <x:v>24.979760323176</x:v>
+        <x:v>178.797046364656</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
finita la creazione della funzione che genera il template del calendario, prossimo step, finire le date di un anno completo
</commit_message>
<xml_diff>
--- a/windows_form_app/ConditionalFormatColorScale.xlsx
+++ b/windows_form_app/ConditionalFormatColorScale.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R9a01dab572b94683"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="Rc4e342cdfb3b4c80"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -345,642 +345,642 @@
   <x:sheetData>
     <x:row r="1">
       <x:c r="A1">
-        <x:v>55.8603827170378</x:v>
+        <x:v>114.949946438405</x:v>
       </x:c>
       <x:c r="B1">
-        <x:v>46.3780275761979</x:v>
+        <x:v>185.887906973198</x:v>
       </x:c>
       <x:c r="C1">
-        <x:v>152.243937995398</x:v>
+        <x:v>125.428022316391</x:v>
       </x:c>
       <x:c r="D1">
-        <x:v>78.9956533717903</x:v>
+        <x:v>37.5679961580634</x:v>
       </x:c>
       <x:c r="E1">
-        <x:v>135.261113538994</x:v>
+        <x:v>185.454230096868</x:v>
       </x:c>
       <x:c r="F1">
-        <x:v>46.9787431168271</x:v>
+        <x:v>140.754750622788</x:v>
       </x:c>
       <x:c r="G1">
-        <x:v>91.0547565161505</x:v>
+        <x:v>123.34300536818</x:v>
       </x:c>
       <x:c r="H1">
-        <x:v>108.087243655737</x:v>
+        <x:v>100.982537540133</x:v>
       </x:c>
       <x:c r="I1">
-        <x:v>131.641277918425</x:v>
+        <x:v>13.9449718473223</x:v>
       </x:c>
       <x:c r="J1">
-        <x:v>26.7630994444541</x:v>
+        <x:v>101.5689083848</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>141.496570101705</x:v>
+        <x:v>108.717175530604</x:v>
       </x:c>
       <x:c r="B2">
-        <x:v>178.752195638955</x:v>
+        <x:v>67.9643290433867</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>1.22404526976126</x:v>
+        <x:v>84.8974579409219</x:v>
       </x:c>
       <x:c r="D2">
-        <x:v>199.819334689444</x:v>
+        <x:v>92.8327521741543</x:v>
       </x:c>
       <x:c r="E2">
-        <x:v>149.854011624052</x:v>
+        <x:v>17.196502917072</x:v>
       </x:c>
       <x:c r="F2">
-        <x:v>105.145647239473</x:v>
+        <x:v>197.092276344584</x:v>
       </x:c>
       <x:c r="G2">
-        <x:v>199.634231254288</x:v>
+        <x:v>77.6451101888181</x:v>
       </x:c>
       <x:c r="H2">
-        <x:v>35.8542567285962</x:v>
+        <x:v>107.689645377775</x:v>
       </x:c>
       <x:c r="I2">
-        <x:v>39.9836600944324</x:v>
+        <x:v>178.059247870957</x:v>
       </x:c>
       <x:c r="J2">
-        <x:v>172.899967885064</x:v>
+        <x:v>34.7992823621255</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>171.821368379435</x:v>
+        <x:v>60.0700568687497</x:v>
       </x:c>
       <x:c r="B3">
-        <x:v>183.284240580762</x:v>
+        <x:v>20.3738832941157</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>99.8080708551258</x:v>
+        <x:v>111.097120824781</x:v>
       </x:c>
       <x:c r="D3">
-        <x:v>179.59213768113</x:v>
+        <x:v>126.994203555861</x:v>
       </x:c>
       <x:c r="E3">
-        <x:v>96.4630233573089</x:v>
+        <x:v>125.388765114075</x:v>
       </x:c>
       <x:c r="F3">
-        <x:v>5.09410631148802</x:v>
+        <x:v>115.580664535789</x:v>
       </x:c>
       <x:c r="G3">
-        <x:v>187.341186212069</x:v>
+        <x:v>186.699653969472</x:v>
       </x:c>
       <x:c r="H3">
-        <x:v>132.477039998619</x:v>
+        <x:v>151.489565219492</x:v>
       </x:c>
       <x:c r="I3">
-        <x:v>107.713346233458</x:v>
+        <x:v>179.992093881588</x:v>
       </x:c>
       <x:c r="J3">
-        <x:v>40.3243849241754</x:v>
+        <x:v>153.088201188058</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>70.8726690480824</x:v>
+        <x:v>155.470422262079</x:v>
       </x:c>
       <x:c r="B4">
-        <x:v>28.3576615286794</x:v>
+        <x:v>90.3641691852194</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>69.8911891644314</x:v>
+        <x:v>182.954371898879</x:v>
       </x:c>
       <x:c r="D4">
-        <x:v>117.031572161723</x:v>
+        <x:v>192.718372397459</x:v>
       </x:c>
       <x:c r="E4">
-        <x:v>107.564645590058</x:v>
+        <x:v>55.0380260939887</x:v>
       </x:c>
       <x:c r="F4">
-        <x:v>66.6489888292965</x:v>
+        <x:v>58.4344572659742</x:v>
       </x:c>
       <x:c r="G4">
-        <x:v>137.187778547959</x:v>
+        <x:v>185.548592538363</x:v>
       </x:c>
       <x:c r="H4">
-        <x:v>144.921344399881</x:v>
+        <x:v>85.797343629318</x:v>
       </x:c>
       <x:c r="I4">
-        <x:v>29.2703065226182</x:v>
+        <x:v>81.7145861134467</x:v>
       </x:c>
       <x:c r="J4">
-        <x:v>152.582909330997</x:v>
+        <x:v>138.018755865292</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5">
-        <x:v>78.0191712444737</x:v>
+        <x:v>152.584969975327</x:v>
       </x:c>
       <x:c r="B5">
-        <x:v>183.04097791344</x:v>
+        <x:v>82.5259498704811</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>188.052196888277</x:v>
+        <x:v>94.7762802684569</x:v>
       </x:c>
       <x:c r="D5">
-        <x:v>98.3287659000274</x:v>
+        <x:v>54.5953426764325</x:v>
       </x:c>
       <x:c r="E5">
-        <x:v>55.9140092022317</x:v>
+        <x:v>36.9117616847678</x:v>
       </x:c>
       <x:c r="F5">
-        <x:v>11.3105726480999</x:v>
+        <x:v>87.587959918933</x:v>
       </x:c>
       <x:c r="G5">
-        <x:v>60.8798746303096</x:v>
+        <x:v>171.969674700857</x:v>
       </x:c>
       <x:c r="H5">
-        <x:v>13.4657994906724</x:v>
+        <x:v>102.146972949685</x:v>
       </x:c>
       <x:c r="I5">
-        <x:v>194.316295345461</x:v>
+        <x:v>97.8994711758101</x:v>
       </x:c>
       <x:c r="J5">
-        <x:v>181.430495707984</x:v>
+        <x:v>139.735567355405</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>3.9219872112954</x:v>
+        <x:v>133.168626173012</x:v>
       </x:c>
       <x:c r="B6">
-        <x:v>163.538239041128</x:v>
+        <x:v>163.818816544404</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>25.0210194964991</x:v>
+        <x:v>124.715224245896</x:v>
       </x:c>
       <x:c r="D6">
-        <x:v>33.8525410899206</x:v>
+        <x:v>16.2769996636906</x:v>
       </x:c>
       <x:c r="E6">
-        <x:v>181.53562768434</x:v>
+        <x:v>109.765918976518</x:v>
       </x:c>
       <x:c r="F6">
-        <x:v>72.5761421362758</x:v>
+        <x:v>94.576063144289</x:v>
       </x:c>
       <x:c r="G6">
-        <x:v>146.569956721072</x:v>
+        <x:v>74.7907861484172</x:v>
       </x:c>
       <x:c r="H6">
-        <x:v>172.651800314268</x:v>
+        <x:v>198.43381876053</x:v>
       </x:c>
       <x:c r="I6">
-        <x:v>182.532630014481</x:v>
+        <x:v>112.179231043988</x:v>
       </x:c>
       <x:c r="J6">
-        <x:v>130.167007227506</x:v>
+        <x:v>69.8735655610792</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>59.6375569047581</x:v>
+        <x:v>154.055096653316</x:v>
       </x:c>
       <x:c r="B7">
-        <x:v>158.577716517531</x:v>
+        <x:v>171.853440148688</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>0.373897422279183</x:v>
+        <x:v>120.990443658545</x:v>
       </x:c>
       <x:c r="D7">
-        <x:v>91.3168929942497</x:v>
+        <x:v>60.8567706592645</x:v>
       </x:c>
       <x:c r="E7">
-        <x:v>155.890430396372</x:v>
+        <x:v>146.098486122721</x:v>
       </x:c>
       <x:c r="F7">
-        <x:v>113.138908573025</x:v>
+        <x:v>18.3530063453843</x:v>
       </x:c>
       <x:c r="G7">
-        <x:v>108.861006474523</x:v>
+        <x:v>85.0099571445072</x:v>
       </x:c>
       <x:c r="H7">
-        <x:v>84.1924731080385</x:v>
+        <x:v>92.1790855434626</x:v>
       </x:c>
       <x:c r="I7">
-        <x:v>92.2546890993857</x:v>
+        <x:v>37.7947260801656</x:v>
       </x:c>
       <x:c r="J7">
-        <x:v>83.2050227947556</x:v>
+        <x:v>158.762045651098</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>167.957868691514</x:v>
+        <x:v>11.5436838062218</x:v>
       </x:c>
       <x:c r="B8">
-        <x:v>54.7128868544069</x:v>
+        <x:v>191.8477665595</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>6.58395020597798</x:v>
+        <x:v>25.9750592643279</x:v>
       </x:c>
       <x:c r="D8">
-        <x:v>87.4007507634353</x:v>
+        <x:v>40.0404920056651</x:v>
       </x:c>
       <x:c r="E8">
-        <x:v>94.8807966405902</x:v>
+        <x:v>82.2143123867988</x:v>
       </x:c>
       <x:c r="F8">
-        <x:v>188.780390465995</x:v>
+        <x:v>177.544106998269</x:v>
       </x:c>
       <x:c r="G8">
-        <x:v>195.232043692485</x:v>
+        <x:v>125.597603025659</x:v>
       </x:c>
       <x:c r="H8">
-        <x:v>1.47930495509845</x:v>
+        <x:v>56.5017781483483</x:v>
       </x:c>
       <x:c r="I8">
-        <x:v>123.678128478899</x:v>
+        <x:v>90.0824418710929</x:v>
       </x:c>
       <x:c r="J8">
-        <x:v>85.1524507092091</x:v>
+        <x:v>37.800805195142</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>144.214231681178</x:v>
+        <x:v>143.610989834932</x:v>
       </x:c>
       <x:c r="B9">
-        <x:v>173.875386721397</x:v>
+        <x:v>84.5526810197871</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>138.160744653158</x:v>
+        <x:v>53.5900940436824</x:v>
       </x:c>
       <x:c r="D9">
-        <x:v>126.282850525474</x:v>
+        <x:v>40.2565265261831</x:v>
       </x:c>
       <x:c r="E9">
-        <x:v>36.40239771288</x:v>
+        <x:v>19.9195750150455</x:v>
       </x:c>
       <x:c r="F9">
-        <x:v>107.334430006954</x:v>
+        <x:v>191.651605717676</x:v>
       </x:c>
       <x:c r="G9">
-        <x:v>3.33664203218028</x:v>
+        <x:v>165.648944939323</x:v>
       </x:c>
       <x:c r="H9">
-        <x:v>36.0386480745108</x:v>
+        <x:v>166.677372235189</x:v>
       </x:c>
       <x:c r="I9">
-        <x:v>135.495944477383</x:v>
+        <x:v>82.952453420941</x:v>
       </x:c>
       <x:c r="J9">
-        <x:v>34.9885034537821</x:v>
+        <x:v>160.4619629497</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>120.079032108224</x:v>
+        <x:v>183.643671117557</x:v>
       </x:c>
       <x:c r="B10">
-        <x:v>164.535978233691</x:v>
+        <x:v>187.114773777833</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>162.3887143854</x:v>
+        <x:v>173.618112585329</x:v>
       </x:c>
       <x:c r="D10">
-        <x:v>99.1032992951122</x:v>
+        <x:v>11.8410205523674</x:v>
       </x:c>
       <x:c r="E10">
-        <x:v>92.945352426239</x:v>
+        <x:v>183.963659211976</x:v>
       </x:c>
       <x:c r="F10">
-        <x:v>119.441454726943</x:v>
+        <x:v>180.731529826639</x:v>
       </x:c>
       <x:c r="G10">
-        <x:v>182.667080491161</x:v>
+        <x:v>161.535506211936</x:v>
       </x:c>
       <x:c r="H10">
-        <x:v>96.7353038940278</x:v>
+        <x:v>33.9195096091924</x:v>
       </x:c>
       <x:c r="I10">
-        <x:v>142.438335503656</x:v>
+        <x:v>108.496856553711</x:v>
       </x:c>
       <x:c r="J10">
-        <x:v>142.775100629206</x:v>
+        <x:v>18.5587553393835</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>102.449566173577</x:v>
+        <x:v>2.57800277442578</x:v>
       </x:c>
       <x:c r="B11">
-        <x:v>176.687401522271</x:v>
+        <x:v>79.7905891573944</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>121.211110391287</x:v>
+        <x:v>64.3522468695195</x:v>
       </x:c>
       <x:c r="D11">
-        <x:v>111.111272550705</x:v>
+        <x:v>139.137425524712</x:v>
       </x:c>
       <x:c r="E11">
-        <x:v>13.4726270164701</x:v>
+        <x:v>128.191883549184</x:v>
       </x:c>
       <x:c r="F11">
-        <x:v>149.209100356889</x:v>
+        <x:v>141.320859613512</x:v>
       </x:c>
       <x:c r="G11">
-        <x:v>156.95428883515</x:v>
+        <x:v>137.843757280076</x:v>
       </x:c>
       <x:c r="H11">
-        <x:v>137.620268733064</x:v>
+        <x:v>84.6747322402311</x:v>
       </x:c>
       <x:c r="I11">
-        <x:v>138.97174444933</x:v>
+        <x:v>134.062687276892</x:v>
       </x:c>
       <x:c r="J11">
-        <x:v>192.755237218344</x:v>
+        <x:v>132.22181197825</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
       <x:c r="A12">
-        <x:v>77.3440984437913</x:v>
+        <x:v>168.97846011863</x:v>
       </x:c>
       <x:c r="B12">
-        <x:v>145.090651765974</x:v>
+        <x:v>18.2890080000688</x:v>
       </x:c>
       <x:c r="C12">
-        <x:v>48.9736718353693</x:v>
+        <x:v>108.351376889437</x:v>
       </x:c>
       <x:c r="D12">
-        <x:v>97.3801793052723</x:v>
+        <x:v>74.3784258488465</x:v>
       </x:c>
       <x:c r="E12">
-        <x:v>185.952775546328</x:v>
+        <x:v>126.262575726147</x:v>
       </x:c>
       <x:c r="F12">
-        <x:v>85.7621701833616</x:v>
+        <x:v>69.5024156335287</x:v>
       </x:c>
       <x:c r="G12">
-        <x:v>20.4169718643729</x:v>
+        <x:v>118.263346105005</x:v>
       </x:c>
       <x:c r="H12">
-        <x:v>74.0910468968056</x:v>
+        <x:v>80.7339171323618</x:v>
       </x:c>
       <x:c r="I12">
-        <x:v>54.9144952813697</x:v>
+        <x:v>40.937195644219</x:v>
       </x:c>
       <x:c r="J12">
-        <x:v>48.5560003894176</x:v>
+        <x:v>154.446880405046</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="A13">
-        <x:v>109.802266540845</x:v>
+        <x:v>52.7040614060611</x:v>
       </x:c>
       <x:c r="B13">
-        <x:v>72.8223584000125</x:v>
+        <x:v>118.332584909318</x:v>
       </x:c>
       <x:c r="C13">
-        <x:v>148.696528630656</x:v>
+        <x:v>9.22663212252158</x:v>
       </x:c>
       <x:c r="D13">
-        <x:v>57.2661856456037</x:v>
+        <x:v>77.3327631304659</x:v>
       </x:c>
       <x:c r="E13">
-        <x:v>163.125990686531</x:v>
+        <x:v>175.118374533541</x:v>
       </x:c>
       <x:c r="F13">
-        <x:v>3.42189045782289</x:v>
+        <x:v>24.4289100283891</x:v>
       </x:c>
       <x:c r="G13">
-        <x:v>92.3241724690069</x:v>
+        <x:v>18.2296539741706</x:v>
       </x:c>
       <x:c r="H13">
-        <x:v>107.480650910866</x:v>
+        <x:v>14.1340387119604</x:v>
       </x:c>
       <x:c r="I13">
-        <x:v>194.455398337196</x:v>
+        <x:v>56.0768327936888</x:v>
       </x:c>
       <x:c r="J13">
-        <x:v>175.439341913648</x:v>
+        <x:v>101.48278256016</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="A14">
-        <x:v>6.11330997483493</x:v>
+        <x:v>16.0086007863323</x:v>
       </x:c>
       <x:c r="B14">
-        <x:v>98.4967397984568</x:v>
+        <x:v>91.6780934164664</x:v>
       </x:c>
       <x:c r="C14">
-        <x:v>59.0409694514428</x:v>
+        <x:v>148.004921594637</x:v>
       </x:c>
       <x:c r="D14">
-        <x:v>180.903027849692</x:v>
+        <x:v>71.5236865317094</x:v>
       </x:c>
       <x:c r="E14">
-        <x:v>182.702884535633</x:v>
+        <x:v>35.2228024207162</x:v>
       </x:c>
       <x:c r="F14">
-        <x:v>167.526830158907</x:v>
+        <x:v>63.8204006775377</x:v>
       </x:c>
       <x:c r="G14">
-        <x:v>52.6642763301098</x:v>
+        <x:v>20.2004341502676</x:v>
       </x:c>
       <x:c r="H14">
-        <x:v>27.0494721024528</x:v>
+        <x:v>114.45266851897</x:v>
       </x:c>
       <x:c r="I14">
-        <x:v>112.810223509004</x:v>
+        <x:v>112.064642977</x:v>
       </x:c>
       <x:c r="J14">
-        <x:v>87.1932973559915</x:v>
+        <x:v>78.5987154015334</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="A15">
-        <x:v>150.380141171804</x:v>
+        <x:v>53.8078484375998</x:v>
       </x:c>
       <x:c r="B15">
-        <x:v>65.7163732991164</x:v>
+        <x:v>80.9742126990921</x:v>
       </x:c>
       <x:c r="C15">
-        <x:v>97.0669036251804</x:v>
+        <x:v>32.6146849582971</x:v>
       </x:c>
       <x:c r="D15">
-        <x:v>142.740707259039</x:v>
+        <x:v>150.730641442691</x:v>
       </x:c>
       <x:c r="E15">
-        <x:v>157.644405009991</x:v>
+        <x:v>191.48350283107</x:v>
       </x:c>
       <x:c r="F15">
-        <x:v>174.988380342251</x:v>
+        <x:v>165.354663117488</x:v>
       </x:c>
       <x:c r="G15">
-        <x:v>115.562306398322</x:v>
+        <x:v>78.7633968883955</x:v>
       </x:c>
       <x:c r="H15">
-        <x:v>65.0085350801277</x:v>
+        <x:v>99.239686736483</x:v>
       </x:c>
       <x:c r="I15">
-        <x:v>113.150523748785</x:v>
+        <x:v>85.5784448262204</x:v>
       </x:c>
       <x:c r="J15">
-        <x:v>7.1831822428774</x:v>
+        <x:v>114.461243578448</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="A16">
-        <x:v>99.0244828625696</x:v>
+        <x:v>62.4681837216337</x:v>
       </x:c>
       <x:c r="B16">
-        <x:v>108.576033594355</x:v>
+        <x:v>80.8015890795745</x:v>
       </x:c>
       <x:c r="C16">
-        <x:v>41.8208086126581</x:v>
+        <x:v>192.982313964973</x:v>
       </x:c>
       <x:c r="D16">
-        <x:v>93.882335114238</x:v>
+        <x:v>154.049976148666</x:v>
       </x:c>
       <x:c r="E16">
-        <x:v>32.9728340883613</x:v>
+        <x:v>165.854693933322</x:v>
       </x:c>
       <x:c r="F16">
-        <x:v>29.627207773564</x:v>
+        <x:v>84.2454178651075</x:v>
       </x:c>
       <x:c r="G16">
-        <x:v>27.9908728916156</x:v>
+        <x:v>70.5639570348728</x:v>
       </x:c>
       <x:c r="H16">
-        <x:v>63.9449247456831</x:v>
+        <x:v>187.019483739054</x:v>
       </x:c>
       <x:c r="I16">
-        <x:v>147.985281864174</x:v>
+        <x:v>164.019050991172</x:v>
       </x:c>
       <x:c r="J16">
-        <x:v>10.0507365586472</x:v>
+        <x:v>103.762973520794</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="A17">
-        <x:v>56.8849278878816</x:v>
+        <x:v>123.091205639341</x:v>
       </x:c>
       <x:c r="B17">
-        <x:v>49.4736379242845</x:v>
+        <x:v>123.709718568115</x:v>
       </x:c>
       <x:c r="C17">
-        <x:v>143.164870395868</x:v>
+        <x:v>28.5978994465423</x:v>
       </x:c>
       <x:c r="D17">
-        <x:v>163.532402535683</x:v>
+        <x:v>32.5799047167319</x:v>
       </x:c>
       <x:c r="E17">
-        <x:v>186.641927243509</x:v>
+        <x:v>116.213211191917</x:v>
       </x:c>
       <x:c r="F17">
-        <x:v>178.847358645335</x:v>
+        <x:v>77.3003667021638</x:v>
       </x:c>
       <x:c r="G17">
-        <x:v>86.0496823145308</x:v>
+        <x:v>70.2840864054319</x:v>
       </x:c>
       <x:c r="H17">
-        <x:v>68.0706439856769</x:v>
+        <x:v>36.8276903577278</x:v>
       </x:c>
       <x:c r="I17">
-        <x:v>114.67729476964</x:v>
+        <x:v>39.1556234281303</x:v>
       </x:c>
       <x:c r="J17">
-        <x:v>18.4259453874202</x:v>
+        <x:v>62.4421750486094</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="A18">
-        <x:v>33.0978938532518</x:v>
+        <x:v>49.3019814832611</x:v>
       </x:c>
       <x:c r="B18">
-        <x:v>193.36749976192</x:v>
+        <x:v>3.81067758603519</x:v>
       </x:c>
       <x:c r="C18">
-        <x:v>161.280823387802</x:v>
+        <x:v>168.669274155362</x:v>
       </x:c>
       <x:c r="D18">
-        <x:v>167.721197925378</x:v>
+        <x:v>162.338480242686</x:v>
       </x:c>
       <x:c r="E18">
-        <x:v>98.1758592176139</x:v>
+        <x:v>100.639031967446</x:v>
       </x:c>
       <x:c r="F18">
-        <x:v>44.0858932417286</x:v>
+        <x:v>171.729848706969</x:v>
       </x:c>
       <x:c r="G18">
-        <x:v>175.755454774832</x:v>
+        <x:v>85.7178999510211</x:v>
       </x:c>
       <x:c r="H18">
-        <x:v>5.95582137161671</x:v>
+        <x:v>58.4959906798303</x:v>
       </x:c>
       <x:c r="I18">
-        <x:v>99.6217806356129</x:v>
+        <x:v>85.8492602993964</x:v>
       </x:c>
       <x:c r="J18">
-        <x:v>188.13761034428</x:v>
+        <x:v>9.76371141605252</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="A19">
-        <x:v>87.8595840595009</x:v>
+        <x:v>145.665513139994</x:v>
       </x:c>
       <x:c r="B19">
-        <x:v>27.3156373888793</x:v>
+        <x:v>118.989967237688</x:v>
       </x:c>
       <x:c r="C19">
-        <x:v>194.330127162081</x:v>
+        <x:v>128.55559388574</x:v>
       </x:c>
       <x:c r="D19">
-        <x:v>187.272216094319</x:v>
+        <x:v>141.615589215241</x:v>
       </x:c>
       <x:c r="E19">
-        <x:v>76.414859051078</x:v>
+        <x:v>39.0145988385261</x:v>
       </x:c>
       <x:c r="F19">
-        <x:v>97.5372763804799</x:v>
+        <x:v>135.207011706758</x:v>
       </x:c>
       <x:c r="G19">
-        <x:v>56.6759311857987</x:v>
+        <x:v>98.6957794514931</x:v>
       </x:c>
       <x:c r="H19">
-        <x:v>165.158634337205</x:v>
+        <x:v>193.954945445971</x:v>
       </x:c>
       <x:c r="I19">
-        <x:v>147.930193761331</x:v>
+        <x:v>105.668992598387</x:v>
       </x:c>
       <x:c r="J19">
-        <x:v>153.075676762068</x:v>
+        <x:v>150.977384555609</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
       <x:c r="A20">
-        <x:v>139.535957267292</x:v>
+        <x:v>193.256443642665</x:v>
       </x:c>
       <x:c r="B20">
-        <x:v>188.719351584427</x:v>
+        <x:v>33.180950411214</x:v>
       </x:c>
       <x:c r="C20">
-        <x:v>79.0641902382784</x:v>
+        <x:v>150.433617527799</x:v>
       </x:c>
       <x:c r="D20">
-        <x:v>102.759486950356</x:v>
+        <x:v>8.30166945620518</x:v>
       </x:c>
       <x:c r="E20">
-        <x:v>30.3083694681099</x:v>
+        <x:v>155.507509762192</x:v>
       </x:c>
       <x:c r="F20">
-        <x:v>100.906503247519</x:v>
+        <x:v>130.098129869484</x:v>
       </x:c>
       <x:c r="G20">
-        <x:v>122.551502903249</x:v>
+        <x:v>52.3763132525498</x:v>
       </x:c>
       <x:c r="H20">
-        <x:v>133.534501089498</x:v>
+        <x:v>0.0347802415652109</x:v>
       </x:c>
       <x:c r="I20">
-        <x:v>156.09878001553</x:v>
+        <x:v>34.5174302507739</x:v>
       </x:c>
       <x:c r="J20">
-        <x:v>178.797046364656</x:v>
+        <x:v>114.183136128906</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
manca il mese di dicembre da mostrare nel foglio excel
</commit_message>
<xml_diff>
--- a/windows_form_app/ConditionalFormatColorScale.xlsx
+++ b/windows_form_app/ConditionalFormatColorScale.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="Rc4e342cdfb3b4c80"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="Rd74eb92fa2c04a7e"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -345,642 +345,642 @@
   <x:sheetData>
     <x:row r="1">
       <x:c r="A1">
-        <x:v>114.949946438405</x:v>
+        <x:v>78.4078284531868</x:v>
       </x:c>
       <x:c r="B1">
-        <x:v>185.887906973198</x:v>
+        <x:v>182.564449209051</x:v>
       </x:c>
       <x:c r="C1">
-        <x:v>125.428022316391</x:v>
+        <x:v>67.3528387524899</x:v>
       </x:c>
       <x:c r="D1">
-        <x:v>37.5679961580634</x:v>
+        <x:v>79.6841525843759</x:v>
       </x:c>
       <x:c r="E1">
-        <x:v>185.454230096868</x:v>
+        <x:v>28.5875222778821</x:v>
       </x:c>
       <x:c r="F1">
-        <x:v>140.754750622788</x:v>
+        <x:v>87.8914307280869</x:v>
       </x:c>
       <x:c r="G1">
-        <x:v>123.34300536818</x:v>
+        <x:v>15.1879239898119</x:v>
       </x:c>
       <x:c r="H1">
-        <x:v>100.982537540133</x:v>
+        <x:v>11.9976429324586</x:v>
       </x:c>
       <x:c r="I1">
-        <x:v>13.9449718473223</x:v>
+        <x:v>60.7411978117848</x:v>
       </x:c>
       <x:c r="J1">
-        <x:v>101.5689083848</x:v>
+        <x:v>118.26333390468</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>108.717175530604</x:v>
+        <x:v>89.9166619823857</x:v>
       </x:c>
       <x:c r="B2">
-        <x:v>67.9643290433867</x:v>
+        <x:v>30.4632081792053</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>84.8974579409219</x:v>
+        <x:v>58.6066634667137</x:v>
       </x:c>
       <x:c r="D2">
-        <x:v>92.8327521741543</x:v>
+        <x:v>156.719543019645</x:v>
       </x:c>
       <x:c r="E2">
-        <x:v>17.196502917072</x:v>
+        <x:v>178.465342232243</x:v>
       </x:c>
       <x:c r="F2">
-        <x:v>197.092276344584</x:v>
+        <x:v>144.7297707874</x:v>
       </x:c>
       <x:c r="G2">
-        <x:v>77.6451101888181</x:v>
+        <x:v>142.85651079512</x:v>
       </x:c>
       <x:c r="H2">
-        <x:v>107.689645377775</x:v>
+        <x:v>127.029146592612</x:v>
       </x:c>
       <x:c r="I2">
-        <x:v>178.059247870957</x:v>
+        <x:v>118.892595227292</x:v>
       </x:c>
       <x:c r="J2">
-        <x:v>34.7992823621255</x:v>
+        <x:v>24.179480515504</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>60.0700568687497</x:v>
+        <x:v>13.2353526601733</x:v>
       </x:c>
       <x:c r="B3">
-        <x:v>20.3738832941157</x:v>
+        <x:v>16.789862335096</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>111.097120824781</x:v>
+        <x:v>64.4125092143251</x:v>
       </x:c>
       <x:c r="D3">
-        <x:v>126.994203555861</x:v>
+        <x:v>91.0139336674539</x:v>
       </x:c>
       <x:c r="E3">
-        <x:v>125.388765114075</x:v>
+        <x:v>60.0258050765962</x:v>
       </x:c>
       <x:c r="F3">
-        <x:v>115.580664535789</x:v>
+        <x:v>190.012591327546</x:v>
       </x:c>
       <x:c r="G3">
-        <x:v>186.699653969472</x:v>
+        <x:v>165.737399629195</x:v>
       </x:c>
       <x:c r="H3">
-        <x:v>151.489565219492</x:v>
+        <x:v>136.806406703222</x:v>
       </x:c>
       <x:c r="I3">
-        <x:v>179.992093881588</x:v>
+        <x:v>70.7165700712784</x:v>
       </x:c>
       <x:c r="J3">
-        <x:v>153.088201188058</x:v>
+        <x:v>90.2644459578509</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>155.470422262079</x:v>
+        <x:v>42.051677052887</x:v>
       </x:c>
       <x:c r="B4">
-        <x:v>90.3641691852194</x:v>
+        <x:v>74.0834727296994</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>182.954371898879</x:v>
+        <x:v>96.4409285674062</x:v>
       </x:c>
       <x:c r="D4">
-        <x:v>192.718372397459</x:v>
+        <x:v>84.5790998472735</x:v>
       </x:c>
       <x:c r="E4">
-        <x:v>55.0380260939887</x:v>
+        <x:v>146.582222239385</x:v>
       </x:c>
       <x:c r="F4">
-        <x:v>58.4344572659742</x:v>
+        <x:v>99.0692046932267</x:v>
       </x:c>
       <x:c r="G4">
-        <x:v>185.548592538363</x:v>
+        <x:v>171.283539184967</x:v>
       </x:c>
       <x:c r="H4">
-        <x:v>85.797343629318</x:v>
+        <x:v>70.1933742827705</x:v>
       </x:c>
       <x:c r="I4">
-        <x:v>81.7145861134467</x:v>
+        <x:v>44.858923389045</x:v>
       </x:c>
       <x:c r="J4">
-        <x:v>138.018755865292</x:v>
+        <x:v>195.312695296161</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5">
-        <x:v>152.584969975327</x:v>
+        <x:v>21.3417588832517</x:v>
       </x:c>
       <x:c r="B5">
-        <x:v>82.5259498704811</x:v>
+        <x:v>99.9221572186435</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>94.7762802684569</x:v>
+        <x:v>123.754329664518</x:v>
       </x:c>
       <x:c r="D5">
-        <x:v>54.5953426764325</x:v>
+        <x:v>22.8757538007925</x:v>
       </x:c>
       <x:c r="E5">
-        <x:v>36.9117616847678</x:v>
+        <x:v>122.170106099066</x:v>
       </x:c>
       <x:c r="F5">
-        <x:v>87.587959918933</x:v>
+        <x:v>170.510997982002</x:v>
       </x:c>
       <x:c r="G5">
-        <x:v>171.969674700857</x:v>
+        <x:v>154.685959478228</x:v>
       </x:c>
       <x:c r="H5">
-        <x:v>102.146972949685</x:v>
+        <x:v>153.219697137</x:v>
       </x:c>
       <x:c r="I5">
-        <x:v>97.8994711758101</x:v>
+        <x:v>46.0396748250535</x:v>
       </x:c>
       <x:c r="J5">
-        <x:v>139.735567355405</x:v>
+        <x:v>123.379056771928</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>133.168626173012</x:v>
+        <x:v>166.750805902644</x:v>
       </x:c>
       <x:c r="B6">
-        <x:v>163.818816544404</x:v>
+        <x:v>54.0387402540253</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>124.715224245896</x:v>
+        <x:v>199.319233093094</x:v>
       </x:c>
       <x:c r="D6">
-        <x:v>16.2769996636906</x:v>
+        <x:v>175.136718701169</x:v>
       </x:c>
       <x:c r="E6">
-        <x:v>109.765918976518</x:v>
+        <x:v>2.42712525763881</x:v>
       </x:c>
       <x:c r="F6">
-        <x:v>94.576063144289</x:v>
+        <x:v>61.6179661180908</x:v>
       </x:c>
       <x:c r="G6">
-        <x:v>74.7907861484172</x:v>
+        <x:v>118.151939994726</x:v>
       </x:c>
       <x:c r="H6">
-        <x:v>198.43381876053</x:v>
+        <x:v>176.338905085036</x:v>
       </x:c>
       <x:c r="I6">
-        <x:v>112.179231043988</x:v>
+        <x:v>19.6583475077796</x:v>
       </x:c>
       <x:c r="J6">
-        <x:v>69.8735655610792</x:v>
+        <x:v>38.5749309503357</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>154.055096653316</x:v>
+        <x:v>122.154031098892</x:v>
       </x:c>
       <x:c r="B7">
-        <x:v>171.853440148688</x:v>
+        <x:v>78.3815172865901</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>120.990443658545</x:v>
+        <x:v>141.28107286118</x:v>
       </x:c>
       <x:c r="D7">
-        <x:v>60.8567706592645</x:v>
+        <x:v>170.476751853934</x:v>
       </x:c>
       <x:c r="E7">
-        <x:v>146.098486122721</x:v>
+        <x:v>76.2116568517926</x:v>
       </x:c>
       <x:c r="F7">
-        <x:v>18.3530063453843</x:v>
+        <x:v>15.8331892526863</x:v>
       </x:c>
       <x:c r="G7">
-        <x:v>85.0099571445072</x:v>
+        <x:v>134.022279611799</x:v>
       </x:c>
       <x:c r="H7">
-        <x:v>92.1790855434626</x:v>
+        <x:v>174.02756361944</x:v>
       </x:c>
       <x:c r="I7">
-        <x:v>37.7947260801656</x:v>
+        <x:v>10.1373207802592</x:v>
       </x:c>
       <x:c r="J7">
-        <x:v>158.762045651098</x:v>
+        <x:v>79.3961375390161</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>11.5436838062218</x:v>
+        <x:v>173.446231602433</x:v>
       </x:c>
       <x:c r="B8">
-        <x:v>191.8477665595</x:v>
+        <x:v>72.6631365123499</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>25.9750592643279</x:v>
+        <x:v>82.170223203567</x:v>
       </x:c>
       <x:c r="D8">
-        <x:v>40.0404920056651</x:v>
+        <x:v>123.579899931131</x:v>
       </x:c>
       <x:c r="E8">
-        <x:v>82.2143123867988</x:v>
+        <x:v>2.83772163225232</x:v>
       </x:c>
       <x:c r="F8">
-        <x:v>177.544106998269</x:v>
+        <x:v>113.31319544153</x:v>
       </x:c>
       <x:c r="G8">
-        <x:v>125.597603025659</x:v>
+        <x:v>93.0355326705778</x:v>
       </x:c>
       <x:c r="H8">
-        <x:v>56.5017781483483</x:v>
+        <x:v>41.5367554135326</x:v>
       </x:c>
       <x:c r="I8">
-        <x:v>90.0824418710929</x:v>
+        <x:v>168.843827568388</x:v>
       </x:c>
       <x:c r="J8">
-        <x:v>37.800805195142</x:v>
+        <x:v>89.5148070945939</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>143.610989834932</x:v>
+        <x:v>35.3266318493181</x:v>
       </x:c>
       <x:c r="B9">
-        <x:v>84.5526810197871</x:v>
+        <x:v>12.517702492195</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>53.5900940436824</x:v>
+        <x:v>90.7667318781683</x:v>
       </x:c>
       <x:c r="D9">
-        <x:v>40.2565265261831</x:v>
+        <x:v>147.33751329935</x:v>
       </x:c>
       <x:c r="E9">
-        <x:v>19.9195750150455</x:v>
+        <x:v>123.513640055206</x:v>
       </x:c>
       <x:c r="F9">
-        <x:v>191.651605717676</x:v>
+        <x:v>188.012936798862</x:v>
       </x:c>
       <x:c r="G9">
-        <x:v>165.648944939323</x:v>
+        <x:v>74.7642396366057</x:v>
       </x:c>
       <x:c r="H9">
-        <x:v>166.677372235189</x:v>
+        <x:v>121.304209866237</x:v>
       </x:c>
       <x:c r="I9">
-        <x:v>82.952453420941</x:v>
+        <x:v>82.1519745896347</x:v>
       </x:c>
       <x:c r="J9">
-        <x:v>160.4619629497</x:v>
+        <x:v>84.9642561212947</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>183.643671117557</x:v>
+        <x:v>180.9172646985</x:v>
       </x:c>
       <x:c r="B10">
-        <x:v>187.114773777833</x:v>
+        <x:v>194.944634099931</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>173.618112585329</x:v>
+        <x:v>50.5350267749909</x:v>
       </x:c>
       <x:c r="D10">
-        <x:v>11.8410205523674</x:v>
+        <x:v>6.28399243870936</x:v>
       </x:c>
       <x:c r="E10">
-        <x:v>183.963659211976</x:v>
+        <x:v>73.1586641972692</x:v>
       </x:c>
       <x:c r="F10">
-        <x:v>180.731529826639</x:v>
+        <x:v>142.960241596662</x:v>
       </x:c>
       <x:c r="G10">
-        <x:v>161.535506211936</x:v>
+        <x:v>158.641084357463</x:v>
       </x:c>
       <x:c r="H10">
-        <x:v>33.9195096091924</x:v>
+        <x:v>153.277577810584</x:v>
       </x:c>
       <x:c r="I10">
-        <x:v>108.496856553711</x:v>
+        <x:v>146.664096949</x:v>
       </x:c>
       <x:c r="J10">
-        <x:v>18.5587553393835</x:v>
+        <x:v>106.33691684638</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>2.57800277442578</x:v>
+        <x:v>36.4887183702033</x:v>
       </x:c>
       <x:c r="B11">
-        <x:v>79.7905891573944</x:v>
+        <x:v>180.658395858788</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>64.3522468695195</x:v>
+        <x:v>143.082376356741</x:v>
       </x:c>
       <x:c r="D11">
-        <x:v>139.137425524712</x:v>
+        <x:v>166.643537286037</x:v>
       </x:c>
       <x:c r="E11">
-        <x:v>128.191883549184</x:v>
+        <x:v>149.932825169495</x:v>
       </x:c>
       <x:c r="F11">
-        <x:v>141.320859613512</x:v>
+        <x:v>94.0876693902946</x:v>
       </x:c>
       <x:c r="G11">
-        <x:v>137.843757280076</x:v>
+        <x:v>171.868517050458</x:v>
       </x:c>
       <x:c r="H11">
-        <x:v>84.6747322402311</x:v>
+        <x:v>75.7393331619628</x:v>
       </x:c>
       <x:c r="I11">
-        <x:v>134.062687276892</x:v>
+        <x:v>172.298997068917</x:v>
       </x:c>
       <x:c r="J11">
-        <x:v>132.22181197825</x:v>
+        <x:v>89.1139298161091</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
       <x:c r="A12">
-        <x:v>168.97846011863</x:v>
+        <x:v>168.582433447513</x:v>
       </x:c>
       <x:c r="B12">
-        <x:v>18.2890080000688</x:v>
+        <x:v>76.6151845811937</x:v>
       </x:c>
       <x:c r="C12">
-        <x:v>108.351376889437</x:v>
+        <x:v>7.49507751664849</x:v>
       </x:c>
       <x:c r="D12">
-        <x:v>74.3784258488465</x:v>
+        <x:v>130.143540413186</x:v>
       </x:c>
       <x:c r="E12">
-        <x:v>126.262575726147</x:v>
+        <x:v>3.24829910101756</x:v>
       </x:c>
       <x:c r="F12">
-        <x:v>69.5024156335287</x:v>
+        <x:v>109.636328606697</x:v>
       </x:c>
       <x:c r="G12">
-        <x:v>118.263346105005</x:v>
+        <x:v>187.614785408422</x:v>
       </x:c>
       <x:c r="H12">
-        <x:v>80.7339171323618</x:v>
+        <x:v>193.94355956183</x:v>
       </x:c>
       <x:c r="I12">
-        <x:v>40.937195644219</x:v>
+        <x:v>46.9631117987275</x:v>
       </x:c>
       <x:c r="J12">
-        <x:v>154.446880405046</x:v>
+        <x:v>88.1987200529309</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="A13">
-        <x:v>52.7040614060611</x:v>
+        <x:v>141.068949616081</x:v>
       </x:c>
       <x:c r="B13">
-        <x:v>118.332584909318</x:v>
+        <x:v>12.7180697455621</x:v>
       </x:c>
       <x:c r="C13">
-        <x:v>9.22663212252158</x:v>
+        <x:v>91.8755890298056</x:v>
       </x:c>
       <x:c r="D13">
-        <x:v>77.3327631304659</x:v>
+        <x:v>125.173064658965</x:v>
       </x:c>
       <x:c r="E13">
-        <x:v>175.118374533541</x:v>
+        <x:v>98.4788728405157</x:v>
       </x:c>
       <x:c r="F13">
-        <x:v>24.4289100283891</x:v>
+        <x:v>178.501597502502</x:v>
       </x:c>
       <x:c r="G13">
-        <x:v>18.2296539741706</x:v>
+        <x:v>22.128109737359</x:v>
       </x:c>
       <x:c r="H13">
-        <x:v>14.1340387119604</x:v>
+        <x:v>75.8862307648576</x:v>
       </x:c>
       <x:c r="I13">
-        <x:v>56.0768327936888</x:v>
+        <x:v>50.4212357338617</x:v>
       </x:c>
       <x:c r="J13">
-        <x:v>101.48278256016</x:v>
+        <x:v>59.8774800355907</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="A14">
-        <x:v>16.0086007863323</x:v>
+        <x:v>154.672111084066</x:v>
       </x:c>
       <x:c r="B14">
-        <x:v>91.6780934164664</x:v>
+        <x:v>139.757954859993</x:v>
       </x:c>
       <x:c r="C14">
-        <x:v>148.004921594637</x:v>
+        <x:v>94.8726584645327</x:v>
       </x:c>
       <x:c r="D14">
-        <x:v>71.5236865317094</x:v>
+        <x:v>62.5069107220075</x:v>
       </x:c>
       <x:c r="E14">
-        <x:v>35.2228024207162</x:v>
+        <x:v>53.0260887243906</x:v>
       </x:c>
       <x:c r="F14">
-        <x:v>63.8204006775377</x:v>
+        <x:v>54.66823599053</x:v>
       </x:c>
       <x:c r="G14">
-        <x:v>20.2004341502676</x:v>
+        <x:v>69.4353261354544</x:v>
       </x:c>
       <x:c r="H14">
-        <x:v>114.45266851897</x:v>
+        <x:v>124.123194592131</x:v>
       </x:c>
       <x:c r="I14">
-        <x:v>112.064642977</x:v>
+        <x:v>197.404688129856</x:v>
       </x:c>
       <x:c r="J14">
-        <x:v>78.5987154015334</x:v>
+        <x:v>29.4259706649119</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="A15">
-        <x:v>53.8078484375998</x:v>
+        <x:v>16.1444197484033</x:v>
       </x:c>
       <x:c r="B15">
-        <x:v>80.9742126990921</x:v>
+        <x:v>199.024906474643</x:v>
       </x:c>
       <x:c r="C15">
-        <x:v>32.6146849582971</x:v>
+        <x:v>149.00521279732</x:v>
       </x:c>
       <x:c r="D15">
-        <x:v>150.730641442691</x:v>
+        <x:v>193.038044773526</x:v>
       </x:c>
       <x:c r="E15">
-        <x:v>191.48350283107</x:v>
+        <x:v>116.381822673782</x:v>
       </x:c>
       <x:c r="F15">
-        <x:v>165.354663117488</x:v>
+        <x:v>104.302080117307</x:v>
       </x:c>
       <x:c r="G15">
-        <x:v>78.7633968883955</x:v>
+        <x:v>187.449556583282</x:v>
       </x:c>
       <x:c r="H15">
-        <x:v>99.239686736483</x:v>
+        <x:v>120.391486361805</x:v>
       </x:c>
       <x:c r="I15">
-        <x:v>85.5784448262204</x:v>
+        <x:v>3.0356933376918</x:v>
       </x:c>
       <x:c r="J15">
-        <x:v>114.461243578448</x:v>
+        <x:v>163.522335590572</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="A16">
-        <x:v>62.4681837216337</x:v>
+        <x:v>155.34545618824</x:v>
       </x:c>
       <x:c r="B16">
-        <x:v>80.8015890795745</x:v>
+        <x:v>164.697524795634</x:v>
       </x:c>
       <x:c r="C16">
-        <x:v>192.982313964973</x:v>
+        <x:v>106.314466011857</x:v>
       </x:c>
       <x:c r="D16">
-        <x:v>154.049976148666</x:v>
+        <x:v>58.4653768960691</x:v>
       </x:c>
       <x:c r="E16">
-        <x:v>165.854693933322</x:v>
+        <x:v>165.267967230299</x:v>
       </x:c>
       <x:c r="F16">
-        <x:v>84.2454178651075</x:v>
+        <x:v>23.7706486246412</x:v>
       </x:c>
       <x:c r="G16">
-        <x:v>70.5639570348728</x:v>
+        <x:v>88.7828068289826</x:v>
       </x:c>
       <x:c r="H16">
-        <x:v>187.019483739054</x:v>
+        <x:v>17.9093116977761</x:v>
       </x:c>
       <x:c r="I16">
-        <x:v>164.019050991172</x:v>
+        <x:v>68.1646644455216</x:v>
       </x:c>
       <x:c r="J16">
-        <x:v>103.762973520794</x:v>
+        <x:v>171.431227666992</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="A17">
-        <x:v>123.091205639341</x:v>
+        <x:v>71.9595596529355</x:v>
       </x:c>
       <x:c r="B17">
-        <x:v>123.709718568115</x:v>
+        <x:v>95.9822862856008</x:v>
       </x:c>
       <x:c r="C17">
-        <x:v>28.5978994465423</x:v>
+        <x:v>25.3180974281012</x:v>
       </x:c>
       <x:c r="D17">
-        <x:v>32.5799047167319</x:v>
+        <x:v>112.421517033326</x:v>
       </x:c>
       <x:c r="E17">
-        <x:v>116.213211191917</x:v>
+        <x:v>134.441818732043</x:v>
       </x:c>
       <x:c r="F17">
-        <x:v>77.3003667021638</x:v>
+        <x:v>28.8244785875196</x:v>
       </x:c>
       <x:c r="G17">
-        <x:v>70.2840864054319</x:v>
+        <x:v>181.742526116661</x:v>
       </x:c>
       <x:c r="H17">
-        <x:v>36.8276903577278</x:v>
+        <x:v>144.988166794641</x:v>
       </x:c>
       <x:c r="I17">
-        <x:v>39.1556234281303</x:v>
+        <x:v>77.1174516887951</x:v>
       </x:c>
       <x:c r="J17">
-        <x:v>62.4421750486094</x:v>
+        <x:v>148.580063110488</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="A18">
-        <x:v>49.3019814832611</x:v>
+        <x:v>40.2010024712426</x:v>
       </x:c>
       <x:c r="B18">
-        <x:v>3.81067758603519</x:v>
+        <x:v>63.4915908162909</x:v>
       </x:c>
       <x:c r="C18">
-        <x:v>168.669274155362</x:v>
+        <x:v>196.538871431974</x:v>
       </x:c>
       <x:c r="D18">
-        <x:v>162.338480242686</x:v>
+        <x:v>17.5371411338156</x:v>
       </x:c>
       <x:c r="E18">
-        <x:v>100.639031967446</x:v>
+        <x:v>72.0543003045275</x:v>
       </x:c>
       <x:c r="F18">
-        <x:v>171.729848706969</x:v>
+        <x:v>142.044043141438</x:v>
       </x:c>
       <x:c r="G18">
-        <x:v>85.7178999510211</x:v>
+        <x:v>63.712856948242</x:v>
       </x:c>
       <x:c r="H18">
-        <x:v>58.4959906798303</x:v>
+        <x:v>98.83754425628</x:v>
       </x:c>
       <x:c r="I18">
-        <x:v>85.8492602993964</x:v>
+        <x:v>8.79124198518286</x:v>
       </x:c>
       <x:c r="J18">
-        <x:v>9.76371141605252</x:v>
+        <x:v>194.176792723209</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="A19">
-        <x:v>145.665513139994</x:v>
+        <x:v>191.05204091922</x:v>
       </x:c>
       <x:c r="B19">
-        <x:v>118.989967237688</x:v>
+        <x:v>101.736623375554</x:v>
       </x:c>
       <x:c r="C19">
-        <x:v>128.55559388574</x:v>
+        <x:v>72.8505374271658</x:v>
       </x:c>
       <x:c r="D19">
-        <x:v>141.615589215241</x:v>
+        <x:v>86.8989001432894</x:v>
       </x:c>
       <x:c r="E19">
-        <x:v>39.0145988385261</x:v>
+        <x:v>104.532023847351</x:v>
       </x:c>
       <x:c r="F19">
-        <x:v>135.207011706758</x:v>
+        <x:v>189.974586288433</x:v>
       </x:c>
       <x:c r="G19">
-        <x:v>98.6957794514931</x:v>
+        <x:v>33.4434888481365</x:v>
       </x:c>
       <x:c r="H19">
-        <x:v>193.954945445971</x:v>
+        <x:v>36.4072815684636</x:v>
       </x:c>
       <x:c r="I19">
-        <x:v>105.668992598387</x:v>
+        <x:v>97.238943491708</x:v>
       </x:c>
       <x:c r="J19">
-        <x:v>150.977384555609</x:v>
+        <x:v>29.2554400997495</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
       <x:c r="A20">
-        <x:v>193.256443642665</x:v>
+        <x:v>165.885429161547</x:v>
       </x:c>
       <x:c r="B20">
-        <x:v>33.180950411214</x:v>
+        <x:v>51.5260144376783</x:v>
       </x:c>
       <x:c r="C20">
-        <x:v>150.433617527799</x:v>
+        <x:v>55.9585301466093</x:v>
       </x:c>
       <x:c r="D20">
-        <x:v>8.30166945620518</x:v>
+        <x:v>25.9734604628633</x:v>
       </x:c>
       <x:c r="E20">
-        <x:v>155.507509762192</x:v>
+        <x:v>157.466411011976</x:v>
       </x:c>
       <x:c r="F20">
-        <x:v>130.098129869484</x:v>
+        <x:v>120.162133462803</x:v>
       </x:c>
       <x:c r="G20">
-        <x:v>52.3763132525498</x:v>
+        <x:v>173.706809046542</x:v>
       </x:c>
       <x:c r="H20">
-        <x:v>0.0347802415652109</x:v>
+        <x:v>36.5836957639939</x:v>
       </x:c>
       <x:c r="I20">
-        <x:v>34.5174302507739</x:v>
+        <x:v>58.5962260414829</x:v>
       </x:c>
       <x:c r="J20">
-        <x:v>114.183136128906</x:v>
+        <x:v>87.5573440862621</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
finito l'anno, ma non dinamico, non reisco a trovare il modo di farlo auto-aggiornan
</commit_message>
<xml_diff>
--- a/windows_form_app/ConditionalFormatColorScale.xlsx
+++ b/windows_form_app/ConditionalFormatColorScale.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R4f066a9e9e6b4c43"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R89ec1bc19f854cbe"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -345,642 +345,642 @@
   <x:sheetData>
     <x:row r="1">
       <x:c r="A1">
-        <x:v>142.387362356478</x:v>
+        <x:v>32.9414084707114</x:v>
       </x:c>
       <x:c r="B1">
-        <x:v>94.565136309045</x:v>
+        <x:v>108.116717780063</x:v>
       </x:c>
       <x:c r="C1">
-        <x:v>174.999694793951</x:v>
+        <x:v>188.851263741428</x:v>
       </x:c>
       <x:c r="D1">
-        <x:v>16.9435832728369</x:v>
+        <x:v>9.29911081180866</x:v>
       </x:c>
       <x:c r="E1">
-        <x:v>135.056371863492</x:v>
+        <x:v>91.1148366942605</x:v>
       </x:c>
       <x:c r="F1">
-        <x:v>124.156704602836</x:v>
+        <x:v>156.880231554099</x:v>
       </x:c>
       <x:c r="G1">
-        <x:v>125.139836745867</x:v>
+        <x:v>11.7141144404719</x:v>
       </x:c>
       <x:c r="H1">
-        <x:v>9.2035966036858</x:v>
+        <x:v>149.384023877505</x:v>
       </x:c>
       <x:c r="I1">
-        <x:v>1.04418238673554</x:v>
+        <x:v>53.415918561358</x:v>
       </x:c>
       <x:c r="J1">
-        <x:v>55.6009685879578</x:v>
+        <x:v>164.375875314873</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>191.851879559388</x:v>
+        <x:v>28.8470517046969</x:v>
       </x:c>
       <x:c r="B2">
-        <x:v>42.4258630920322</x:v>
+        <x:v>140.439572716337</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>182.397302883862</x:v>
+        <x:v>124.278133792932</x:v>
       </x:c>
       <x:c r="D2">
-        <x:v>13.7158932228181</x:v>
+        <x:v>0.282906275374306</x:v>
       </x:c>
       <x:c r="E2">
-        <x:v>126.06074517875</x:v>
+        <x:v>112.74384237488</x:v>
       </x:c>
       <x:c r="F2">
-        <x:v>11.2924912997021</x:v>
+        <x:v>86.9387512500113</x:v>
       </x:c>
       <x:c r="G2">
-        <x:v>32.2453376055906</x:v>
+        <x:v>150.847064308285</x:v>
       </x:c>
       <x:c r="H2">
-        <x:v>5.26013477019041</x:v>
+        <x:v>179.575945334312</x:v>
       </x:c>
       <x:c r="I2">
-        <x:v>24.1248241738066</x:v>
+        <x:v>107.160048516076</x:v>
       </x:c>
       <x:c r="J2">
-        <x:v>38.7006974959284</x:v>
+        <x:v>190.545255965807</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>61.0862390422664</x:v>
+        <x:v>66.217780423452</x:v>
       </x:c>
       <x:c r="B3">
-        <x:v>158.72392699063</x:v>
+        <x:v>7.18497354871825</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>10.114102442802</x:v>
+        <x:v>3.4049037859798</x:v>
       </x:c>
       <x:c r="D3">
-        <x:v>23.2137896228646</x:v>
+        <x:v>128.198529560211</x:v>
       </x:c>
       <x:c r="E3">
-        <x:v>91.9238473716769</x:v>
+        <x:v>174.958692851923</x:v>
       </x:c>
       <x:c r="F3">
-        <x:v>146.466026430235</x:v>
+        <x:v>154.288465228997</x:v>
       </x:c>
       <x:c r="G3">
-        <x:v>183.173015426459</x:v>
+        <x:v>25.108172942469</x:v>
       </x:c>
       <x:c r="H3">
-        <x:v>82.7354509768707</x:v>
+        <x:v>103.82220945499</x:v>
       </x:c>
       <x:c r="I3">
-        <x:v>114.754220244826</x:v>
+        <x:v>132.524444410822</x:v>
       </x:c>
       <x:c r="J3">
-        <x:v>178.561466549785</x:v>
+        <x:v>108.985220039722</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>179.214997021116</x:v>
+        <x:v>195.135846172988</x:v>
       </x:c>
       <x:c r="B4">
-        <x:v>46.0777153475572</x:v>
+        <x:v>2.64957714949249</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>70.9949544961541</x:v>
+        <x:v>5.7952925589845</x:v>
       </x:c>
       <x:c r="D4">
-        <x:v>3.20866545811699</x:v>
+        <x:v>102.310986119467</x:v>
       </x:c>
       <x:c r="E4">
-        <x:v>105.442541979925</x:v>
+        <x:v>18.1320874104891</x:v>
       </x:c>
       <x:c r="F4">
-        <x:v>171.719427766148</x:v>
+        <x:v>114.406534989554</x:v>
       </x:c>
       <x:c r="G4">
-        <x:v>192.027862738831</x:v>
+        <x:v>181.640655725096</x:v>
       </x:c>
       <x:c r="H4">
-        <x:v>129.996733427978</x:v>
+        <x:v>7.13782022108222</x:v>
       </x:c>
       <x:c r="I4">
-        <x:v>145.126113921928</x:v>
+        <x:v>152.050067648315</x:v>
       </x:c>
       <x:c r="J4">
-        <x:v>37.3431131417598</x:v>
+        <x:v>182.08702103332</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5">
-        <x:v>37.720557133537</x:v>
+        <x:v>183.363339576574</x:v>
       </x:c>
       <x:c r="B5">
-        <x:v>167.872203964681</x:v>
+        <x:v>11.9944848176066</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>67.705831149456</x:v>
+        <x:v>5.11998692765831</x:v>
       </x:c>
       <x:c r="D5">
-        <x:v>189.825522242964</x:v>
+        <x:v>25.8805357971604</x:v>
       </x:c>
       <x:c r="E5">
-        <x:v>4.8581971809539</x:v>
+        <x:v>160.020234324047</x:v>
       </x:c>
       <x:c r="F5">
-        <x:v>156.030717285364</x:v>
+        <x:v>131.233907645212</x:v>
       </x:c>
       <x:c r="G5">
-        <x:v>185.732766513588</x:v>
+        <x:v>143.220596640939</x:v>
       </x:c>
       <x:c r="H5">
-        <x:v>0.840889476631251</x:v>
+        <x:v>89.440680336878</x:v>
       </x:c>
       <x:c r="I5">
-        <x:v>93.1110724309045</x:v>
+        <x:v>58.8428589789396</x:v>
       </x:c>
       <x:c r="J5">
-        <x:v>108.154596438703</x:v>
+        <x:v>66.359319568779</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>130.914571942256</x:v>
+        <x:v>172.180705783973</x:v>
       </x:c>
       <x:c r="B6">
-        <x:v>76.1944373493057</x:v>
+        <x:v>175.792729191386</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>111.618736438276</x:v>
+        <x:v>27.6833604218826</x:v>
       </x:c>
       <x:c r="D6">
-        <x:v>198.115350491421</x:v>
+        <x:v>24.3489646466211</x:v>
       </x:c>
       <x:c r="E6">
-        <x:v>15.8046424462482</x:v>
+        <x:v>84.2274857145862</x:v>
       </x:c>
       <x:c r="F6">
-        <x:v>183.663435365848</x:v>
+        <x:v>25.7564349219931</x:v>
       </x:c>
       <x:c r="G6">
-        <x:v>84.451033866243</x:v>
+        <x:v>104.711813994083</x:v>
       </x:c>
       <x:c r="H6">
-        <x:v>151.785905171086</x:v>
+        <x:v>60.6527341812163</x:v>
       </x:c>
       <x:c r="I6">
-        <x:v>125.01973590116</x:v>
+        <x:v>34.3404179598859</x:v>
       </x:c>
       <x:c r="J6">
-        <x:v>188.590345433257</x:v>
+        <x:v>136.826371465263</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>140.983689176377</x:v>
+        <x:v>131.77205861163</x:v>
       </x:c>
       <x:c r="B7">
-        <x:v>42.4043857689967</x:v>
+        <x:v>107.891904985482</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>94.4493763588599</x:v>
+        <x:v>16.8595794666836</x:v>
       </x:c>
       <x:c r="D7">
-        <x:v>22.4827158369509</x:v>
+        <x:v>144.430698521636</x:v>
       </x:c>
       <x:c r="E7">
-        <x:v>76.3859715668419</x:v>
+        <x:v>169.240029141884</x:v>
       </x:c>
       <x:c r="F7">
-        <x:v>145.774164211831</x:v>
+        <x:v>26.1974745552044</x:v>
       </x:c>
       <x:c r="G7">
-        <x:v>171.430908595878</x:v>
+        <x:v>134.644280157352</x:v>
       </x:c>
       <x:c r="H7">
-        <x:v>179.188637425745</x:v>
+        <x:v>21.9671476734649</x:v>
       </x:c>
       <x:c r="I7">
-        <x:v>108.273351242893</x:v>
+        <x:v>182.150818864885</x:v>
       </x:c>
       <x:c r="J7">
-        <x:v>154.341317412602</x:v>
+        <x:v>198.337307385326</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>19.2646285608712</x:v>
+        <x:v>105.298095524916</x:v>
       </x:c>
       <x:c r="B8">
-        <x:v>102.248604177613</x:v>
+        <x:v>143.709244087203</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>60.1340208482621</x:v>
+        <x:v>27.5258776859966</x:v>
       </x:c>
       <x:c r="D8">
-        <x:v>186.781711032047</x:v>
+        <x:v>125.073027482756</x:v>
       </x:c>
       <x:c r="E8">
-        <x:v>0.980140362391314</x:v>
+        <x:v>7.18191638923339</x:v>
       </x:c>
       <x:c r="F8">
-        <x:v>93.2140350775859</x:v>
+        <x:v>54.2232956058454</x:v>
       </x:c>
       <x:c r="G8">
-        <x:v>91.0180958411741</x:v>
+        <x:v>2.06498662105994</x:v>
       </x:c>
       <x:c r="H8">
-        <x:v>20.288580199838</x:v>
+        <x:v>177.524367988819</x:v>
       </x:c>
       <x:c r="I8">
-        <x:v>18.3555924419107</x:v>
+        <x:v>168.178295236164</x:v>
       </x:c>
       <x:c r="J8">
-        <x:v>135.893130086313</x:v>
+        <x:v>43.7247852067113</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>160.733259916647</x:v>
+        <x:v>11.0678685880582</x:v>
       </x:c>
       <x:c r="B9">
-        <x:v>182.332125949828</x:v>
+        <x:v>135.667492605591</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>189.624378545966</x:v>
+        <x:v>44.9793504760504</x:v>
       </x:c>
       <x:c r="D9">
-        <x:v>6.59962380612251</x:v>
+        <x:v>66.1651248420426</x:v>
       </x:c>
       <x:c r="E9">
-        <x:v>47.6468946075285</x:v>
+        <x:v>136.804514255749</x:v>
       </x:c>
       <x:c r="F9">
-        <x:v>103.02055967181</x:v>
+        <x:v>19.3431169816028</x:v>
       </x:c>
       <x:c r="G9">
-        <x:v>134.458978909282</x:v>
+        <x:v>174.96621672761</x:v>
       </x:c>
       <x:c r="H9">
-        <x:v>72.8796040047331</x:v>
+        <x:v>181.446327912363</x:v>
       </x:c>
       <x:c r="I9">
-        <x:v>187.404023011869</x:v>
+        <x:v>18.0835004048811</x:v>
       </x:c>
       <x:c r="J9">
-        <x:v>121.779106614077</x:v>
+        <x:v>192.375652488496</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>87.2683938999048</x:v>
+        <x:v>9.69472099547029</x:v>
       </x:c>
       <x:c r="B10">
-        <x:v>40.2419575677449</x:v>
+        <x:v>120.987921543879</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>4.97699752681749</x:v>
+        <x:v>172.797402261196</x:v>
       </x:c>
       <x:c r="D10">
-        <x:v>156.535768488672</x:v>
+        <x:v>15.2236961830518</x:v>
       </x:c>
       <x:c r="E10">
-        <x:v>96.359423965383</x:v>
+        <x:v>50.3149624216906</x:v>
       </x:c>
       <x:c r="F10">
-        <x:v>195.31617136454</x:v>
+        <x:v>75.4714345910919</x:v>
       </x:c>
       <x:c r="G10">
-        <x:v>73.4228276058207</x:v>
+        <x:v>195.134905350923</x:v>
       </x:c>
       <x:c r="H10">
-        <x:v>45.2231153125051</x:v>
+        <x:v>60.6892884060225</x:v>
       </x:c>
       <x:c r="I10">
-        <x:v>113.439550676122</x:v>
+        <x:v>56.6405066552761</x:v>
       </x:c>
       <x:c r="J10">
-        <x:v>59.0840329691228</x:v>
+        <x:v>133.822759768843</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>184.599808689486</x:v>
+        <x:v>196.58962748786</x:v>
       </x:c>
       <x:c r="B11">
-        <x:v>6.54412908784306</x:v>
+        <x:v>121.253448967474</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>92.5675382337382</x:v>
+        <x:v>107.289861471993</x:v>
       </x:c>
       <x:c r="D11">
-        <x:v>138.769755018302</x:v>
+        <x:v>60.5055515936136</x:v>
       </x:c>
       <x:c r="E11">
-        <x:v>88.8899678778322</x:v>
+        <x:v>161.061224043863</x:v>
       </x:c>
       <x:c r="F11">
-        <x:v>28.665967764643</x:v>
+        <x:v>28.4714616967698</x:v>
       </x:c>
       <x:c r="G11">
-        <x:v>16.0604165010436</x:v>
+        <x:v>148.266851505389</x:v>
       </x:c>
       <x:c r="H11">
-        <x:v>124.837025406229</x:v>
+        <x:v>102.610332939127</x:v>
       </x:c>
       <x:c r="I11">
-        <x:v>197.13521012903</x:v>
+        <x:v>17.1670482573877</x:v>
       </x:c>
       <x:c r="J11">
-        <x:v>122.590607368662</x:v>
+        <x:v>30.0041901087408</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
       <x:c r="A12">
-        <x:v>92.6453395246739</x:v>
+        <x:v>23.6914483009332</x:v>
       </x:c>
       <x:c r="B12">
-        <x:v>64.162453666405</x:v>
+        <x:v>127.187446005264</x:v>
       </x:c>
       <x:c r="C12">
-        <x:v>133.430312729175</x:v>
+        <x:v>92.4744389450524</x:v>
       </x:c>
       <x:c r="D12">
-        <x:v>189.126605814847</x:v>
+        <x:v>190.615632753175</x:v>
       </x:c>
       <x:c r="E12">
-        <x:v>27.8570855166098</x:v>
+        <x:v>125.758502877205</x:v>
       </x:c>
       <x:c r="F12">
-        <x:v>158.651563226549</x:v>
+        <x:v>196.104566006039</x:v>
       </x:c>
       <x:c r="G12">
-        <x:v>52.7800072230306</x:v>
+        <x:v>62.9125545094314</x:v>
       </x:c>
       <x:c r="H12">
-        <x:v>87.8497525527374</x:v>
+        <x:v>150.694454624641</x:v>
       </x:c>
       <x:c r="I12">
-        <x:v>174.835821229422</x:v>
+        <x:v>7.62618426588652</x:v>
       </x:c>
       <x:c r="J12">
-        <x:v>173.365411895032</x:v>
+        <x:v>149.896912160282</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="A13">
-        <x:v>11.3151853025496</x:v>
+        <x:v>51.2312578275945</x:v>
       </x:c>
       <x:c r="B13">
-        <x:v>98.551304591145</x:v>
+        <x:v>153.197952244989</x:v>
       </x:c>
       <x:c r="C13">
-        <x:v>191.784614413876</x:v>
+        <x:v>3.88364726858383</x:v>
       </x:c>
       <x:c r="D13">
-        <x:v>186.494244628816</x:v>
+        <x:v>189.775166376389</x:v>
       </x:c>
       <x:c r="E13">
-        <x:v>67.0729235126976</x:v>
+        <x:v>188.642586389856</x:v>
       </x:c>
       <x:c r="F13">
-        <x:v>179.022670993126</x:v>
+        <x:v>184.310173981036</x:v>
       </x:c>
       <x:c r="G13">
-        <x:v>97.2716066507956</x:v>
+        <x:v>170.911841826007</x:v>
       </x:c>
       <x:c r="H13">
-        <x:v>103.598252359591</x:v>
+        <x:v>12.3021815029449</x:v>
       </x:c>
       <x:c r="I13">
-        <x:v>90.4222870666638</x:v>
+        <x:v>74.7580650610654</x:v>
       </x:c>
       <x:c r="J13">
-        <x:v>5.663968997851</x:v>
+        <x:v>131.710481798142</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="A14">
-        <x:v>19.7912074717652</x:v>
+        <x:v>59.0883902549224</x:v>
       </x:c>
       <x:c r="B14">
-        <x:v>45.794980528669</x:v>
+        <x:v>141.375698215037</x:v>
       </x:c>
       <x:c r="C14">
-        <x:v>106.849029523716</x:v>
+        <x:v>120.883861333543</x:v>
       </x:c>
       <x:c r="D14">
-        <x:v>159.271559472788</x:v>
+        <x:v>34.3555354673208</x:v>
       </x:c>
       <x:c r="E14">
-        <x:v>151.293321396826</x:v>
+        <x:v>47.1351577188518</x:v>
       </x:c>
       <x:c r="F14">
-        <x:v>154.189130828804</x:v>
+        <x:v>89.814419620584</x:v>
       </x:c>
       <x:c r="G14">
-        <x:v>89.7645877160898</x:v>
+        <x:v>28.3776311335981</x:v>
       </x:c>
       <x:c r="H14">
-        <x:v>50.8546235276641</x:v>
+        <x:v>184.473798882437</x:v>
       </x:c>
       <x:c r="I14">
-        <x:v>117.70965592829</x:v>
+        <x:v>105.103900798179</x:v>
       </x:c>
       <x:c r="J14">
-        <x:v>18.9809268428855</x:v>
+        <x:v>108.33305255898</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="A15">
-        <x:v>86.9601431707666</x:v>
+        <x:v>71.0762654762139</x:v>
       </x:c>
       <x:c r="B15">
-        <x:v>9.62195350305268</x:v>
+        <x:v>72.3558837884832</x:v>
       </x:c>
       <x:c r="C15">
-        <x:v>75.7443938757034</x:v>
+        <x:v>164.279279654976</x:v>
       </x:c>
       <x:c r="D15">
-        <x:v>64.8134156432065</x:v>
+        <x:v>188.07931029614</x:v>
       </x:c>
       <x:c r="E15">
-        <x:v>29.1337670894031</x:v>
+        <x:v>168.684204187563</x:v>
       </x:c>
       <x:c r="F15">
-        <x:v>23.1059402334997</x:v>
+        <x:v>82.5072749902062</x:v>
       </x:c>
       <x:c r="G15">
-        <x:v>106.81164483857</x:v>
+        <x:v>28.513482598827</x:v>
       </x:c>
       <x:c r="H15">
-        <x:v>15.85039171197</x:v>
+        <x:v>182.181769508022</x:v>
       </x:c>
       <x:c r="I15">
-        <x:v>128.678682972062</x:v>
+        <x:v>89.4651933058469</x:v>
       </x:c>
       <x:c r="J15">
-        <x:v>137.707860738834</x:v>
+        <x:v>54.210396415652</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="A16">
-        <x:v>142.53616414151</x:v>
+        <x:v>12.5588800816605</x:v>
       </x:c>
       <x:c r="B16">
-        <x:v>185.573075053083</x:v>
+        <x:v>44.4404507262821</x:v>
       </x:c>
       <x:c r="C16">
-        <x:v>70.3872940830827</x:v>
+        <x:v>53.063104140136</x:v>
       </x:c>
       <x:c r="D16">
-        <x:v>140.07413878109</x:v>
+        <x:v>106.743594494995</x:v>
       </x:c>
       <x:c r="E16">
-        <x:v>47.7688476665732</x:v>
+        <x:v>82.5915019412486</x:v>
       </x:c>
       <x:c r="F16">
-        <x:v>86.0485040983411</x:v>
+        <x:v>43.3916752428709</x:v>
       </x:c>
       <x:c r="G16">
-        <x:v>14.7595146739667</x:v>
+        <x:v>117.36980169889</x:v>
       </x:c>
       <x:c r="H16">
-        <x:v>106.073293604922</x:v>
+        <x:v>117.514695095604</x:v>
       </x:c>
       <x:c r="I16">
-        <x:v>71.6968315056045</x:v>
+        <x:v>71.8629652037578</x:v>
       </x:c>
       <x:c r="J16">
-        <x:v>109.867296884706</x:v>
+        <x:v>176.751050062827</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="A17">
-        <x:v>131.394361113847</x:v>
+        <x:v>57.5596198707631</x:v>
       </x:c>
       <x:c r="B17">
-        <x:v>112.462164141453</x:v>
+        <x:v>135.964670002444</x:v>
       </x:c>
       <x:c r="C17">
-        <x:v>34.4147383395651</x:v>
+        <x:v>27.8522678780613</x:v>
       </x:c>
       <x:c r="D17">
-        <x:v>191.471241131179</x:v>
+        <x:v>85.4565664592462</x:v>
       </x:c>
       <x:c r="E17">
-        <x:v>102.799399896897</x:v>
+        <x:v>170.915799853818</x:v>
       </x:c>
       <x:c r="F17">
-        <x:v>46.850358996005</x:v>
+        <x:v>82.3157500858958</x:v>
       </x:c>
       <x:c r="G17">
-        <x:v>157.313424142689</x:v>
+        <x:v>6.30358467172067</x:v>
       </x:c>
       <x:c r="H17">
-        <x:v>174.158753256387</x:v>
+        <x:v>58.1189034777316</x:v>
       </x:c>
       <x:c r="I17">
-        <x:v>37.833284418021</x:v>
+        <x:v>143.480475034323</x:v>
       </x:c>
       <x:c r="J17">
-        <x:v>73.6679546878058</x:v>
+        <x:v>35.9440832566209</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="A18">
-        <x:v>68.8869755104589</x:v>
+        <x:v>167.72693487244</x:v>
       </x:c>
       <x:c r="B18">
-        <x:v>1.92538369536651</x:v>
+        <x:v>78.4387556269945</x:v>
       </x:c>
       <x:c r="C18">
-        <x:v>170.140096624447</x:v>
+        <x:v>45.5905538264618</x:v>
       </x:c>
       <x:c r="D18">
-        <x:v>155.854894386537</x:v>
+        <x:v>99.293131706907</x:v>
       </x:c>
       <x:c r="E18">
-        <x:v>86.4052687242652</x:v>
+        <x:v>78.8206466840676</x:v>
       </x:c>
       <x:c r="F18">
-        <x:v>1.69323179949691</x:v>
+        <x:v>178.875374039111</x:v>
       </x:c>
       <x:c r="G18">
-        <x:v>22.8069107154416</x:v>
+        <x:v>188.918672590013</x:v>
       </x:c>
       <x:c r="H18">
-        <x:v>126.97119877067</x:v>
+        <x:v>15.8043369724435</x:v>
       </x:c>
       <x:c r="I18">
-        <x:v>157.360477539413</x:v>
+        <x:v>21.0909621888264</x:v>
       </x:c>
       <x:c r="J18">
-        <x:v>43.9669832791979</x:v>
+        <x:v>106.13531139965</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="A19">
-        <x:v>72.2110261545568</x:v>
+        <x:v>155.796691382209</x:v>
       </x:c>
       <x:c r="B19">
-        <x:v>81.4212149388256</x:v>
+        <x:v>188.730072317985</x:v>
       </x:c>
       <x:c r="C19">
-        <x:v>174.919569387529</x:v>
+        <x:v>122.836988197098</x:v>
       </x:c>
       <x:c r="D19">
-        <x:v>152.714426327829</x:v>
+        <x:v>20.5476686454134</x:v>
       </x:c>
       <x:c r="E19">
-        <x:v>63.1278048563412</x:v>
+        <x:v>119.151601716481</x:v>
       </x:c>
       <x:c r="F19">
-        <x:v>34.2181324186819</x:v>
+        <x:v>14.6479395286403</x:v>
       </x:c>
       <x:c r="G19">
-        <x:v>175.407686445586</x:v>
+        <x:v>88.3125940749015</x:v>
       </x:c>
       <x:c r="H19">
-        <x:v>166.774890742626</x:v>
+        <x:v>14.1402668385488</x:v>
       </x:c>
       <x:c r="I19">
-        <x:v>111.502711806215</x:v>
+        <x:v>151.764033526072</x:v>
       </x:c>
       <x:c r="J19">
-        <x:v>65.2448172984853</x:v>
+        <x:v>3.74348247598088</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
       <x:c r="A20">
-        <x:v>139.429616154837</x:v>
+        <x:v>172.444617921694</x:v>
       </x:c>
       <x:c r="B20">
-        <x:v>183.691294111168</x:v>
+        <x:v>110.862936037994</x:v>
       </x:c>
       <x:c r="C20">
-        <x:v>179.15779202206</x:v>
+        <x:v>112.610833678679</x:v>
       </x:c>
       <x:c r="D20">
-        <x:v>7.84235904358437</x:v>
+        <x:v>128.352850735352</x:v>
       </x:c>
       <x:c r="E20">
-        <x:v>87.5865657290381</x:v>
+        <x:v>50.7734326882164</x:v>
       </x:c>
       <x:c r="F20">
-        <x:v>174.497979029314</x:v>
+        <x:v>135.11159547377</x:v>
       </x:c>
       <x:c r="G20">
-        <x:v>175.207215163488</x:v>
+        <x:v>44.5036159104219</x:v>
       </x:c>
       <x:c r="H20">
-        <x:v>84.2731527445247</x:v>
+        <x:v>78.8227131957294</x:v>
       </x:c>
       <x:c r="I20">
-        <x:v>162.014015746309</x:v>
+        <x:v>17.1635104423219</x:v>
       </x:c>
       <x:c r="J20">
-        <x:v>182.283408093398</x:v>
+        <x:v>86.368454101667</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Da finire la visualizzazione il data binding
</commit_message>
<xml_diff>
--- a/windows_form_app/ConditionalFormatColorScale.xlsx
+++ b/windows_form_app/ConditionalFormatColorScale.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R89ec1bc19f854cbe"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R3205782c566045ee"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -345,642 +345,642 @@
   <x:sheetData>
     <x:row r="1">
       <x:c r="A1">
-        <x:v>32.9414084707114</x:v>
+        <x:v>160.334686357684</x:v>
       </x:c>
       <x:c r="B1">
-        <x:v>108.116717780063</x:v>
+        <x:v>20.6578374005192</x:v>
       </x:c>
       <x:c r="C1">
-        <x:v>188.851263741428</x:v>
+        <x:v>125.304815138366</x:v>
       </x:c>
       <x:c r="D1">
-        <x:v>9.29911081180866</x:v>
+        <x:v>7.42962435233855</x:v>
       </x:c>
       <x:c r="E1">
-        <x:v>91.1148366942605</x:v>
+        <x:v>141.576353060816</x:v>
       </x:c>
       <x:c r="F1">
-        <x:v>156.880231554099</x:v>
+        <x:v>72.0289083533124</x:v>
       </x:c>
       <x:c r="G1">
-        <x:v>11.7141144404719</x:v>
+        <x:v>99.7806833590291</x:v>
       </x:c>
       <x:c r="H1">
-        <x:v>149.384023877505</x:v>
+        <x:v>10.6914648835973</x:v>
       </x:c>
       <x:c r="I1">
-        <x:v>53.415918561358</x:v>
+        <x:v>29.0826002271299</x:v>
       </x:c>
       <x:c r="J1">
-        <x:v>164.375875314873</x:v>
+        <x:v>186.48344063502</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>28.8470517046969</x:v>
+        <x:v>49.5330577015565</x:v>
       </x:c>
       <x:c r="B2">
-        <x:v>140.439572716337</x:v>
+        <x:v>21.2742932239893</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>124.278133792932</x:v>
+        <x:v>42.4062806379079</x:v>
       </x:c>
       <x:c r="D2">
-        <x:v>0.282906275374306</x:v>
+        <x:v>39.5965671351164</x:v>
       </x:c>
       <x:c r="E2">
-        <x:v>112.74384237488</x:v>
+        <x:v>103.93235157427</x:v>
       </x:c>
       <x:c r="F2">
-        <x:v>86.9387512500113</x:v>
+        <x:v>139.959372458961</x:v>
       </x:c>
       <x:c r="G2">
-        <x:v>150.847064308285</x:v>
+        <x:v>137.812589638779</x:v>
       </x:c>
       <x:c r="H2">
-        <x:v>179.575945334312</x:v>
+        <x:v>6.90119434469435</x:v>
       </x:c>
       <x:c r="I2">
-        <x:v>107.160048516076</x:v>
+        <x:v>139.518385166078</x:v>
       </x:c>
       <x:c r="J2">
-        <x:v>190.545255965807</x:v>
+        <x:v>165.918658844157</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>66.217780423452</x:v>
+        <x:v>180.165873831215</x:v>
       </x:c>
       <x:c r="B3">
-        <x:v>7.18497354871825</x:v>
+        <x:v>131.93953006153</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>3.4049037859798</x:v>
+        <x:v>186.906220757824</x:v>
       </x:c>
       <x:c r="D3">
-        <x:v>128.198529560211</x:v>
+        <x:v>58.8757023489455</x:v>
       </x:c>
       <x:c r="E3">
-        <x:v>174.958692851923</x:v>
+        <x:v>62.2783218800455</x:v>
       </x:c>
       <x:c r="F3">
-        <x:v>154.288465228997</x:v>
+        <x:v>128.016692087062</x:v>
       </x:c>
       <x:c r="G3">
-        <x:v>25.108172942469</x:v>
+        <x:v>149.201590264776</x:v>
       </x:c>
       <x:c r="H3">
-        <x:v>103.82220945499</x:v>
+        <x:v>45.5876905683371</x:v>
       </x:c>
       <x:c r="I3">
-        <x:v>132.524444410822</x:v>
+        <x:v>118.602181653773</x:v>
       </x:c>
       <x:c r="J3">
-        <x:v>108.985220039722</x:v>
+        <x:v>62.258485454255</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>195.135846172988</x:v>
+        <x:v>35.4854357594091</x:v>
       </x:c>
       <x:c r="B4">
-        <x:v>2.64957714949249</x:v>
+        <x:v>101.26448846481</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>5.7952925589845</x:v>
+        <x:v>47.5028627773295</x:v>
       </x:c>
       <x:c r="D4">
-        <x:v>102.310986119467</x:v>
+        <x:v>92.8036313004809</x:v>
       </x:c>
       <x:c r="E4">
-        <x:v>18.1320874104891</x:v>
+        <x:v>0.8067236285688</x:v>
       </x:c>
       <x:c r="F4">
-        <x:v>114.406534989554</x:v>
+        <x:v>101.407469763145</x:v>
       </x:c>
       <x:c r="G4">
-        <x:v>181.640655725096</x:v>
+        <x:v>74.5363784369716</x:v>
       </x:c>
       <x:c r="H4">
-        <x:v>7.13782022108222</x:v>
+        <x:v>181.77221239627</x:v>
       </x:c>
       <x:c r="I4">
-        <x:v>152.050067648315</x:v>
+        <x:v>191.688250653301</x:v>
       </x:c>
       <x:c r="J4">
-        <x:v>182.08702103332</x:v>
+        <x:v>90.7576557671454</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5">
-        <x:v>183.363339576574</x:v>
+        <x:v>94.9912441405427</x:v>
       </x:c>
       <x:c r="B5">
-        <x:v>11.9944848176066</x:v>
+        <x:v>3.69410598822595</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>5.11998692765831</x:v>
+        <x:v>4.29676138064673</x:v>
       </x:c>
       <x:c r="D5">
-        <x:v>25.8805357971604</x:v>
+        <x:v>190.969530209419</x:v>
       </x:c>
       <x:c r="E5">
-        <x:v>160.020234324047</x:v>
+        <x:v>126.354855823496</x:v>
       </x:c>
       <x:c r="F5">
-        <x:v>131.233907645212</x:v>
+        <x:v>29.8405539383369</x:v>
       </x:c>
       <x:c r="G5">
-        <x:v>143.220596640939</x:v>
+        <x:v>101.439659065306</x:v>
       </x:c>
       <x:c r="H5">
-        <x:v>89.440680336878</x:v>
+        <x:v>116.551897729073</x:v>
       </x:c>
       <x:c r="I5">
-        <x:v>58.8428589789396</x:v>
+        <x:v>105.142685726817</x:v>
       </x:c>
       <x:c r="J5">
-        <x:v>66.359319568779</x:v>
+        <x:v>199.370667151814</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>172.180705783973</x:v>
+        <x:v>44.2154777442177</x:v>
       </x:c>
       <x:c r="B6">
-        <x:v>175.792729191386</x:v>
+        <x:v>160.873748250713</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>27.6833604218826</x:v>
+        <x:v>112.889927585092</x:v>
       </x:c>
       <x:c r="D6">
-        <x:v>24.3489646466211</x:v>
+        <x:v>124.503278231483</x:v>
       </x:c>
       <x:c r="E6">
-        <x:v>84.2274857145862</x:v>
+        <x:v>163.190609478946</x:v>
       </x:c>
       <x:c r="F6">
-        <x:v>25.7564349219931</x:v>
+        <x:v>28.3951562961541</x:v>
       </x:c>
       <x:c r="G6">
-        <x:v>104.711813994083</x:v>
+        <x:v>33.7516166426947</x:v>
       </x:c>
       <x:c r="H6">
-        <x:v>60.6527341812163</x:v>
+        <x:v>66.4291127894209</x:v>
       </x:c>
       <x:c r="I6">
-        <x:v>34.3404179598859</x:v>
+        <x:v>145.151302472293</x:v>
       </x:c>
       <x:c r="J6">
-        <x:v>136.826371465263</x:v>
+        <x:v>13.5596609737536</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>131.77205861163</x:v>
+        <x:v>122.827318088537</x:v>
       </x:c>
       <x:c r="B7">
-        <x:v>107.891904985482</x:v>
+        <x:v>54.192992790692</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>16.8595794666836</x:v>
+        <x:v>92.0892832298247</x:v>
       </x:c>
       <x:c r="D7">
-        <x:v>144.430698521636</x:v>
+        <x:v>166.824114772875</x:v>
       </x:c>
       <x:c r="E7">
-        <x:v>169.240029141884</x:v>
+        <x:v>150.998004875611</x:v>
       </x:c>
       <x:c r="F7">
-        <x:v>26.1974745552044</x:v>
+        <x:v>148.268569236746</x:v>
       </x:c>
       <x:c r="G7">
-        <x:v>134.644280157352</x:v>
+        <x:v>173.77143044666</x:v>
       </x:c>
       <x:c r="H7">
-        <x:v>21.9671476734649</x:v>
+        <x:v>149.602649337427</x:v>
       </x:c>
       <x:c r="I7">
-        <x:v>182.150818864885</x:v>
+        <x:v>38.7898435065475</x:v>
       </x:c>
       <x:c r="J7">
-        <x:v>198.337307385326</x:v>
+        <x:v>2.52488181112561</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>105.298095524916</x:v>
+        <x:v>65.4229940219889</x:v>
       </x:c>
       <x:c r="B8">
-        <x:v>143.709244087203</x:v>
+        <x:v>156.040377242509</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>27.5258776859966</x:v>
+        <x:v>15.2129436913938</x:v>
       </x:c>
       <x:c r="D8">
-        <x:v>125.073027482756</x:v>
+        <x:v>48.7607293989326</x:v>
       </x:c>
       <x:c r="E8">
-        <x:v>7.18191638923339</x:v>
+        <x:v>70.9274147036147</x:v>
       </x:c>
       <x:c r="F8">
-        <x:v>54.2232956058454</x:v>
+        <x:v>176.471767842989</x:v>
       </x:c>
       <x:c r="G8">
-        <x:v>2.06498662105994</x:v>
+        <x:v>127.642768680883</x:v>
       </x:c>
       <x:c r="H8">
-        <x:v>177.524367988819</x:v>
+        <x:v>195.936690548405</x:v>
       </x:c>
       <x:c r="I8">
-        <x:v>168.178295236164</x:v>
+        <x:v>132.52084652545</x:v>
       </x:c>
       <x:c r="J8">
-        <x:v>43.7247852067113</x:v>
+        <x:v>32.4377679417086</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>11.0678685880582</x:v>
+        <x:v>26.577033021756</x:v>
       </x:c>
       <x:c r="B9">
-        <x:v>135.667492605591</x:v>
+        <x:v>32.6496925357029</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>44.9793504760504</x:v>
+        <x:v>140.44500484152</x:v>
       </x:c>
       <x:c r="D9">
-        <x:v>66.1651248420426</x:v>
+        <x:v>119.231514501959</x:v>
       </x:c>
       <x:c r="E9">
-        <x:v>136.804514255749</x:v>
+        <x:v>18.0430077100373</x:v>
       </x:c>
       <x:c r="F9">
-        <x:v>19.3431169816028</x:v>
+        <x:v>74.6116875086965</x:v>
       </x:c>
       <x:c r="G9">
-        <x:v>174.96621672761</x:v>
+        <x:v>188.374560879718</x:v>
       </x:c>
       <x:c r="H9">
-        <x:v>181.446327912363</x:v>
+        <x:v>122.999584545847</x:v>
       </x:c>
       <x:c r="I9">
-        <x:v>18.0835004048811</x:v>
+        <x:v>129.613021821535</x:v>
       </x:c>
       <x:c r="J9">
-        <x:v>192.375652488496</x:v>
+        <x:v>172.411567332415</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>9.69472099547029</x:v>
+        <x:v>67.6558531204499</x:v>
       </x:c>
       <x:c r="B10">
-        <x:v>120.987921543879</x:v>
+        <x:v>8.1072656475507</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>172.797402261196</x:v>
+        <x:v>36.6209099239767</x:v>
       </x:c>
       <x:c r="D10">
-        <x:v>15.2236961830518</x:v>
+        <x:v>178.128589679547</x:v>
       </x:c>
       <x:c r="E10">
-        <x:v>50.3149624216906</x:v>
+        <x:v>167.930337678609</x:v>
       </x:c>
       <x:c r="F10">
-        <x:v>75.4714345910919</x:v>
+        <x:v>40.7982513498507</x:v>
       </x:c>
       <x:c r="G10">
-        <x:v>195.134905350923</x:v>
+        <x:v>111.604822758401</x:v>
       </x:c>
       <x:c r="H10">
-        <x:v>60.6892884060225</x:v>
+        <x:v>37.4726466077718</x:v>
       </x:c>
       <x:c r="I10">
-        <x:v>56.6405066552761</x:v>
+        <x:v>39.9715253338085</x:v>
       </x:c>
       <x:c r="J10">
-        <x:v>133.822759768843</x:v>
+        <x:v>178.08628658675</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>196.58962748786</x:v>
+        <x:v>56.069123491677</x:v>
       </x:c>
       <x:c r="B11">
-        <x:v>121.253448967474</x:v>
+        <x:v>151.837009727879</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>107.289861471993</x:v>
+        <x:v>77.7620542225251</x:v>
       </x:c>
       <x:c r="D11">
-        <x:v>60.5055515936136</x:v>
+        <x:v>102.617803915691</x:v>
       </x:c>
       <x:c r="E11">
-        <x:v>161.061224043863</x:v>
+        <x:v>133.947673129825</x:v>
       </x:c>
       <x:c r="F11">
-        <x:v>28.4714616967698</x:v>
+        <x:v>88.1751005017083</x:v>
       </x:c>
       <x:c r="G11">
-        <x:v>148.266851505389</x:v>
+        <x:v>145.660804559319</x:v>
       </x:c>
       <x:c r="H11">
-        <x:v>102.610332939127</x:v>
+        <x:v>64.1291981861597</x:v>
       </x:c>
       <x:c r="I11">
-        <x:v>17.1670482573877</x:v>
+        <x:v>53.5758635278679</x:v>
       </x:c>
       <x:c r="J11">
-        <x:v>30.0041901087408</x:v>
+        <x:v>186.718841635957</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
       <x:c r="A12">
-        <x:v>23.6914483009332</x:v>
+        <x:v>100.752387615271</x:v>
       </x:c>
       <x:c r="B12">
-        <x:v>127.187446005264</x:v>
+        <x:v>37.8149260942894</x:v>
       </x:c>
       <x:c r="C12">
-        <x:v>92.4744389450524</x:v>
+        <x:v>133.908266263971</x:v>
       </x:c>
       <x:c r="D12">
-        <x:v>190.615632753175</x:v>
+        <x:v>112.713534530584</x:v>
       </x:c>
       <x:c r="E12">
-        <x:v>125.758502877205</x:v>
+        <x:v>186.982627951998</x:v>
       </x:c>
       <x:c r="F12">
-        <x:v>196.104566006039</x:v>
+        <x:v>90.1776255528338</x:v>
       </x:c>
       <x:c r="G12">
-        <x:v>62.9125545094314</x:v>
+        <x:v>113.747987949172</x:v>
       </x:c>
       <x:c r="H12">
-        <x:v>150.694454624641</x:v>
+        <x:v>172.857768727866</x:v>
       </x:c>
       <x:c r="I12">
-        <x:v>7.62618426588652</x:v>
+        <x:v>148.781107062838</x:v>
       </x:c>
       <x:c r="J12">
-        <x:v>149.896912160282</x:v>
+        <x:v>76.386317366914</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="A13">
-        <x:v>51.2312578275945</x:v>
+        <x:v>159.894008357028</x:v>
       </x:c>
       <x:c r="B13">
-        <x:v>153.197952244989</x:v>
+        <x:v>50.771845900813</x:v>
       </x:c>
       <x:c r="C13">
-        <x:v>3.88364726858383</x:v>
+        <x:v>19.9896275158923</x:v>
       </x:c>
       <x:c r="D13">
-        <x:v>189.775166376389</x:v>
+        <x:v>66.3782761741329</x:v>
       </x:c>
       <x:c r="E13">
-        <x:v>188.642586389856</x:v>
+        <x:v>134.869028690676</x:v>
       </x:c>
       <x:c r="F13">
-        <x:v>184.310173981036</x:v>
+        <x:v>57.3157283744382</x:v>
       </x:c>
       <x:c r="G13">
-        <x:v>170.911841826007</x:v>
+        <x:v>119.419467318533</x:v>
       </x:c>
       <x:c r="H13">
-        <x:v>12.3021815029449</x:v>
+        <x:v>37.0843540118469</x:v>
       </x:c>
       <x:c r="I13">
-        <x:v>74.7580650610654</x:v>
+        <x:v>80.830391720324</x:v>
       </x:c>
       <x:c r="J13">
-        <x:v>131.710481798142</x:v>
+        <x:v>30.1291633537641</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="A14">
-        <x:v>59.0883902549224</x:v>
+        <x:v>64.8669450845881</x:v>
       </x:c>
       <x:c r="B14">
-        <x:v>141.375698215037</x:v>
+        <x:v>90.1701220731112</x:v>
       </x:c>
       <x:c r="C14">
-        <x:v>120.883861333543</x:v>
+        <x:v>155.965165214597</x:v>
       </x:c>
       <x:c r="D14">
-        <x:v>34.3555354673208</x:v>
+        <x:v>154.4345599387</x:v>
       </x:c>
       <x:c r="E14">
-        <x:v>47.1351577188518</x:v>
+        <x:v>176.368644450032</x:v>
       </x:c>
       <x:c r="F14">
-        <x:v>89.814419620584</x:v>
+        <x:v>74.740023293877</x:v>
       </x:c>
       <x:c r="G14">
-        <x:v>28.3776311335981</x:v>
+        <x:v>154.887638313178</x:v>
       </x:c>
       <x:c r="H14">
-        <x:v>184.473798882437</x:v>
+        <x:v>37.8272009258285</x:v>
       </x:c>
       <x:c r="I14">
-        <x:v>105.103900798179</x:v>
+        <x:v>185.283841372134</x:v>
       </x:c>
       <x:c r="J14">
-        <x:v>108.33305255898</x:v>
+        <x:v>129.867907208329</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="A15">
-        <x:v>71.0762654762139</x:v>
+        <x:v>128.950882949378</x:v>
       </x:c>
       <x:c r="B15">
-        <x:v>72.3558837884832</x:v>
+        <x:v>124.245362693558</x:v>
       </x:c>
       <x:c r="C15">
-        <x:v>164.279279654976</x:v>
+        <x:v>69.423721017979</x:v>
       </x:c>
       <x:c r="D15">
-        <x:v>188.07931029614</x:v>
+        <x:v>142.894180185578</x:v>
       </x:c>
       <x:c r="E15">
-        <x:v>168.684204187563</x:v>
+        <x:v>71.6591797171436</x:v>
       </x:c>
       <x:c r="F15">
-        <x:v>82.5072749902062</x:v>
+        <x:v>29.8409270261605</x:v>
       </x:c>
       <x:c r="G15">
-        <x:v>28.513482598827</x:v>
+        <x:v>74.1989993835795</x:v>
       </x:c>
       <x:c r="H15">
-        <x:v>182.181769508022</x:v>
+        <x:v>123.907375393392</x:v>
       </x:c>
       <x:c r="I15">
-        <x:v>89.4651933058469</x:v>
+        <x:v>191.145961727549</x:v>
       </x:c>
       <x:c r="J15">
-        <x:v>54.210396415652</x:v>
+        <x:v>77.7527121257748</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="A16">
-        <x:v>12.5588800816605</x:v>
+        <x:v>127.050263400679</x:v>
       </x:c>
       <x:c r="B16">
-        <x:v>44.4404507262821</x:v>
+        <x:v>138.747054030535</x:v>
       </x:c>
       <x:c r="C16">
-        <x:v>53.063104140136</x:v>
+        <x:v>88.6915395449342</x:v>
       </x:c>
       <x:c r="D16">
-        <x:v>106.743594494995</x:v>
+        <x:v>163.585207966894</x:v>
       </x:c>
       <x:c r="E16">
-        <x:v>82.5915019412486</x:v>
+        <x:v>18.192278229721</x:v>
       </x:c>
       <x:c r="F16">
-        <x:v>43.3916752428709</x:v>
+        <x:v>5.297277590864</x:v>
       </x:c>
       <x:c r="G16">
-        <x:v>117.36980169889</x:v>
+        <x:v>131.847382211987</x:v>
       </x:c>
       <x:c r="H16">
-        <x:v>117.514695095604</x:v>
+        <x:v>11.3837780483923</x:v>
       </x:c>
       <x:c r="I16">
-        <x:v>71.8629652037578</x:v>
+        <x:v>167.748775225016</x:v>
       </x:c>
       <x:c r="J16">
-        <x:v>176.751050062827</x:v>
+        <x:v>76.6319447553865</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="A17">
-        <x:v>57.5596198707631</x:v>
+        <x:v>168.755633183176</x:v>
       </x:c>
       <x:c r="B17">
-        <x:v>135.964670002444</x:v>
+        <x:v>108.576450547472</x:v>
       </x:c>
       <x:c r="C17">
-        <x:v>27.8522678780613</x:v>
+        <x:v>183.298806465836</x:v>
       </x:c>
       <x:c r="D17">
-        <x:v>85.4565664592462</x:v>
+        <x:v>23.4467001741038</x:v>
       </x:c>
       <x:c r="E17">
-        <x:v>170.915799853818</x:v>
+        <x:v>121.851896551369</x:v>
       </x:c>
       <x:c r="F17">
-        <x:v>82.3157500858958</x:v>
+        <x:v>10.5822655421599</x:v>
       </x:c>
       <x:c r="G17">
-        <x:v>6.30358467172067</x:v>
+        <x:v>81.8497608796925</x:v>
       </x:c>
       <x:c r="H17">
-        <x:v>58.1189034777316</x:v>
+        <x:v>179.473706325271</x:v>
       </x:c>
       <x:c r="I17">
-        <x:v>143.480475034323</x:v>
+        <x:v>136.344890080553</x:v>
       </x:c>
       <x:c r="J17">
-        <x:v>35.9440832566209</x:v>
+        <x:v>112.242604658121</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="A18">
-        <x:v>167.72693487244</x:v>
+        <x:v>135.289987239656</x:v>
       </x:c>
       <x:c r="B18">
-        <x:v>78.4387556269945</x:v>
+        <x:v>75.9207870233435</x:v>
       </x:c>
       <x:c r="C18">
-        <x:v>45.5905538264618</x:v>
+        <x:v>187.573927355732</x:v>
       </x:c>
       <x:c r="D18">
-        <x:v>99.293131706907</x:v>
+        <x:v>18.9131998545086</x:v>
       </x:c>
       <x:c r="E18">
-        <x:v>78.8206466840676</x:v>
+        <x:v>147.435434417536</x:v>
       </x:c>
       <x:c r="F18">
-        <x:v>178.875374039111</x:v>
+        <x:v>35.6486456634703</x:v>
       </x:c>
       <x:c r="G18">
-        <x:v>188.918672590013</x:v>
+        <x:v>181.348124882834</x:v>
       </x:c>
       <x:c r="H18">
-        <x:v>15.8043369724435</x:v>
+        <x:v>77.0954473303144</x:v>
       </x:c>
       <x:c r="I18">
-        <x:v>21.0909621888264</x:v>
+        <x:v>194.719096456989</x:v>
       </x:c>
       <x:c r="J18">
-        <x:v>106.13531139965</x:v>
+        <x:v>105.028101664515</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="A19">
-        <x:v>155.796691382209</x:v>
+        <x:v>183.116728990859</x:v>
       </x:c>
       <x:c r="B19">
-        <x:v>188.730072317985</x:v>
+        <x:v>195.512091925141</x:v>
       </x:c>
       <x:c r="C19">
-        <x:v>122.836988197098</x:v>
+        <x:v>45.9383922842976</x:v>
       </x:c>
       <x:c r="D19">
-        <x:v>20.5476686454134</x:v>
+        <x:v>3.0776795945492</x:v>
       </x:c>
       <x:c r="E19">
-        <x:v>119.151601716481</x:v>
+        <x:v>103.078899953085</x:v>
       </x:c>
       <x:c r="F19">
-        <x:v>14.6479395286403</x:v>
+        <x:v>126.119891054053</x:v>
       </x:c>
       <x:c r="G19">
-        <x:v>88.3125940749015</x:v>
+        <x:v>1.47858252817699</x:v>
       </x:c>
       <x:c r="H19">
-        <x:v>14.1402668385488</x:v>
+        <x:v>192.379957247702</x:v>
       </x:c>
       <x:c r="I19">
-        <x:v>151.764033526072</x:v>
+        <x:v>136.242281708979</x:v>
       </x:c>
       <x:c r="J19">
-        <x:v>3.74348247598088</x:v>
+        <x:v>171.071366859168</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
       <x:c r="A20">
-        <x:v>172.444617921694</x:v>
+        <x:v>142.89264108189</x:v>
       </x:c>
       <x:c r="B20">
-        <x:v>110.862936037994</x:v>
+        <x:v>143.503860264786</x:v>
       </x:c>
       <x:c r="C20">
-        <x:v>112.610833678679</x:v>
+        <x:v>70.0784257008128</x:v>
       </x:c>
       <x:c r="D20">
-        <x:v>128.352850735352</x:v>
+        <x:v>108.651896616748</x:v>
       </x:c>
       <x:c r="E20">
-        <x:v>50.7734326882164</x:v>
+        <x:v>161.112274025153</x:v>
       </x:c>
       <x:c r="F20">
-        <x:v>135.11159547377</x:v>
+        <x:v>20.374432401906</x:v>
       </x:c>
       <x:c r="G20">
-        <x:v>44.5036159104219</x:v>
+        <x:v>140.946556227722</x:v>
       </x:c>
       <x:c r="H20">
-        <x:v>78.8227131957294</x:v>
+        <x:v>45.9770208438751</x:v>
       </x:c>
       <x:c r="I20">
-        <x:v>17.1635104423219</x:v>
+        <x:v>21.0422836342092</x:v>
       </x:c>
       <x:c r="J20">
-        <x:v>86.368454101667</x:v>
+        <x:v>61.0769141749837</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
da finire il data binding
</commit_message>
<xml_diff>
--- a/windows_form_app/ConditionalFormatColorScale.xlsx
+++ b/windows_form_app/ConditionalFormatColorScale.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R3205782c566045ee"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R89ec1bc19f854cbe"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -345,642 +345,642 @@
   <x:sheetData>
     <x:row r="1">
       <x:c r="A1">
-        <x:v>160.334686357684</x:v>
+        <x:v>32.9414084707114</x:v>
       </x:c>
       <x:c r="B1">
-        <x:v>20.6578374005192</x:v>
+        <x:v>108.116717780063</x:v>
       </x:c>
       <x:c r="C1">
-        <x:v>125.304815138366</x:v>
+        <x:v>188.851263741428</x:v>
       </x:c>
       <x:c r="D1">
-        <x:v>7.42962435233855</x:v>
+        <x:v>9.29911081180866</x:v>
       </x:c>
       <x:c r="E1">
-        <x:v>141.576353060816</x:v>
+        <x:v>91.1148366942605</x:v>
       </x:c>
       <x:c r="F1">
-        <x:v>72.0289083533124</x:v>
+        <x:v>156.880231554099</x:v>
       </x:c>
       <x:c r="G1">
-        <x:v>99.7806833590291</x:v>
+        <x:v>11.7141144404719</x:v>
       </x:c>
       <x:c r="H1">
-        <x:v>10.6914648835973</x:v>
+        <x:v>149.384023877505</x:v>
       </x:c>
       <x:c r="I1">
-        <x:v>29.0826002271299</x:v>
+        <x:v>53.415918561358</x:v>
       </x:c>
       <x:c r="J1">
-        <x:v>186.48344063502</x:v>
+        <x:v>164.375875314873</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>49.5330577015565</x:v>
+        <x:v>28.8470517046969</x:v>
       </x:c>
       <x:c r="B2">
-        <x:v>21.2742932239893</x:v>
+        <x:v>140.439572716337</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>42.4062806379079</x:v>
+        <x:v>124.278133792932</x:v>
       </x:c>
       <x:c r="D2">
-        <x:v>39.5965671351164</x:v>
+        <x:v>0.282906275374306</x:v>
       </x:c>
       <x:c r="E2">
-        <x:v>103.93235157427</x:v>
+        <x:v>112.74384237488</x:v>
       </x:c>
       <x:c r="F2">
-        <x:v>139.959372458961</x:v>
+        <x:v>86.9387512500113</x:v>
       </x:c>
       <x:c r="G2">
-        <x:v>137.812589638779</x:v>
+        <x:v>150.847064308285</x:v>
       </x:c>
       <x:c r="H2">
-        <x:v>6.90119434469435</x:v>
+        <x:v>179.575945334312</x:v>
       </x:c>
       <x:c r="I2">
-        <x:v>139.518385166078</x:v>
+        <x:v>107.160048516076</x:v>
       </x:c>
       <x:c r="J2">
-        <x:v>165.918658844157</x:v>
+        <x:v>190.545255965807</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>180.165873831215</x:v>
+        <x:v>66.217780423452</x:v>
       </x:c>
       <x:c r="B3">
-        <x:v>131.93953006153</x:v>
+        <x:v>7.18497354871825</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>186.906220757824</x:v>
+        <x:v>3.4049037859798</x:v>
       </x:c>
       <x:c r="D3">
-        <x:v>58.8757023489455</x:v>
+        <x:v>128.198529560211</x:v>
       </x:c>
       <x:c r="E3">
-        <x:v>62.2783218800455</x:v>
+        <x:v>174.958692851923</x:v>
       </x:c>
       <x:c r="F3">
-        <x:v>128.016692087062</x:v>
+        <x:v>154.288465228997</x:v>
       </x:c>
       <x:c r="G3">
-        <x:v>149.201590264776</x:v>
+        <x:v>25.108172942469</x:v>
       </x:c>
       <x:c r="H3">
-        <x:v>45.5876905683371</x:v>
+        <x:v>103.82220945499</x:v>
       </x:c>
       <x:c r="I3">
-        <x:v>118.602181653773</x:v>
+        <x:v>132.524444410822</x:v>
       </x:c>
       <x:c r="J3">
-        <x:v>62.258485454255</x:v>
+        <x:v>108.985220039722</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>35.4854357594091</x:v>
+        <x:v>195.135846172988</x:v>
       </x:c>
       <x:c r="B4">
-        <x:v>101.26448846481</x:v>
+        <x:v>2.64957714949249</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>47.5028627773295</x:v>
+        <x:v>5.7952925589845</x:v>
       </x:c>
       <x:c r="D4">
-        <x:v>92.8036313004809</x:v>
+        <x:v>102.310986119467</x:v>
       </x:c>
       <x:c r="E4">
-        <x:v>0.8067236285688</x:v>
+        <x:v>18.1320874104891</x:v>
       </x:c>
       <x:c r="F4">
-        <x:v>101.407469763145</x:v>
+        <x:v>114.406534989554</x:v>
       </x:c>
       <x:c r="G4">
-        <x:v>74.5363784369716</x:v>
+        <x:v>181.640655725096</x:v>
       </x:c>
       <x:c r="H4">
-        <x:v>181.77221239627</x:v>
+        <x:v>7.13782022108222</x:v>
       </x:c>
       <x:c r="I4">
-        <x:v>191.688250653301</x:v>
+        <x:v>152.050067648315</x:v>
       </x:c>
       <x:c r="J4">
-        <x:v>90.7576557671454</x:v>
+        <x:v>182.08702103332</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5">
-        <x:v>94.9912441405427</x:v>
+        <x:v>183.363339576574</x:v>
       </x:c>
       <x:c r="B5">
-        <x:v>3.69410598822595</x:v>
+        <x:v>11.9944848176066</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>4.29676138064673</x:v>
+        <x:v>5.11998692765831</x:v>
       </x:c>
       <x:c r="D5">
-        <x:v>190.969530209419</x:v>
+        <x:v>25.8805357971604</x:v>
       </x:c>
       <x:c r="E5">
-        <x:v>126.354855823496</x:v>
+        <x:v>160.020234324047</x:v>
       </x:c>
       <x:c r="F5">
-        <x:v>29.8405539383369</x:v>
+        <x:v>131.233907645212</x:v>
       </x:c>
       <x:c r="G5">
-        <x:v>101.439659065306</x:v>
+        <x:v>143.220596640939</x:v>
       </x:c>
       <x:c r="H5">
-        <x:v>116.551897729073</x:v>
+        <x:v>89.440680336878</x:v>
       </x:c>
       <x:c r="I5">
-        <x:v>105.142685726817</x:v>
+        <x:v>58.8428589789396</x:v>
       </x:c>
       <x:c r="J5">
-        <x:v>199.370667151814</x:v>
+        <x:v>66.359319568779</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>44.2154777442177</x:v>
+        <x:v>172.180705783973</x:v>
       </x:c>
       <x:c r="B6">
-        <x:v>160.873748250713</x:v>
+        <x:v>175.792729191386</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>112.889927585092</x:v>
+        <x:v>27.6833604218826</x:v>
       </x:c>
       <x:c r="D6">
-        <x:v>124.503278231483</x:v>
+        <x:v>24.3489646466211</x:v>
       </x:c>
       <x:c r="E6">
-        <x:v>163.190609478946</x:v>
+        <x:v>84.2274857145862</x:v>
       </x:c>
       <x:c r="F6">
-        <x:v>28.3951562961541</x:v>
+        <x:v>25.7564349219931</x:v>
       </x:c>
       <x:c r="G6">
-        <x:v>33.7516166426947</x:v>
+        <x:v>104.711813994083</x:v>
       </x:c>
       <x:c r="H6">
-        <x:v>66.4291127894209</x:v>
+        <x:v>60.6527341812163</x:v>
       </x:c>
       <x:c r="I6">
-        <x:v>145.151302472293</x:v>
+        <x:v>34.3404179598859</x:v>
       </x:c>
       <x:c r="J6">
-        <x:v>13.5596609737536</x:v>
+        <x:v>136.826371465263</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>122.827318088537</x:v>
+        <x:v>131.77205861163</x:v>
       </x:c>
       <x:c r="B7">
-        <x:v>54.192992790692</x:v>
+        <x:v>107.891904985482</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>92.0892832298247</x:v>
+        <x:v>16.8595794666836</x:v>
       </x:c>
       <x:c r="D7">
-        <x:v>166.824114772875</x:v>
+        <x:v>144.430698521636</x:v>
       </x:c>
       <x:c r="E7">
-        <x:v>150.998004875611</x:v>
+        <x:v>169.240029141884</x:v>
       </x:c>
       <x:c r="F7">
-        <x:v>148.268569236746</x:v>
+        <x:v>26.1974745552044</x:v>
       </x:c>
       <x:c r="G7">
-        <x:v>173.77143044666</x:v>
+        <x:v>134.644280157352</x:v>
       </x:c>
       <x:c r="H7">
-        <x:v>149.602649337427</x:v>
+        <x:v>21.9671476734649</x:v>
       </x:c>
       <x:c r="I7">
-        <x:v>38.7898435065475</x:v>
+        <x:v>182.150818864885</x:v>
       </x:c>
       <x:c r="J7">
-        <x:v>2.52488181112561</x:v>
+        <x:v>198.337307385326</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>65.4229940219889</x:v>
+        <x:v>105.298095524916</x:v>
       </x:c>
       <x:c r="B8">
-        <x:v>156.040377242509</x:v>
+        <x:v>143.709244087203</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>15.2129436913938</x:v>
+        <x:v>27.5258776859966</x:v>
       </x:c>
       <x:c r="D8">
-        <x:v>48.7607293989326</x:v>
+        <x:v>125.073027482756</x:v>
       </x:c>
       <x:c r="E8">
-        <x:v>70.9274147036147</x:v>
+        <x:v>7.18191638923339</x:v>
       </x:c>
       <x:c r="F8">
-        <x:v>176.471767842989</x:v>
+        <x:v>54.2232956058454</x:v>
       </x:c>
       <x:c r="G8">
-        <x:v>127.642768680883</x:v>
+        <x:v>2.06498662105994</x:v>
       </x:c>
       <x:c r="H8">
-        <x:v>195.936690548405</x:v>
+        <x:v>177.524367988819</x:v>
       </x:c>
       <x:c r="I8">
-        <x:v>132.52084652545</x:v>
+        <x:v>168.178295236164</x:v>
       </x:c>
       <x:c r="J8">
-        <x:v>32.4377679417086</x:v>
+        <x:v>43.7247852067113</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>26.577033021756</x:v>
+        <x:v>11.0678685880582</x:v>
       </x:c>
       <x:c r="B9">
-        <x:v>32.6496925357029</x:v>
+        <x:v>135.667492605591</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>140.44500484152</x:v>
+        <x:v>44.9793504760504</x:v>
       </x:c>
       <x:c r="D9">
-        <x:v>119.231514501959</x:v>
+        <x:v>66.1651248420426</x:v>
       </x:c>
       <x:c r="E9">
-        <x:v>18.0430077100373</x:v>
+        <x:v>136.804514255749</x:v>
       </x:c>
       <x:c r="F9">
-        <x:v>74.6116875086965</x:v>
+        <x:v>19.3431169816028</x:v>
       </x:c>
       <x:c r="G9">
-        <x:v>188.374560879718</x:v>
+        <x:v>174.96621672761</x:v>
       </x:c>
       <x:c r="H9">
-        <x:v>122.999584545847</x:v>
+        <x:v>181.446327912363</x:v>
       </x:c>
       <x:c r="I9">
-        <x:v>129.613021821535</x:v>
+        <x:v>18.0835004048811</x:v>
       </x:c>
       <x:c r="J9">
-        <x:v>172.411567332415</x:v>
+        <x:v>192.375652488496</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>67.6558531204499</x:v>
+        <x:v>9.69472099547029</x:v>
       </x:c>
       <x:c r="B10">
-        <x:v>8.1072656475507</x:v>
+        <x:v>120.987921543879</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>36.6209099239767</x:v>
+        <x:v>172.797402261196</x:v>
       </x:c>
       <x:c r="D10">
-        <x:v>178.128589679547</x:v>
+        <x:v>15.2236961830518</x:v>
       </x:c>
       <x:c r="E10">
-        <x:v>167.930337678609</x:v>
+        <x:v>50.3149624216906</x:v>
       </x:c>
       <x:c r="F10">
-        <x:v>40.7982513498507</x:v>
+        <x:v>75.4714345910919</x:v>
       </x:c>
       <x:c r="G10">
-        <x:v>111.604822758401</x:v>
+        <x:v>195.134905350923</x:v>
       </x:c>
       <x:c r="H10">
-        <x:v>37.4726466077718</x:v>
+        <x:v>60.6892884060225</x:v>
       </x:c>
       <x:c r="I10">
-        <x:v>39.9715253338085</x:v>
+        <x:v>56.6405066552761</x:v>
       </x:c>
       <x:c r="J10">
-        <x:v>178.08628658675</x:v>
+        <x:v>133.822759768843</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>56.069123491677</x:v>
+        <x:v>196.58962748786</x:v>
       </x:c>
       <x:c r="B11">
-        <x:v>151.837009727879</x:v>
+        <x:v>121.253448967474</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>77.7620542225251</x:v>
+        <x:v>107.289861471993</x:v>
       </x:c>
       <x:c r="D11">
-        <x:v>102.617803915691</x:v>
+        <x:v>60.5055515936136</x:v>
       </x:c>
       <x:c r="E11">
-        <x:v>133.947673129825</x:v>
+        <x:v>161.061224043863</x:v>
       </x:c>
       <x:c r="F11">
-        <x:v>88.1751005017083</x:v>
+        <x:v>28.4714616967698</x:v>
       </x:c>
       <x:c r="G11">
-        <x:v>145.660804559319</x:v>
+        <x:v>148.266851505389</x:v>
       </x:c>
       <x:c r="H11">
-        <x:v>64.1291981861597</x:v>
+        <x:v>102.610332939127</x:v>
       </x:c>
       <x:c r="I11">
-        <x:v>53.5758635278679</x:v>
+        <x:v>17.1670482573877</x:v>
       </x:c>
       <x:c r="J11">
-        <x:v>186.718841635957</x:v>
+        <x:v>30.0041901087408</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
       <x:c r="A12">
-        <x:v>100.752387615271</x:v>
+        <x:v>23.6914483009332</x:v>
       </x:c>
       <x:c r="B12">
-        <x:v>37.8149260942894</x:v>
+        <x:v>127.187446005264</x:v>
       </x:c>
       <x:c r="C12">
-        <x:v>133.908266263971</x:v>
+        <x:v>92.4744389450524</x:v>
       </x:c>
       <x:c r="D12">
-        <x:v>112.713534530584</x:v>
+        <x:v>190.615632753175</x:v>
       </x:c>
       <x:c r="E12">
-        <x:v>186.982627951998</x:v>
+        <x:v>125.758502877205</x:v>
       </x:c>
       <x:c r="F12">
-        <x:v>90.1776255528338</x:v>
+        <x:v>196.104566006039</x:v>
       </x:c>
       <x:c r="G12">
-        <x:v>113.747987949172</x:v>
+        <x:v>62.9125545094314</x:v>
       </x:c>
       <x:c r="H12">
-        <x:v>172.857768727866</x:v>
+        <x:v>150.694454624641</x:v>
       </x:c>
       <x:c r="I12">
-        <x:v>148.781107062838</x:v>
+        <x:v>7.62618426588652</x:v>
       </x:c>
       <x:c r="J12">
-        <x:v>76.386317366914</x:v>
+        <x:v>149.896912160282</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="A13">
-        <x:v>159.894008357028</x:v>
+        <x:v>51.2312578275945</x:v>
       </x:c>
       <x:c r="B13">
-        <x:v>50.771845900813</x:v>
+        <x:v>153.197952244989</x:v>
       </x:c>
       <x:c r="C13">
-        <x:v>19.9896275158923</x:v>
+        <x:v>3.88364726858383</x:v>
       </x:c>
       <x:c r="D13">
-        <x:v>66.3782761741329</x:v>
+        <x:v>189.775166376389</x:v>
       </x:c>
       <x:c r="E13">
-        <x:v>134.869028690676</x:v>
+        <x:v>188.642586389856</x:v>
       </x:c>
       <x:c r="F13">
-        <x:v>57.3157283744382</x:v>
+        <x:v>184.310173981036</x:v>
       </x:c>
       <x:c r="G13">
-        <x:v>119.419467318533</x:v>
+        <x:v>170.911841826007</x:v>
       </x:c>
       <x:c r="H13">
-        <x:v>37.0843540118469</x:v>
+        <x:v>12.3021815029449</x:v>
       </x:c>
       <x:c r="I13">
-        <x:v>80.830391720324</x:v>
+        <x:v>74.7580650610654</x:v>
       </x:c>
       <x:c r="J13">
-        <x:v>30.1291633537641</x:v>
+        <x:v>131.710481798142</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="A14">
-        <x:v>64.8669450845881</x:v>
+        <x:v>59.0883902549224</x:v>
       </x:c>
       <x:c r="B14">
-        <x:v>90.1701220731112</x:v>
+        <x:v>141.375698215037</x:v>
       </x:c>
       <x:c r="C14">
-        <x:v>155.965165214597</x:v>
+        <x:v>120.883861333543</x:v>
       </x:c>
       <x:c r="D14">
-        <x:v>154.4345599387</x:v>
+        <x:v>34.3555354673208</x:v>
       </x:c>
       <x:c r="E14">
-        <x:v>176.368644450032</x:v>
+        <x:v>47.1351577188518</x:v>
       </x:c>
       <x:c r="F14">
-        <x:v>74.740023293877</x:v>
+        <x:v>89.814419620584</x:v>
       </x:c>
       <x:c r="G14">
-        <x:v>154.887638313178</x:v>
+        <x:v>28.3776311335981</x:v>
       </x:c>
       <x:c r="H14">
-        <x:v>37.8272009258285</x:v>
+        <x:v>184.473798882437</x:v>
       </x:c>
       <x:c r="I14">
-        <x:v>185.283841372134</x:v>
+        <x:v>105.103900798179</x:v>
       </x:c>
       <x:c r="J14">
-        <x:v>129.867907208329</x:v>
+        <x:v>108.33305255898</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="A15">
-        <x:v>128.950882949378</x:v>
+        <x:v>71.0762654762139</x:v>
       </x:c>
       <x:c r="B15">
-        <x:v>124.245362693558</x:v>
+        <x:v>72.3558837884832</x:v>
       </x:c>
       <x:c r="C15">
-        <x:v>69.423721017979</x:v>
+        <x:v>164.279279654976</x:v>
       </x:c>
       <x:c r="D15">
-        <x:v>142.894180185578</x:v>
+        <x:v>188.07931029614</x:v>
       </x:c>
       <x:c r="E15">
-        <x:v>71.6591797171436</x:v>
+        <x:v>168.684204187563</x:v>
       </x:c>
       <x:c r="F15">
-        <x:v>29.8409270261605</x:v>
+        <x:v>82.5072749902062</x:v>
       </x:c>
       <x:c r="G15">
-        <x:v>74.1989993835795</x:v>
+        <x:v>28.513482598827</x:v>
       </x:c>
       <x:c r="H15">
-        <x:v>123.907375393392</x:v>
+        <x:v>182.181769508022</x:v>
       </x:c>
       <x:c r="I15">
-        <x:v>191.145961727549</x:v>
+        <x:v>89.4651933058469</x:v>
       </x:c>
       <x:c r="J15">
-        <x:v>77.7527121257748</x:v>
+        <x:v>54.210396415652</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="A16">
-        <x:v>127.050263400679</x:v>
+        <x:v>12.5588800816605</x:v>
       </x:c>
       <x:c r="B16">
-        <x:v>138.747054030535</x:v>
+        <x:v>44.4404507262821</x:v>
       </x:c>
       <x:c r="C16">
-        <x:v>88.6915395449342</x:v>
+        <x:v>53.063104140136</x:v>
       </x:c>
       <x:c r="D16">
-        <x:v>163.585207966894</x:v>
+        <x:v>106.743594494995</x:v>
       </x:c>
       <x:c r="E16">
-        <x:v>18.192278229721</x:v>
+        <x:v>82.5915019412486</x:v>
       </x:c>
       <x:c r="F16">
-        <x:v>5.297277590864</x:v>
+        <x:v>43.3916752428709</x:v>
       </x:c>
       <x:c r="G16">
-        <x:v>131.847382211987</x:v>
+        <x:v>117.36980169889</x:v>
       </x:c>
       <x:c r="H16">
-        <x:v>11.3837780483923</x:v>
+        <x:v>117.514695095604</x:v>
       </x:c>
       <x:c r="I16">
-        <x:v>167.748775225016</x:v>
+        <x:v>71.8629652037578</x:v>
       </x:c>
       <x:c r="J16">
-        <x:v>76.6319447553865</x:v>
+        <x:v>176.751050062827</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="A17">
-        <x:v>168.755633183176</x:v>
+        <x:v>57.5596198707631</x:v>
       </x:c>
       <x:c r="B17">
-        <x:v>108.576450547472</x:v>
+        <x:v>135.964670002444</x:v>
       </x:c>
       <x:c r="C17">
-        <x:v>183.298806465836</x:v>
+        <x:v>27.8522678780613</x:v>
       </x:c>
       <x:c r="D17">
-        <x:v>23.4467001741038</x:v>
+        <x:v>85.4565664592462</x:v>
       </x:c>
       <x:c r="E17">
-        <x:v>121.851896551369</x:v>
+        <x:v>170.915799853818</x:v>
       </x:c>
       <x:c r="F17">
-        <x:v>10.5822655421599</x:v>
+        <x:v>82.3157500858958</x:v>
       </x:c>
       <x:c r="G17">
-        <x:v>81.8497608796925</x:v>
+        <x:v>6.30358467172067</x:v>
       </x:c>
       <x:c r="H17">
-        <x:v>179.473706325271</x:v>
+        <x:v>58.1189034777316</x:v>
       </x:c>
       <x:c r="I17">
-        <x:v>136.344890080553</x:v>
+        <x:v>143.480475034323</x:v>
       </x:c>
       <x:c r="J17">
-        <x:v>112.242604658121</x:v>
+        <x:v>35.9440832566209</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="A18">
-        <x:v>135.289987239656</x:v>
+        <x:v>167.72693487244</x:v>
       </x:c>
       <x:c r="B18">
-        <x:v>75.9207870233435</x:v>
+        <x:v>78.4387556269945</x:v>
       </x:c>
       <x:c r="C18">
-        <x:v>187.573927355732</x:v>
+        <x:v>45.5905538264618</x:v>
       </x:c>
       <x:c r="D18">
-        <x:v>18.9131998545086</x:v>
+        <x:v>99.293131706907</x:v>
       </x:c>
       <x:c r="E18">
-        <x:v>147.435434417536</x:v>
+        <x:v>78.8206466840676</x:v>
       </x:c>
       <x:c r="F18">
-        <x:v>35.6486456634703</x:v>
+        <x:v>178.875374039111</x:v>
       </x:c>
       <x:c r="G18">
-        <x:v>181.348124882834</x:v>
+        <x:v>188.918672590013</x:v>
       </x:c>
       <x:c r="H18">
-        <x:v>77.0954473303144</x:v>
+        <x:v>15.8043369724435</x:v>
       </x:c>
       <x:c r="I18">
-        <x:v>194.719096456989</x:v>
+        <x:v>21.0909621888264</x:v>
       </x:c>
       <x:c r="J18">
-        <x:v>105.028101664515</x:v>
+        <x:v>106.13531139965</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="A19">
-        <x:v>183.116728990859</x:v>
+        <x:v>155.796691382209</x:v>
       </x:c>
       <x:c r="B19">
-        <x:v>195.512091925141</x:v>
+        <x:v>188.730072317985</x:v>
       </x:c>
       <x:c r="C19">
-        <x:v>45.9383922842976</x:v>
+        <x:v>122.836988197098</x:v>
       </x:c>
       <x:c r="D19">
-        <x:v>3.0776795945492</x:v>
+        <x:v>20.5476686454134</x:v>
       </x:c>
       <x:c r="E19">
-        <x:v>103.078899953085</x:v>
+        <x:v>119.151601716481</x:v>
       </x:c>
       <x:c r="F19">
-        <x:v>126.119891054053</x:v>
+        <x:v>14.6479395286403</x:v>
       </x:c>
       <x:c r="G19">
-        <x:v>1.47858252817699</x:v>
+        <x:v>88.3125940749015</x:v>
       </x:c>
       <x:c r="H19">
-        <x:v>192.379957247702</x:v>
+        <x:v>14.1402668385488</x:v>
       </x:c>
       <x:c r="I19">
-        <x:v>136.242281708979</x:v>
+        <x:v>151.764033526072</x:v>
       </x:c>
       <x:c r="J19">
-        <x:v>171.071366859168</x:v>
+        <x:v>3.74348247598088</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
       <x:c r="A20">
-        <x:v>142.89264108189</x:v>
+        <x:v>172.444617921694</x:v>
       </x:c>
       <x:c r="B20">
-        <x:v>143.503860264786</x:v>
+        <x:v>110.862936037994</x:v>
       </x:c>
       <x:c r="C20">
-        <x:v>70.0784257008128</x:v>
+        <x:v>112.610833678679</x:v>
       </x:c>
       <x:c r="D20">
-        <x:v>108.651896616748</x:v>
+        <x:v>128.352850735352</x:v>
       </x:c>
       <x:c r="E20">
-        <x:v>161.112274025153</x:v>
+        <x:v>50.7734326882164</x:v>
       </x:c>
       <x:c r="F20">
-        <x:v>20.374432401906</x:v>
+        <x:v>135.11159547377</x:v>
       </x:c>
       <x:c r="G20">
-        <x:v>140.946556227722</x:v>
+        <x:v>44.5036159104219</x:v>
       </x:c>
       <x:c r="H20">
-        <x:v>45.9770208438751</x:v>
+        <x:v>78.8227131957294</x:v>
       </x:c>
       <x:c r="I20">
-        <x:v>21.0422836342092</x:v>
+        <x:v>17.1635104423219</x:v>
       </x:c>
       <x:c r="J20">
-        <x:v>61.0769141749837</x:v>
+        <x:v>86.368454101667</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>